<commit_message>
Add missing file to analysis of turnover by gender
</commit_message>
<xml_diff>
--- a/HRDataset_analysis.xlsx
+++ b/HRDataset_analysis.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8beb163ab15076dd/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="476" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0E35372-11C1-48B6-AF07-058F58541AA6}"/>
+  <xr:revisionPtr revIDLastSave="572" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCAEDFC5-EEB9-42DA-A4C7-953D04092DC5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
   </bookViews>
   <sheets>
     <sheet name="HRDataset_raw" sheetId="1" r:id="rId1"/>
     <sheet name="HRDataset_clean" sheetId="2" r:id="rId2"/>
     <sheet name="Turnover_by_department" sheetId="5" r:id="rId3"/>
+    <sheet name="Turnover_by_gender" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">HRDataset_clean!$A$1:$N$312</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="729">
   <si>
     <t>Employee_Name,EmpID,MarriedID,MaritalStatusID,GenderID,EmpStatusID,DeptID,PerfScoreID,FromDiversityJobFairID,Salary,Termd,PositionID,Position,State,Zip,DOB,Sex,MaritalDesc,CitizenDesc,HispanicLatino,RaceDesc,DateofHire,DateofTermination,TermReason,EmploymentStatus,Department,ManagerName,ManagerID,RecruitmentSource,PerformanceScore,EngagementSurvey,EmpSatisfaction,SpecialProjectsCount,LastPerformanceReview_Date,DaysLateLast30,Absences</t>
   </si>
@@ -2230,6 +2231,12 @@
   </si>
   <si>
     <t>Employee turnover: in which departments there are the most dismissals?</t>
+  </si>
+  <si>
+    <t>Gender/ Employment status</t>
+  </si>
+  <si>
+    <t>Does the turnover differ between men and women?</t>
   </si>
 </sst>
 </file>
@@ -2775,10 +2782,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% – колірна тема 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3135,19 +3142,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="70000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3978,6 +3973,721 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="uk-UA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[HRDataset_analysis.xlsx]Turnover_by_gender!Зведена таблиця1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Employee turnover by gender</a:t>
+            </a:r>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="uk-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="70000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="uk-UA"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="25000"/>
+              <a:lumOff val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="25000"/>
+              <a:lumOff val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="25000"/>
+              <a:lumOff val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Turnover_by_gender!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Підсумок</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-BDAD-43E8-9672-982F4FBBE835}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-BDAD-43E8-9672-982F4FBBE835}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BDAD-43E8-9672-982F4FBBE835}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-BDAD-43E8-9672-982F4FBBE835}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-BDAD-43E8-9672-982F4FBBE835}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-BDAD-43E8-9672-982F4FBBE835}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="uk-UA"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Turnover_by_gender!$A$4:$A$12</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Active</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Terminated for Cause</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Voluntarily Terminated</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Active</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Terminated for Cause</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Voluntarily Terminated</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>F</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>M </c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Turnover_by_gender!$B$4:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BDAD-43E8-9672-982F4FBBE835}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="80"/>
+        <c:overlap val="25"/>
+        <c:axId val="760905679"/>
+        <c:axId val="760891279"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="760905679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="760891279"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="760891279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="760905679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="uk-UA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4018,7 +4728,539 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4727,6 +5969,262 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>606425</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>301625</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Діаграма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5E234C0-53AA-DBF9-529F-F7EE391C399C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3822700" cy="2768600"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B05B213-4563-6D50-2FBB-27F7D37D717C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9112250" y="419100"/>
+          <a:ext cx="3822700" cy="2768600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The absolute ratio of women/men in the company is 176/135,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> relative ratio: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>57%/43%. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Absolute indicators among Voluntarily Terminated</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> employees</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>women - 51, men - 37, relative</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> ratio: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>women - 29%, men - 27%. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Absolute indicators among </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Terminated</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> for Cause employees</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>women - 9, men - 7, relative indicators: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>women - 5%, men - 5%.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>►</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Conclusions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>: In absolute numbers, we can see that more women are dismissed, but the total number of women in the company is also larger, so this is expected. In the calculation of Voluntary Terminated</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Terminated for Cause employees</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>in relation to the total number of women and men in the company, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>there is almost no difference in dismissals between the sexes</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="uk-UA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -4756,7 +6254,10 @@
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1951-01-02T00:00:00" maxDate="1992-08-18T00:00:00"/>
     </cacheField>
     <cacheField name="Sex" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="2">
+        <s v="M "/>
+        <s v="F"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="CitizenDesc" numFmtId="0">
       <sharedItems/>
@@ -4814,7 +6315,7 @@
     <n v="62506"/>
     <s v="Production Technician I"/>
     <d v="1983-07-10T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <m/>
@@ -4832,7 +6333,7 @@
     <n v="104437"/>
     <s v="Sr. DBA"/>
     <d v="1975-05-05T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <d v="2016-06-16T00:00:00"/>
@@ -4850,7 +6351,7 @@
     <n v="64955"/>
     <s v="Production Technician II"/>
     <d v="1988-09-19T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <d v="2012-09-24T00:00:00"/>
@@ -4868,7 +6369,7 @@
     <n v="64991"/>
     <s v="Production Technician I"/>
     <d v="1988-09-27T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2008-01-07T00:00:00"/>
     <m/>
@@ -4886,7 +6387,7 @@
     <n v="50825"/>
     <s v="Production Technician I"/>
     <d v="1989-09-08T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-07-11T00:00:00"/>
     <d v="2016-09-06T00:00:00"/>
@@ -4904,7 +6405,7 @@
     <n v="57568"/>
     <s v="Production Technician I"/>
     <d v="1977-05-22T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-01-09T00:00:00"/>
     <m/>
@@ -4922,7 +6423,7 @@
     <n v="95660"/>
     <s v="Software Engineer"/>
     <d v="1979-05-24T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-11-10T00:00:00"/>
     <m/>
@@ -4940,7 +6441,7 @@
     <n v="59365"/>
     <s v="Production Technician I"/>
     <d v="1983-02-18T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-09-30T00:00:00"/>
     <m/>
@@ -4958,7 +6459,7 @@
     <n v="47837"/>
     <s v="Production Technician I"/>
     <d v="1970-02-11T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2009-07-06T00:00:00"/>
     <m/>
@@ -4976,7 +6477,7 @@
     <n v="50178"/>
     <s v="IT Support"/>
     <d v="1988-01-07T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <m/>
@@ -4994,7 +6495,7 @@
     <n v="54670"/>
     <s v="Production Technician I"/>
     <d v="1974-01-12T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2017-01-12T00:00:00"/>
@@ -5012,7 +6513,7 @@
     <n v="47211"/>
     <s v="Production Technician I"/>
     <d v="1974-02-21T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-04-02T00:00:00"/>
     <d v="2016-09-19T00:00:00"/>
@@ -5030,7 +6531,7 @@
     <n v="92328"/>
     <s v="Data Analyst"/>
     <d v="1988-07-04T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-11-10T00:00:00"/>
     <m/>
@@ -5048,7 +6549,7 @@
     <n v="58709"/>
     <s v="Production Technician I"/>
     <d v="1983-07-20T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-02-20T00:00:00"/>
     <m/>
@@ -5066,7 +6567,7 @@
     <n v="52505"/>
     <s v="Production Technician I"/>
     <d v="1977-07-15T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-09-24T00:00:00"/>
     <d v="2017-04-06T00:00:00"/>
@@ -5084,7 +6585,7 @@
     <n v="57834"/>
     <s v="Production Technician I"/>
     <d v="1981-10-18T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-02-21T00:00:00"/>
     <d v="2017-08-04T00:00:00"/>
@@ -5102,7 +6603,7 @@
     <n v="70131"/>
     <s v="Production Technician II"/>
     <d v="1966-04-17T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2016-07-21T00:00:00"/>
     <m/>
@@ -5120,7 +6621,7 @@
     <n v="59026"/>
     <s v="Production Technician I"/>
     <d v="1970-10-27T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="Eligible NonCitizen"/>
     <d v="2011-04-04T00:00:00"/>
     <m/>
@@ -5138,7 +6639,7 @@
     <n v="110000"/>
     <s v="Database Administrator"/>
     <d v="1986-04-04T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-07-07T00:00:00"/>
     <d v="2015-09-12T00:00:00"/>
@@ -5156,7 +6657,7 @@
     <n v="53250"/>
     <s v="Production Technician I"/>
     <d v="1979-04-06T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-07-08T00:00:00"/>
     <m/>
@@ -5174,7 +6675,7 @@
     <n v="51044"/>
     <s v="Production Technician I"/>
     <d v="1970-12-22T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-04-02T00:00:00"/>
     <m/>
@@ -5192,7 +6693,7 @@
     <n v="64919"/>
     <s v="Production Technician I"/>
     <d v="1958-12-27T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-08-19T00:00:00"/>
     <m/>
@@ -5210,7 +6711,7 @@
     <n v="62910"/>
     <s v="Production Technician I"/>
     <d v="1989-09-01T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-07-07T00:00:00"/>
     <m/>
@@ -5228,7 +6729,7 @@
     <n v="66441"/>
     <s v="Production Technician II"/>
     <d v="1990-09-21T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-04-04T00:00:00"/>
     <m/>
@@ -5246,7 +6747,7 @@
     <n v="57815"/>
     <s v="Production Technician II"/>
     <d v="1967-01-16T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2014-04-04T00:00:00"/>
@@ -5264,7 +6765,7 @@
     <n v="103613"/>
     <s v="Enterprise Architect"/>
     <d v="1964-07-30T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-02-17T00:00:00"/>
     <d v="2016-02-19T00:00:00"/>
@@ -5282,7 +6783,7 @@
     <n v="106367"/>
     <s v="Sr. Accountant"/>
     <d v="1987-04-04T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-02-16T00:00:00"/>
     <m/>
@@ -5300,7 +6801,7 @@
     <n v="74312"/>
     <s v="Production Manager"/>
     <d v="1970-03-10T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-09-30T00:00:00"/>
     <d v="2014-08-07T00:00:00"/>
@@ -5318,7 +6819,7 @@
     <n v="53492"/>
     <s v="Production Technician I"/>
     <d v="1990-08-24T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-04-02T00:00:00"/>
     <d v="2013-06-15T00:00:00"/>
@@ -5336,7 +6837,7 @@
     <n v="63000"/>
     <s v="Accountant I"/>
     <d v="1987-11-24T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2008-10-27T00:00:00"/>
     <m/>
@@ -5354,7 +6855,7 @@
     <n v="65288"/>
     <s v="Production Technician II"/>
     <d v="1983-07-28T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -5372,7 +6873,7 @@
     <n v="64375"/>
     <s v="Production Technician I"/>
     <d v="1969-10-30T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-11-11T00:00:00"/>
     <m/>
@@ -5390,7 +6891,7 @@
     <n v="74326"/>
     <s v="Area Sales Manager"/>
     <d v="1964-06-01T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="Eligible NonCitizen"/>
     <d v="2011-08-15T00:00:00"/>
     <d v="2014-08-02T00:00:00"/>
@@ -5408,7 +6909,7 @@
     <n v="63763"/>
     <s v="Production Technician II"/>
     <d v="1980-03-02T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-03-05T00:00:00"/>
     <m/>
@@ -5426,7 +6927,7 @@
     <n v="62162"/>
     <s v="Production Technician II"/>
     <d v="1977-08-19T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-04-04T00:00:00"/>
     <m/>
@@ -5444,7 +6945,7 @@
     <n v="77692"/>
     <s v="Software Engineering Manager"/>
     <d v="1966-11-22T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-08-15T00:00:00"/>
     <m/>
@@ -5462,7 +6963,7 @@
     <n v="72640"/>
     <s v="Production Manager"/>
     <d v="1983-08-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2016-01-28T00:00:00"/>
     <m/>
@@ -5480,7 +6981,7 @@
     <n v="93396"/>
     <s v="Software Engineer"/>
     <d v="1987-04-05T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-11-11T00:00:00"/>
     <m/>
@@ -5498,7 +6999,7 @@
     <n v="52846"/>
     <s v="Production Technician I"/>
     <d v="1983-02-02T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-03-31T00:00:00"/>
     <m/>
@@ -5516,7 +7017,7 @@
     <n v="100031"/>
     <s v="Sr. DBA"/>
     <d v="1986-06-06T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2016-06-30T00:00:00"/>
     <m/>
@@ -5534,7 +7035,7 @@
     <n v="71860"/>
     <s v="Area Sales Manager"/>
     <d v="1963-05-15T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-08-18T00:00:00"/>
     <m/>
@@ -5552,7 +7053,7 @@
     <n v="61656"/>
     <s v="Production Technician I"/>
     <d v="1951-01-02T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -5570,7 +7071,7 @@
     <n v="110929"/>
     <s v="BI Director"/>
     <d v="1972-02-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2016-09-06T00:00:00"/>
     <m/>
@@ -5588,7 +7089,7 @@
     <n v="54237"/>
     <s v="Production Technician I"/>
     <d v="1979-02-12T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-05-12T00:00:00"/>
     <m/>
@@ -5606,7 +7107,7 @@
     <n v="60380"/>
     <s v="Production Technician I"/>
     <d v="1983-08-24T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-07-08T00:00:00"/>
     <m/>
@@ -5624,7 +7125,7 @@
     <n v="66808"/>
     <s v="Area Sales Manager"/>
     <d v="1970-06-11T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="Eligible NonCitizen"/>
     <d v="2012-05-14T00:00:00"/>
     <m/>
@@ -5642,7 +7143,7 @@
     <n v="64786"/>
     <s v="Production Technician I"/>
     <d v="1983-08-27T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-06-27T00:00:00"/>
     <d v="2015-11-15T00:00:00"/>
@@ -5660,7 +7161,7 @@
     <n v="64816"/>
     <s v="Production Technician I"/>
     <d v="1988-05-31T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="Non-Citizen"/>
     <d v="2011-10-03T00:00:00"/>
     <m/>
@@ -5678,7 +7179,7 @@
     <n v="68678"/>
     <s v="IT Support"/>
     <d v="1985-09-05T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-09-05T00:00:00"/>
     <m/>
@@ -5696,7 +7197,7 @@
     <n v="64066"/>
     <s v="Production Technician II"/>
     <d v="1981-08-31T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-05-16T00:00:00"/>
     <d v="2013-01-07T00:00:00"/>
@@ -5714,7 +7215,7 @@
     <n v="59369"/>
     <s v="Production Technician II"/>
     <d v="1978-11-25T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2010-08-30T00:00:00"/>
     <d v="2011-09-26T00:00:00"/>
@@ -5732,7 +7233,7 @@
     <n v="50373"/>
     <s v="Production Technician I"/>
     <d v="1980-08-26T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2016-07-06T00:00:00"/>
     <m/>
@@ -5750,7 +7251,7 @@
     <n v="63108"/>
     <s v="Production Technician I"/>
     <d v="1977-09-08T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-07-08T00:00:00"/>
     <m/>
@@ -5768,7 +7269,7 @@
     <n v="59144"/>
     <s v="Production Technician I"/>
     <d v="1979-08-12T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-07-11T00:00:00"/>
     <d v="2016-09-23T00:00:00"/>
@@ -5786,7 +7287,7 @@
     <n v="68051"/>
     <s v="Production Manager"/>
     <d v="1975-12-17T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2010-07-20T00:00:00"/>
     <m/>
@@ -5804,7 +7305,7 @@
     <n v="170500"/>
     <s v="Director of Operations"/>
     <d v="1983-03-19T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2009-01-05T00:00:00"/>
     <m/>
@@ -5822,7 +7323,7 @@
     <n v="63381"/>
     <s v="Production Technician I"/>
     <d v="1977-03-31T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <m/>
@@ -5840,7 +7341,7 @@
     <n v="83552"/>
     <s v="Data Analyst"/>
     <d v="1986-08-26T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -5858,7 +7359,7 @@
     <n v="56149"/>
     <s v="Production Technician I"/>
     <d v="1987-04-10T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2016-07-06T00:00:00"/>
     <m/>
@@ -5876,7 +7377,7 @@
     <n v="92329"/>
     <s v="Sr. Network Engineer"/>
     <d v="1965-09-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-11-10T00:00:00"/>
     <m/>
@@ -5894,7 +7395,7 @@
     <n v="65729"/>
     <s v="Sales Manager"/>
     <d v="1990-04-19T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-05-05T00:00:00"/>
     <m/>
@@ -5912,7 +7413,7 @@
     <n v="85028"/>
     <s v="Sr. Network Engineer"/>
     <d v="1952-01-18T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-11-10T00:00:00"/>
     <m/>
@@ -5930,7 +7431,7 @@
     <n v="57583"/>
     <s v="Production Technician I"/>
     <d v="1978-11-05T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-07-02T00:00:00"/>
     <m/>
@@ -5948,7 +7449,7 @@
     <n v="56294"/>
     <s v="Production Technician II"/>
     <d v="1979-09-14T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="Eligible NonCitizen"/>
     <d v="2011-11-07T00:00:00"/>
     <m/>
@@ -5966,7 +7467,7 @@
     <n v="56991"/>
     <s v="Production Technician I"/>
     <d v="1988-04-15T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2018-07-09T00:00:00"/>
     <m/>
@@ -5984,7 +7485,7 @@
     <n v="55722"/>
     <s v="Production Technician I"/>
     <d v="1977-10-31T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-05-16T00:00:00"/>
     <d v="2016-06-08T00:00:00"/>
@@ -6002,7 +7503,7 @@
     <n v="101199"/>
     <s v="Software Engineer"/>
     <d v="1979-07-05T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-01-09T00:00:00"/>
     <m/>
@@ -6020,7 +7521,7 @@
     <n v="61568"/>
     <s v="Area Sales Manager"/>
     <d v="1975-11-02T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -6038,7 +7539,7 @@
     <n v="58275"/>
     <s v="Production Technician II"/>
     <d v="1951-02-25T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-04-04T00:00:00"/>
     <d v="2015-11-04T00:00:00"/>
@@ -6056,7 +7557,7 @@
     <n v="53189"/>
     <s v="Production Technician I"/>
     <d v="1967-04-19T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-07-07T00:00:00"/>
     <m/>
@@ -6074,7 +7575,7 @@
     <n v="96820"/>
     <s v="BI Developer"/>
     <d v="1983-09-04T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2017-02-15T00:00:00"/>
     <m/>
@@ -6092,7 +7593,7 @@
     <n v="51259"/>
     <s v="Production Technician I"/>
     <d v="1982-11-15T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-05-12T00:00:00"/>
     <m/>
@@ -6110,7 +7611,7 @@
     <n v="59231"/>
     <s v="Area Sales Manager"/>
     <d v="1987-05-14T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-02-20T00:00:00"/>
     <m/>
@@ -6128,7 +7629,7 @@
     <n v="61584"/>
     <s v="Production Technician I"/>
     <d v="1978-12-02T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-01-07T00:00:00"/>
     <m/>
@@ -6146,7 +7647,7 @@
     <n v="46335"/>
     <s v="Production Technician I"/>
     <d v="1986-10-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-04-02T00:00:00"/>
     <m/>
@@ -6164,7 +7665,7 @@
     <n v="70621"/>
     <s v="IT Support"/>
     <d v="1988-07-18T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <m/>
@@ -6182,7 +7683,7 @@
     <n v="138888"/>
     <s v="IT Manager - Support"/>
     <d v="1970-07-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-01-05T00:00:00"/>
     <m/>
@@ -6200,7 +7701,7 @@
     <n v="74241"/>
     <s v="Area Sales Manager"/>
     <d v="1988-11-08T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <m/>
@@ -6218,7 +7719,7 @@
     <n v="75188"/>
     <s v="Production Manager"/>
     <d v="1973-11-28T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-09-18T00:00:00"/>
     <m/>
@@ -6236,7 +7737,7 @@
     <n v="62514"/>
     <s v="Production Technician I"/>
     <d v="1973-09-23T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2010-04-26T00:00:00"/>
     <m/>
@@ -6254,7 +7755,7 @@
     <n v="60070"/>
     <s v="Production Technician I"/>
     <d v="1991-09-05T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-04-04T00:00:00"/>
     <d v="2017-06-06T00:00:00"/>
@@ -6272,7 +7773,7 @@
     <n v="48888"/>
     <s v="Production Technician I"/>
     <d v="1974-05-31T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-11-10T00:00:00"/>
     <m/>
@@ -6290,7 +7791,7 @@
     <n v="54285"/>
     <s v="Production Technician I"/>
     <d v="1978-08-25T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-03-31T00:00:00"/>
     <m/>
@@ -6308,7 +7809,7 @@
     <n v="56847"/>
     <s v="Production Technician II"/>
     <d v="1989-08-25T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-07-07T00:00:00"/>
     <m/>
@@ -6326,7 +7827,7 @@
     <n v="60340"/>
     <s v="Production Technician I"/>
     <d v="1983-09-02T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-04-02T00:00:00"/>
     <d v="2018-09-27T00:00:00"/>
@@ -6344,7 +7845,7 @@
     <n v="59124"/>
     <s v="Production Technician I"/>
     <d v="1989-05-06T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-02-17T00:00:00"/>
     <d v="2018-02-25T00:00:00"/>
@@ -6362,7 +7863,7 @@
     <n v="99280"/>
     <s v="Software Engineer"/>
     <d v="1987-05-15T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-05-02T00:00:00"/>
     <d v="2013-06-05T00:00:00"/>
@@ -6380,7 +7881,7 @@
     <n v="71776"/>
     <s v="Production Technician II"/>
     <d v="1978-09-22T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-07-07T00:00:00"/>
     <m/>
@@ -6398,7 +7899,7 @@
     <n v="65902"/>
     <s v="Production Technician II"/>
     <d v="1987-09-27T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-02-17T00:00:00"/>
     <m/>
@@ -6416,7 +7917,7 @@
     <n v="57748"/>
     <s v="Production Technician I"/>
     <d v="1955-04-14T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-11-07T00:00:00"/>
     <d v="2016-05-17T00:00:00"/>
@@ -6434,7 +7935,7 @@
     <n v="64057"/>
     <s v="Production Technician I"/>
     <d v="1989-10-18T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-05-11T00:00:00"/>
     <m/>
@@ -6452,7 +7953,7 @@
     <n v="53366"/>
     <s v="Network Engineer"/>
     <d v="1987-06-18T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -6470,7 +7971,7 @@
     <n v="58530"/>
     <s v="Production Technician I"/>
     <d v="1981-03-16T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-01-09T00:00:00"/>
     <m/>
@@ -6488,7 +7989,7 @@
     <n v="72609"/>
     <s v="Production Technician II"/>
     <d v="1981-10-01T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-05-16T00:00:00"/>
     <d v="2013-06-24T00:00:00"/>
@@ -6506,7 +8007,7 @@
     <n v="55965"/>
     <s v="Production Technician II"/>
     <d v="1983-11-08T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-04-04T00:00:00"/>
     <d v="2013-01-09T00:00:00"/>
@@ -6524,7 +8025,7 @@
     <n v="70187"/>
     <s v="Area Sales Manager"/>
     <d v="1975-07-07T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <d v="2018-08-19T00:00:00"/>
@@ -6542,7 +8043,7 @@
     <n v="178000"/>
     <s v="IT Director"/>
     <d v="1980-07-05T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-04-15T00:00:00"/>
     <m/>
@@ -6560,7 +8061,7 @@
     <n v="99351"/>
     <s v="Sr. Accountant"/>
     <d v="1979-04-16T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2009-01-05T00:00:00"/>
     <m/>
@@ -6578,7 +8079,7 @@
     <n v="67251"/>
     <s v="Area Sales Manager"/>
     <d v="1963-08-28T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-09-06T00:00:00"/>
     <m/>
@@ -6596,7 +8097,7 @@
     <n v="65707"/>
     <s v="IT Support"/>
     <d v="1968-07-06T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2010-05-01T00:00:00"/>
     <m/>
@@ -6614,7 +8115,7 @@
     <n v="52249"/>
     <s v="Production Technician I"/>
     <d v="1985-09-15T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -6632,7 +8133,7 @@
     <n v="53171"/>
     <s v="Production Technician I"/>
     <d v="1983-12-02T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-05-16T00:00:00"/>
     <m/>
@@ -6650,7 +8151,7 @@
     <n v="51337"/>
     <s v="Production Technician I"/>
     <d v="1990-10-01T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -6668,7 +8169,7 @@
     <n v="51505"/>
     <s v="Production Technician I"/>
     <d v="1970-05-15T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-11-07T00:00:00"/>
     <d v="2016-11-15T00:00:00"/>
@@ -6686,7 +8187,7 @@
     <n v="59370"/>
     <s v="Area Sales Manager"/>
     <d v="1971-07-10T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-07-07T00:00:00"/>
     <d v="2015-09-05T00:00:00"/>
@@ -6704,7 +8205,7 @@
     <n v="54933"/>
     <s v="Production Technician I"/>
     <d v="1974-08-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-04-02T00:00:00"/>
     <d v="2015-06-25T00:00:00"/>
@@ -6722,7 +8223,7 @@
     <n v="57815"/>
     <s v="Production Technician I"/>
     <d v="1980-05-08T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -6740,7 +8241,7 @@
     <n v="61555"/>
     <s v="Area Sales Manager"/>
     <d v="1989-09-22T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-02-16T00:00:00"/>
     <m/>
@@ -6758,7 +8259,7 @@
     <n v="114800"/>
     <s v="Database Administrator"/>
     <d v="1971-10-23T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-02-16T00:00:00"/>
     <d v="2015-03-15T00:00:00"/>
@@ -6776,7 +8277,7 @@
     <n v="74679"/>
     <s v="IT Support"/>
     <d v="1989-11-24T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -6794,7 +8295,7 @@
     <n v="53018"/>
     <s v="Production Technician I"/>
     <d v="1992-06-18T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-11-11T00:00:00"/>
     <m/>
@@ -6812,7 +8313,7 @@
     <n v="59892"/>
     <s v="Production Technician I"/>
     <d v="1969-09-29T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-07-11T00:00:00"/>
     <m/>
@@ -6830,7 +8331,7 @@
     <n v="68898"/>
     <s v="Production Technician II"/>
     <d v="1964-10-12T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2010-04-26T00:00:00"/>
     <d v="2011-05-30T00:00:00"/>
@@ -6848,7 +8349,7 @@
     <n v="61242"/>
     <s v="IT Support"/>
     <d v="1981-04-16T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <m/>
@@ -6866,7 +8367,7 @@
     <n v="66825"/>
     <s v="Production Technician II"/>
     <d v="1986-05-25T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-05-12T00:00:00"/>
     <m/>
@@ -6884,7 +8385,7 @@
     <n v="48285"/>
     <s v="Production Technician I"/>
     <d v="1979-05-21T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-07-02T00:00:00"/>
     <m/>
@@ -6902,7 +8403,7 @@
     <n v="66149"/>
     <s v="Production Technician II"/>
     <d v="1983-12-08T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-09-30T00:00:00"/>
     <m/>
@@ -6920,7 +8421,7 @@
     <n v="49256"/>
     <s v="Production Technician I"/>
     <d v="1974-10-09T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-08-19T00:00:00"/>
     <m/>
@@ -6938,7 +8439,7 @@
     <n v="62957"/>
     <s v="Production Manager"/>
     <d v="1981-07-11T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-06-02T00:00:00"/>
     <m/>
@@ -6956,7 +8457,7 @@
     <n v="63813"/>
     <s v="Production Technician I"/>
     <d v="1983-05-21T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-02-21T00:00:00"/>
     <d v="2014-01-11T00:00:00"/>
@@ -6974,7 +8475,7 @@
     <n v="99020"/>
     <s v="BI Developer"/>
     <d v="1989-06-30T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2017-04-20T00:00:00"/>
     <m/>
@@ -6992,7 +8493,7 @@
     <n v="71707"/>
     <s v="Area Sales Manager"/>
     <d v="1969-02-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-03-07T00:00:00"/>
     <d v="2014-10-31T00:00:00"/>
@@ -7010,7 +8511,7 @@
     <n v="54828"/>
     <s v="Production Technician I"/>
     <d v="1977-03-23T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-11-28T00:00:00"/>
     <m/>
@@ -7028,7 +8529,7 @@
     <n v="64246"/>
     <s v="Production Technician II"/>
     <d v="1988-08-10T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-11-11T00:00:00"/>
     <m/>
@@ -7046,7 +8547,7 @@
     <n v="52177"/>
     <s v="Production Technician I"/>
     <d v="1952-08-18T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-01-09T00:00:00"/>
     <d v="2015-12-15T00:00:00"/>
@@ -7064,7 +8565,7 @@
     <n v="62065"/>
     <s v="Production Technician I"/>
     <d v="1974-05-02T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-05-12T00:00:00"/>
     <m/>
@@ -7082,7 +8583,7 @@
     <n v="46998"/>
     <s v="Production Technician I"/>
     <d v="1984-01-04T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-08-13T00:00:00"/>
     <m/>
@@ -7100,7 +8601,7 @@
     <n v="68099"/>
     <s v="Production Technician II"/>
     <d v="1972-08-27T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2013-06-18T00:00:00"/>
@@ -7118,7 +8619,7 @@
     <n v="70545"/>
     <s v="Area Sales Manager"/>
     <d v="1988-09-14T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-08-18T00:00:00"/>
     <m/>
@@ -7136,7 +8637,7 @@
     <n v="63478"/>
     <s v="Production Technician II"/>
     <d v="1984-02-16T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="Non-Citizen"/>
     <d v="2011-08-15T00:00:00"/>
     <d v="2012-04-07T00:00:00"/>
@@ -7154,7 +8655,7 @@
     <n v="97999"/>
     <s v="Database Administrator"/>
     <d v="1984-02-21T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -7172,7 +8673,7 @@
     <n v="180000"/>
     <s v="Director of Sales"/>
     <d v="1966-03-17T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-05-05T00:00:00"/>
     <m/>
@@ -7190,7 +8691,7 @@
     <n v="49920"/>
     <s v="Administrative Assistant"/>
     <d v="1985-09-16T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-02-16T00:00:00"/>
     <d v="2015-04-15T00:00:00"/>
@@ -7208,7 +8709,7 @@
     <n v="55425"/>
     <s v="Production Technician I"/>
     <d v="1986-06-10T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-02-20T00:00:00"/>
     <m/>
@@ -7226,7 +8727,7 @@
     <n v="69340"/>
     <s v="Production Technician II"/>
     <d v="1984-03-11T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2016-06-06T00:00:00"/>
     <m/>
@@ -7244,7 +8745,7 @@
     <n v="64995"/>
     <s v="Production Technician II"/>
     <d v="1992-05-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-06-05T00:00:00"/>
     <m/>
@@ -7262,7 +8763,7 @@
     <n v="68182"/>
     <s v="Production Technician II"/>
     <d v="1976-09-22T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-02-21T00:00:00"/>
     <d v="2013-04-01T00:00:00"/>
@@ -7280,7 +8781,7 @@
     <n v="83082"/>
     <s v="Production Manager"/>
     <d v="1976-11-15T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-02-21T00:00:00"/>
     <d v="2012-09-24T00:00:00"/>
@@ -7298,7 +8799,7 @@
     <n v="51908"/>
     <s v="Production Technician I"/>
     <d v="1991-01-28T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-08-19T00:00:00"/>
     <m/>
@@ -7316,7 +8817,7 @@
     <n v="61242"/>
     <s v="Production Technician I"/>
     <d v="1972-09-11T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-11-05T00:00:00"/>
     <m/>
@@ -7334,7 +8835,7 @@
     <n v="45069"/>
     <s v="Production Technician I"/>
     <d v="1966-03-22T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-09-30T00:00:00"/>
     <m/>
@@ -7352,7 +8853,7 @@
     <n v="60724"/>
     <s v="Production Technician II"/>
     <d v="1986-11-06T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <m/>
@@ -7370,7 +8871,7 @@
     <n v="60436"/>
     <s v="Production Technician I"/>
     <d v="1964-04-13T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-01-06T00:00:00"/>
     <m/>
@@ -7388,7 +8889,7 @@
     <n v="46837"/>
     <s v="Production Technician I"/>
     <d v="1959-08-19T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-11-07T00:00:00"/>
     <d v="2018-04-29T00:00:00"/>
@@ -7406,7 +8907,7 @@
     <n v="105700"/>
     <s v="Database Administrator"/>
     <d v="1986-11-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <m/>
@@ -7424,7 +8925,7 @@
     <n v="63322"/>
     <s v="Production Technician II"/>
     <d v="1969-09-08T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-07-07T00:00:00"/>
     <m/>
@@ -7442,7 +8943,7 @@
     <n v="61154"/>
     <s v="Production Technician I"/>
     <d v="1986-04-17T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2016-04-01T00:00:00"/>
@@ -7460,7 +8961,7 @@
     <n v="68999"/>
     <s v="Sales Manager"/>
     <d v="1989-11-11T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-11-07T00:00:00"/>
     <d v="2014-04-24T00:00:00"/>
@@ -7478,7 +8979,7 @@
     <n v="50482"/>
     <s v="Production Technician I"/>
     <d v="1976-01-19T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-09-30T00:00:00"/>
     <m/>
@@ -7496,7 +8997,7 @@
     <n v="65310"/>
     <s v="Area Sales Manager"/>
     <d v="1979-11-27T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-08-19T00:00:00"/>
     <m/>
@@ -7514,7 +9015,7 @@
     <n v="250000"/>
     <s v="President &amp; CEO"/>
     <d v="1954-09-21T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-07-02T00:00:00"/>
     <m/>
@@ -7532,7 +9033,7 @@
     <n v="54005"/>
     <s v="Production Technician I"/>
     <d v="1973-12-08T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-09-26T00:00:00"/>
     <d v="2015-06-04T00:00:00"/>
@@ -7550,7 +9051,7 @@
     <n v="45433"/>
     <s v="Production Technician I"/>
     <d v="1970-10-08T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-09-26T00:00:00"/>
     <d v="2014-01-09T00:00:00"/>
@@ -7568,7 +9069,7 @@
     <n v="46654"/>
     <s v="Production Technician I"/>
     <d v="1977-11-10T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-02-17T00:00:00"/>
     <m/>
@@ -7586,7 +9087,7 @@
     <n v="63973"/>
     <s v="Production Technician I"/>
     <d v="1980-02-02T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <m/>
@@ -7604,7 +9105,7 @@
     <n v="71339"/>
     <s v="Area Sales Manager"/>
     <d v="1969-02-24T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-03-07T00:00:00"/>
     <m/>
@@ -7622,7 +9123,7 @@
     <n v="93206"/>
     <s v="Sr. Network Engineer"/>
     <d v="1986-04-23T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-11-10T00:00:00"/>
     <m/>
@@ -7640,7 +9141,7 @@
     <n v="82758"/>
     <s v="Production Manager"/>
     <d v="1972-07-01T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2015-12-12T00:00:00"/>
@@ -7658,7 +9159,7 @@
     <n v="66074"/>
     <s v="Production Technician II"/>
     <d v="1979-07-25T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-01-07T00:00:00"/>
     <d v="2014-03-31T00:00:00"/>
@@ -7676,7 +9177,7 @@
     <n v="46120"/>
     <s v="Production Technician I"/>
     <d v="1986-12-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-07-09T00:00:00"/>
     <m/>
@@ -7694,7 +9195,7 @@
     <n v="64520"/>
     <s v="Accountant I"/>
     <d v="1984-04-26T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-01-06T00:00:00"/>
     <m/>
@@ -7712,7 +9213,7 @@
     <n v="61962"/>
     <s v="Production Technician II"/>
     <d v="1984-05-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-04-02T00:00:00"/>
     <d v="2013-04-15T00:00:00"/>
@@ -7730,7 +9231,7 @@
     <n v="81584"/>
     <s v="Senior BI Developer"/>
     <d v="1987-06-14T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2016-10-02T00:00:00"/>
     <m/>
@@ -7748,7 +9249,7 @@
     <n v="63676"/>
     <s v="Production Technician I"/>
     <d v="1979-01-17T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-09-26T00:00:00"/>
     <d v="2018-08-19T00:00:00"/>
@@ -7766,7 +9267,7 @@
     <n v="93046"/>
     <s v="Shared Services Manager"/>
     <d v="1984-06-10T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2016-01-05T00:00:00"/>
     <m/>
@@ -7784,7 +9285,7 @@
     <n v="64738"/>
     <s v="Production Technician I"/>
     <d v="1982-09-02T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-05-14T00:00:00"/>
     <m/>
@@ -7802,7 +9303,7 @@
     <n v="70468"/>
     <s v="Area Sales Manager"/>
     <d v="1988-12-27T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-04-30T00:00:00"/>
     <m/>
@@ -7820,7 +9321,7 @@
     <n v="77915"/>
     <s v="Production Manager"/>
     <d v="1981-10-26T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-09-30T00:00:00"/>
     <m/>
@@ -7838,7 +9339,7 @@
     <n v="52624"/>
     <s v="Production Technician I"/>
     <d v="1981-03-26T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <d v="2018-09-26T00:00:00"/>
@@ -7856,7 +9357,7 @@
     <n v="63450"/>
     <s v="Production Technician II"/>
     <d v="1979-03-19T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-07-08T00:00:00"/>
     <m/>
@@ -7874,7 +9375,7 @@
     <n v="51777"/>
     <s v="IT Support"/>
     <d v="1988-10-05T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-21T00:00:00"/>
     <m/>
@@ -7892,7 +9393,7 @@
     <n v="67237"/>
     <s v="Production Technician II"/>
     <d v="1976-12-26T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-07-08T00:00:00"/>
     <d v="2016-09-15T00:00:00"/>
@@ -7910,7 +9411,7 @@
     <n v="73330"/>
     <s v="Production Technician II"/>
     <d v="1982-03-28T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-08-19T00:00:00"/>
     <m/>
@@ -7928,7 +9429,7 @@
     <n v="52057"/>
     <s v="Production Technician I"/>
     <d v="1975-10-22T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-02-16T00:00:00"/>
     <m/>
@@ -7946,7 +9447,7 @@
     <n v="47434"/>
     <s v="Production Technician I"/>
     <d v="1973-02-14T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-11-07T00:00:00"/>
     <d v="2015-11-14T00:00:00"/>
@@ -7964,7 +9465,7 @@
     <n v="52788"/>
     <s v="Production Technician I"/>
     <d v="1972-11-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-09-24T00:00:00"/>
     <d v="2017-09-26T00:00:00"/>
@@ -7982,7 +9483,7 @@
     <n v="45395"/>
     <s v="Production Technician I"/>
     <d v="1986-07-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-01-06T00:00:00"/>
     <m/>
@@ -8000,7 +9501,7 @@
     <n v="62385"/>
     <s v="Production Technician II"/>
     <d v="1976-08-25T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2016-05-11T00:00:00"/>
     <m/>
@@ -8018,7 +9519,7 @@
     <n v="68407"/>
     <s v="Production Technician II"/>
     <d v="1986-12-10T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <d v="2012-08-19T00:00:00"/>
@@ -8036,7 +9537,7 @@
     <n v="61349"/>
     <s v="Production Technician I"/>
     <d v="1974-11-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-11-11T00:00:00"/>
     <m/>
@@ -8054,7 +9555,7 @@
     <n v="105688"/>
     <s v="Software Engineer"/>
     <d v="1987-11-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-11-11T00:00:00"/>
     <m/>
@@ -8072,7 +9573,7 @@
     <n v="54132"/>
     <s v="Production Technician I"/>
     <d v="1977-11-22T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-05-31T00:00:00"/>
     <m/>
@@ -8090,7 +9591,7 @@
     <n v="55315"/>
     <s v="Production Technician II"/>
     <d v="1987-05-21T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -8108,7 +9609,7 @@
     <n v="62810"/>
     <s v="Production Technician I"/>
     <d v="1987-01-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-01-07T00:00:00"/>
     <m/>
@@ -8126,7 +9627,7 @@
     <n v="63291"/>
     <s v="Area Sales Manager"/>
     <d v="1984-07-01T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2016-07-06T00:00:00"/>
     <m/>
@@ -8144,7 +9645,7 @@
     <n v="62659"/>
     <s v="Production Technician I"/>
     <d v="1968-05-30T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-04-02T00:00:00"/>
     <d v="2016-11-11T00:00:00"/>
@@ -8162,7 +9663,7 @@
     <n v="55688"/>
     <s v="Production Technician I"/>
     <d v="1976-09-22T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -8180,7 +9681,7 @@
     <n v="83667"/>
     <s v="Production Manager"/>
     <d v="1981-08-10T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-08-16T00:00:00"/>
     <m/>
@@ -8198,7 +9699,7 @@
     <n v="55800"/>
     <s v="Production Technician II"/>
     <d v="1985-06-29T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-08-15T00:00:00"/>
     <d v="2014-09-04T00:00:00"/>
@@ -8216,7 +9717,7 @@
     <n v="58207"/>
     <s v="Production Technician II"/>
     <d v="1992-08-17T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-11-07T00:00:00"/>
     <m/>
@@ -8234,7 +9735,7 @@
     <n v="157000"/>
     <s v="IT Manager - Infra"/>
     <d v="1986-10-05T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="Eligible NonCitizen"/>
     <d v="2012-02-15T00:00:00"/>
     <m/>
@@ -8252,7 +9753,7 @@
     <n v="72460"/>
     <s v="Production Technician II"/>
     <d v="1970-04-24T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-05-13T00:00:00"/>
     <m/>
@@ -8270,7 +9771,7 @@
     <n v="72106"/>
     <s v="Production Technician II"/>
     <d v="1976-12-03T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-01-09T00:00:00"/>
     <m/>
@@ -8288,7 +9789,7 @@
     <n v="52599"/>
     <s v="Network Engineer"/>
     <d v="1979-04-04T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-02-16T00:00:00"/>
     <m/>
@@ -8306,7 +9807,7 @@
     <n v="63430"/>
     <s v="Production Technician I"/>
     <d v="1984-07-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-04-01T00:00:00"/>
     <m/>
@@ -8324,7 +9825,7 @@
     <n v="74417"/>
     <s v="Production Technician II"/>
     <d v="1974-12-01T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-05-13T00:00:00"/>
     <m/>
@@ -8342,7 +9843,7 @@
     <n v="57575"/>
     <s v="Production Technician I"/>
     <d v="1980-04-18T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-07-08T00:00:00"/>
     <m/>
@@ -8360,7 +9861,7 @@
     <n v="87921"/>
     <s v="Senior BI Developer"/>
     <d v="1970-04-25T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2017-02-10T00:00:00"/>
     <m/>
@@ -8378,7 +9879,7 @@
     <n v="50470"/>
     <s v="Production Technician I"/>
     <d v="1989-05-02T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-09-26T00:00:00"/>
     <d v="2014-04-04T00:00:00"/>
@@ -8396,7 +9897,7 @@
     <n v="46664"/>
     <s v="Production Technician I"/>
     <d v="1983-03-28T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-04-01T00:00:00"/>
     <d v="2016-05-25T00:00:00"/>
@@ -8414,7 +9915,7 @@
     <n v="48495"/>
     <s v="Production Technician I"/>
     <d v="1977-04-08T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-05-12T00:00:00"/>
     <m/>
@@ -8432,7 +9933,7 @@
     <n v="52984"/>
     <s v="Production Technician I"/>
     <d v="1967-06-03T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-04-01T00:00:00"/>
     <m/>
@@ -8450,7 +9951,7 @@
     <n v="63695"/>
     <s v="Area Sales Manager"/>
     <d v="1989-03-31T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-07-08T00:00:00"/>
     <m/>
@@ -8468,7 +9969,7 @@
     <n v="62061"/>
     <s v="Production Technician I"/>
     <d v="1984-07-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-07-08T00:00:00"/>
     <m/>
@@ -8486,7 +9987,7 @@
     <n v="66738"/>
     <s v="Production Technician II"/>
     <d v="1985-11-23T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-11-10T00:00:00"/>
     <m/>
@@ -8504,7 +10005,7 @@
     <n v="52674"/>
     <s v="Production Technician I"/>
     <d v="1980-09-30T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-03-31T00:00:00"/>
     <d v="2018-05-01T00:00:00"/>
@@ -8522,7 +10023,7 @@
     <n v="71966"/>
     <s v="Production Technician II"/>
     <d v="1952-02-11T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-05-14T00:00:00"/>
     <d v="2013-08-19T00:00:00"/>
@@ -8540,7 +10041,7 @@
     <n v="63051"/>
     <s v="Area Sales Manager"/>
     <d v="1990-05-11T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-09-30T00:00:00"/>
     <m/>
@@ -8558,7 +10059,7 @@
     <n v="47414"/>
     <s v="Production Technician I"/>
     <d v="1976-12-11T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-09-30T00:00:00"/>
     <m/>
@@ -8576,7 +10077,7 @@
     <n v="53060"/>
     <s v="Production Technician I"/>
     <d v="1979-11-24T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-02-17T00:00:00"/>
     <m/>
@@ -8594,7 +10095,7 @@
     <n v="68829"/>
     <s v="Area Sales Manager"/>
     <d v="1982-05-19T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <m/>
@@ -8612,7 +10113,7 @@
     <n v="63515"/>
     <s v="Production Technician I"/>
     <d v="1979-05-01T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-02-07T00:00:00"/>
     <d v="2014-01-12T00:00:00"/>
@@ -8630,7 +10131,7 @@
     <n v="108987"/>
     <s v="Software Engineer"/>
     <d v="1979-02-20T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-11-07T00:00:00"/>
     <d v="2015-09-07T00:00:00"/>
@@ -8648,7 +10149,7 @@
     <n v="93093"/>
     <s v="Data Analyst"/>
     <d v="1984-09-05T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-12-01T00:00:00"/>
     <d v="2016-05-01T00:00:00"/>
@@ -8666,7 +10167,7 @@
     <n v="53564"/>
     <s v="Production Technician I"/>
     <d v="1988-03-17T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2017-12-28T00:00:00"/>
@@ -8684,7 +10185,7 @@
     <n v="60270"/>
     <s v="Production Technician II"/>
     <d v="1989-07-18T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <d v="2015-09-15T00:00:00"/>
@@ -8702,7 +10203,7 @@
     <n v="45998"/>
     <s v="Production Technician I"/>
     <d v="1986-07-20T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-05-16T00:00:00"/>
     <d v="2015-10-25T00:00:00"/>
@@ -8720,7 +10221,7 @@
     <n v="57954"/>
     <s v="Production Technician II"/>
     <d v="1986-08-17T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-05-16T00:00:00"/>
     <d v="2013-02-04T00:00:00"/>
@@ -8738,7 +10239,7 @@
     <n v="74669"/>
     <s v="Production Manager"/>
     <d v="1977-05-09T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2010-10-25T00:00:00"/>
     <d v="2016-05-18T00:00:00"/>
@@ -8756,7 +10257,7 @@
     <n v="74226"/>
     <s v="Production Technician II"/>
     <d v="1979-03-10T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="Eligible NonCitizen"/>
     <d v="2012-04-02T00:00:00"/>
     <m/>
@@ -8774,7 +10275,7 @@
     <n v="93554"/>
     <s v="Data Analyst"/>
     <d v="1984-09-16T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-11-10T00:00:00"/>
     <m/>
@@ -8792,7 +10293,7 @@
     <n v="64724"/>
     <s v="Production Technician I"/>
     <d v="1988-03-06T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <d v="2012-11-30T00:00:00"/>
@@ -8810,7 +10311,7 @@
     <n v="47001"/>
     <s v="Production Technician I"/>
     <d v="1981-11-23T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2007-11-05T00:00:00"/>
     <m/>
@@ -8828,7 +10329,7 @@
     <n v="61844"/>
     <s v="Area Sales Manager"/>
     <d v="1988-08-29T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-01-09T00:00:00"/>
     <m/>
@@ -8846,7 +10347,7 @@
     <n v="46799"/>
     <s v="Production Technician I"/>
     <d v="1984-10-15T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="Eligible NonCitizen"/>
     <d v="2011-05-16T00:00:00"/>
     <d v="2018-06-04T00:00:00"/>
@@ -8864,7 +10365,7 @@
     <n v="59472"/>
     <s v="Production Technician I"/>
     <d v="1961-06-19T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-01-06T00:00:00"/>
     <m/>
@@ -8882,7 +10383,7 @@
     <n v="46430"/>
     <s v="Production Technician I"/>
     <d v="1970-09-22T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-09-24T00:00:00"/>
     <d v="2013-06-18T00:00:00"/>
@@ -8900,7 +10401,7 @@
     <n v="83363"/>
     <s v="Software Engineer"/>
     <d v="1984-11-06T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="Eligible NonCitizen"/>
     <d v="2011-02-21T00:00:00"/>
     <d v="2015-08-15T00:00:00"/>
@@ -8918,7 +10419,7 @@
     <n v="95920"/>
     <s v="BI Developer"/>
     <d v="1980-05-12T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2016-10-02T00:00:00"/>
     <m/>
@@ -8936,7 +10437,7 @@
     <n v="61729"/>
     <s v="Production Technician I"/>
     <d v="1984-12-31T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-09-26T00:00:00"/>
     <d v="2018-04-07T00:00:00"/>
@@ -8954,7 +10455,7 @@
     <n v="61809"/>
     <s v="Area Sales Manager"/>
     <d v="1954-10-12T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-05-12T00:00:00"/>
     <m/>
@@ -8972,7 +10473,7 @@
     <n v="45115"/>
     <s v="Production Technician I"/>
     <d v="1982-07-22T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-05-16T00:00:00"/>
     <d v="2016-01-15T00:00:00"/>
@@ -8990,7 +10491,7 @@
     <n v="46738"/>
     <s v="Production Technician I"/>
     <d v="1973-01-12T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-11-28T00:00:00"/>
     <m/>
@@ -9008,7 +10509,7 @@
     <n v="64971"/>
     <s v="Production Technician II"/>
     <d v="1981-09-05T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="Eligible NonCitizen"/>
     <d v="2011-09-26T00:00:00"/>
     <d v="2011-10-22T00:00:00"/>
@@ -9026,7 +10527,7 @@
     <n v="55578"/>
     <s v="Production Technician II"/>
     <d v="1972-07-03T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <d v="2012-02-08T00:00:00"/>
@@ -9044,7 +10545,7 @@
     <n v="50428"/>
     <s v="Production Technician I"/>
     <d v="1974-01-07T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2016-01-26T00:00:00"/>
@@ -9062,7 +10563,7 @@
     <n v="61422"/>
     <s v="Production Technician I"/>
     <d v="1985-01-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2016-05-17T00:00:00"/>
@@ -9080,7 +10581,7 @@
     <n v="63353"/>
     <s v="Production Technician I"/>
     <d v="1985-01-28T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-07-08T00:00:00"/>
     <m/>
@@ -9098,7 +10599,7 @@
     <n v="89883"/>
     <s v="Data Analyst"/>
     <d v="1981-10-11T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-02-16T00:00:00"/>
     <m/>
@@ -9116,7 +10617,7 @@
     <n v="120000"/>
     <s v="Principal Data Architect"/>
     <d v="1973-05-27T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <d v="2018-11-10T00:00:00"/>
@@ -9134,7 +10635,7 @@
     <n v="150290"/>
     <s v="Data Architect"/>
     <d v="1972-11-21T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2017-01-07T00:00:00"/>
     <m/>
@@ -9152,7 +10653,7 @@
     <n v="60627"/>
     <s v="Production Technician I"/>
     <d v="1974-12-05T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-01-06T00:00:00"/>
     <m/>
@@ -9170,7 +10671,7 @@
     <n v="53180"/>
     <s v="Production Technician I"/>
     <d v="1987-03-18T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-04-04T00:00:00"/>
     <d v="2018-08-13T00:00:00"/>
@@ -9188,7 +10689,7 @@
     <n v="140920"/>
     <s v="IT Manager - DB"/>
     <d v="1973-04-05T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-01-20T00:00:00"/>
     <m/>
@@ -9206,7 +10707,7 @@
     <n v="148999"/>
     <s v="IT Manager - DB"/>
     <d v="1964-01-04T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-01-09T00:00:00"/>
     <d v="2015-11-04T00:00:00"/>
@@ -9224,7 +10725,7 @@
     <n v="86214"/>
     <s v="Software Engineer"/>
     <d v="1986-07-24T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-11-05T00:00:00"/>
     <m/>
@@ -9242,7 +10743,7 @@
     <n v="47750"/>
     <s v="Production Technician I"/>
     <d v="1968-06-06T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2016-07-04T00:00:00"/>
     <m/>
@@ -9260,7 +10761,7 @@
     <n v="46428"/>
     <s v="Production Technician I"/>
     <d v="1974-12-21T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2009-01-05T00:00:00"/>
     <d v="2018-07-30T00:00:00"/>
@@ -9278,7 +10779,7 @@
     <n v="57975"/>
     <s v="Production Technician II"/>
     <d v="1986-04-26T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2010-08-30T00:00:00"/>
     <m/>
@@ -9296,7 +10797,7 @@
     <n v="88527"/>
     <s v="Data Analyst"/>
     <d v="1987-12-17T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <d v="2015-10-31T00:00:00"/>
@@ -9314,7 +10815,7 @@
     <n v="56147"/>
     <s v="Production Technician I"/>
     <d v="1988-07-10T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -9332,7 +10833,7 @@
     <n v="50923"/>
     <s v="Production Technician I"/>
     <d v="1975-03-10T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-09-30T00:00:00"/>
     <m/>
@@ -9350,7 +10851,7 @@
     <n v="50750"/>
     <s v="Network Engineer"/>
     <d v="1981-04-14T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-09-30T00:00:00"/>
     <m/>
@@ -9368,7 +10869,7 @@
     <n v="52087"/>
     <s v="Production Technician I"/>
     <d v="1985-08-24T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-08-19T00:00:00"/>
     <m/>
@@ -9386,7 +10887,7 @@
     <n v="87826"/>
     <s v="Data Analyst"/>
     <d v="1970-02-08T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <m/>
@@ -9404,7 +10905,7 @@
     <n v="51920"/>
     <s v="Administrative Assistant"/>
     <d v="1988-05-19T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-05-01T00:00:00"/>
     <m/>
@@ -9422,7 +10923,7 @@
     <n v="63878"/>
     <s v="Production Technician II"/>
     <d v="1987-11-25T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2009-10-26T00:00:00"/>
     <d v="2015-04-08T00:00:00"/>
@@ -9440,7 +10941,7 @@
     <n v="60656"/>
     <s v="Production Technician II"/>
     <d v="1963-10-30T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -9458,7 +10959,7 @@
     <n v="72992"/>
     <s v="Sales Manager"/>
     <d v="1984-08-16T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-05-18T00:00:00"/>
     <m/>
@@ -9476,7 +10977,7 @@
     <n v="55000"/>
     <s v="Administrative Assistant"/>
     <d v="1987-06-14T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-09-26T00:00:00"/>
     <d v="2013-09-25T00:00:00"/>
@@ -9494,7 +10995,7 @@
     <n v="58939"/>
     <s v="Production Technician I"/>
     <d v="1965-02-02T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-11-11T00:00:00"/>
     <m/>
@@ -9512,7 +11013,7 @@
     <n v="66593"/>
     <s v="IT Support"/>
     <d v="1973-03-12T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-06-10T00:00:00"/>
     <m/>
@@ -9530,7 +11031,7 @@
     <n v="87565"/>
     <s v="Sr. Network Engineer"/>
     <d v="1983-02-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2016-06-30T00:00:00"/>
     <m/>
@@ -9548,7 +11049,7 @@
     <n v="64021"/>
     <s v="Production Technician I"/>
     <d v="1968-07-20T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-02-20T00:00:00"/>
     <m/>
@@ -9566,7 +11067,7 @@
     <n v="65714"/>
     <s v="Production Manager"/>
     <d v="1975-09-30T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-10-02T00:00:00"/>
     <m/>
@@ -9584,7 +11085,7 @@
     <n v="62425"/>
     <s v="Production Technician I"/>
     <d v="1973-03-26T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-05-13T00:00:00"/>
     <d v="2015-06-29T00:00:00"/>
@@ -9602,7 +11103,7 @@
     <n v="47961"/>
     <s v="Production Technician I"/>
     <d v="1982-08-25T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <m/>
@@ -9620,7 +11121,7 @@
     <n v="58273"/>
     <s v="Area Sales Manager"/>
     <d v="1974-05-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-05-12T00:00:00"/>
     <m/>
@@ -9638,7 +11139,7 @@
     <n v="63003"/>
     <s v="Accountant I"/>
     <d v="1986-09-01T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -9656,7 +11157,7 @@
     <n v="61355"/>
     <s v="Production Technician I"/>
     <d v="1985-03-14T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-02-17T00:00:00"/>
     <m/>
@@ -9674,7 +11175,7 @@
     <n v="60120"/>
     <s v="Area Sales Manager"/>
     <d v="1989-05-12T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2010-09-27T00:00:00"/>
     <m/>
@@ -9692,7 +11193,7 @@
     <n v="63682"/>
     <s v="Production Manager"/>
     <d v="1978-03-28T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2009-01-08T00:00:00"/>
     <m/>
@@ -9710,7 +11211,7 @@
     <n v="63025"/>
     <s v="Production Technician I"/>
     <d v="1982-10-07T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <m/>
@@ -9728,7 +11229,7 @@
     <n v="59238"/>
     <s v="Production Technician I"/>
     <d v="1968-08-15T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="Eligible NonCitizen"/>
     <d v="2012-05-14T00:00:00"/>
     <m/>
@@ -9746,7 +11247,7 @@
     <n v="92989"/>
     <s v="Software Engineer"/>
     <d v="1983-05-06T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-07-07T00:00:00"/>
     <m/>
@@ -9764,7 +11265,7 @@
     <n v="90100"/>
     <s v="BI Developer"/>
     <d v="1987-10-24T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2017-04-20T00:00:00"/>
     <m/>
@@ -9782,7 +11283,7 @@
     <n v="60754"/>
     <s v="Production Technician I"/>
     <d v="1975-04-03T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="Non-Citizen"/>
     <d v="2009-04-27T00:00:00"/>
     <d v="2013-04-01T00:00:00"/>
@@ -9800,7 +11301,7 @@
     <n v="72202"/>
     <s v="Production Technician II"/>
     <d v="1953-05-24T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-05-16T00:00:00"/>
     <d v="2017-07-08T00:00:00"/>
@@ -9818,7 +11319,7 @@
     <n v="58370"/>
     <s v="Area Sales Manager"/>
     <d v="1965-05-07T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -9836,7 +11337,7 @@
     <n v="48413"/>
     <s v="Production Technician I"/>
     <d v="1965-05-09T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <d v="2016-09-05T00:00:00"/>
@@ -9854,7 +11355,7 @@
     <n v="67176"/>
     <s v="Production Technician II"/>
     <d v="1975-09-16T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2007-06-25T00:00:00"/>
     <d v="2010-08-30T00:00:00"/>
@@ -9872,7 +11373,7 @@
     <n v="56339"/>
     <s v="Production Technician I"/>
     <d v="1967-06-05T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2013-02-18T00:00:00"/>
     <m/>
@@ -9890,7 +11391,7 @@
     <n v="64397"/>
     <s v="Area Sales Manager"/>
     <d v="1968-01-15T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2006-01-09T00:00:00"/>
     <m/>
@@ -9908,7 +11409,7 @@
     <n v="63025"/>
     <s v="Production Technician I"/>
     <d v="1983-05-16T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-02-17T00:00:00"/>
     <m/>
@@ -9926,7 +11427,7 @@
     <n v="75281"/>
     <s v="Network Engineer"/>
     <d v="1988-05-05T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-01-05T00:00:00"/>
     <d v="2016-02-12T00:00:00"/>
@@ -9944,7 +11445,7 @@
     <n v="100416"/>
     <s v="Software Engineer"/>
     <d v="1983-06-14T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="Non-Citizen"/>
     <d v="2013-02-18T00:00:00"/>
     <d v="2018-04-15T00:00:00"/>
@@ -9962,7 +11463,7 @@
     <n v="74813"/>
     <s v="Production Technician II"/>
     <d v="1985-03-15T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2014-07-02T00:00:00"/>
@@ -9980,7 +11481,7 @@
     <n v="76029"/>
     <s v="Network Engineer"/>
     <d v="1969-03-31T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="Eligible NonCitizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -9998,7 +11499,7 @@
     <n v="57859"/>
     <s v="Area Sales Manager"/>
     <d v="1991-05-23T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-07-05T00:00:00"/>
     <m/>
@@ -10016,7 +11517,7 @@
     <n v="58523"/>
     <s v="Production Technician I"/>
     <d v="1987-01-31T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-08-13T00:00:00"/>
     <d v="2016-02-05T00:00:00"/>
@@ -10034,7 +11535,7 @@
     <n v="88976"/>
     <s v="Production Manager"/>
     <d v="1968-10-10T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-08-01T00:00:00"/>
     <m/>
@@ -10052,7 +11553,7 @@
     <n v="55875"/>
     <s v="Area Sales Manager"/>
     <d v="1989-07-11T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2012-03-05T00:00:00"/>
     <m/>
@@ -10070,7 +11571,7 @@
     <n v="113999"/>
     <s v="Database Administrator"/>
     <d v="1986-08-07T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2015-02-16T00:00:00"/>
     <d v="2017-02-22T00:00:00"/>
@@ -10088,7 +11589,7 @@
     <n v="49773"/>
     <s v="Production Technician I"/>
     <d v="1986-06-03T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-09-26T00:00:00"/>
     <d v="2016-02-08T00:00:00"/>
@@ -10106,7 +11607,7 @@
     <n v="62068"/>
     <s v="Production Technician I"/>
     <d v="1985-04-06T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-07-05T00:00:00"/>
     <m/>
@@ -10124,7 +11625,7 @@
     <n v="66541"/>
     <s v="Production Technician II"/>
     <d v="1976-02-10T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-08-18T00:00:00"/>
     <m/>
@@ -10142,7 +11643,7 @@
     <n v="80512"/>
     <s v="Production Manager"/>
     <d v="1955-11-14T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-09-26T00:00:00"/>
     <d v="2012-01-02T00:00:00"/>
@@ -10160,7 +11661,7 @@
     <n v="50274"/>
     <s v="Production Technician I"/>
     <d v="1980-08-02T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-08-13T00:00:00"/>
     <d v="2015-09-01T00:00:00"/>
@@ -10178,7 +11679,7 @@
     <n v="84903"/>
     <s v="Senior BI Developer"/>
     <d v="1981-07-08T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2017-02-15T00:00:00"/>
     <m/>
@@ -10196,7 +11697,7 @@
     <n v="107226"/>
     <s v="Sr. Network Engineer"/>
     <d v="1978-05-02T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -10214,7 +11715,7 @@
     <n v="58371"/>
     <s v="Production Technician I"/>
     <d v="1987-05-24T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2014-05-15T00:00:00"/>
@@ -10232,7 +11733,7 @@
     <n v="55140"/>
     <s v="Production Technician I"/>
     <d v="1965-09-09T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="Eligible NonCitizen"/>
     <d v="2011-05-16T00:00:00"/>
     <d v="2015-09-07T00:00:00"/>
@@ -10250,7 +11751,7 @@
     <n v="58062"/>
     <s v="Production Technician I"/>
     <d v="1983-07-30T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2011-01-10T00:00:00"/>
     <d v="2012-05-14T00:00:00"/>
@@ -10268,7 +11769,7 @@
     <n v="59728"/>
     <s v="Production Technician I"/>
     <d v="1969-10-02T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2012-01-09T00:00:00"/>
     <d v="2015-06-27T00:00:00"/>
@@ -10286,7 +11787,7 @@
     <n v="70507"/>
     <s v="Production Technician II"/>
     <d v="1958-11-07T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2013-01-07T00:00:00"/>
     <d v="2016-02-21T00:00:00"/>
@@ -10304,7 +11805,7 @@
     <n v="60446"/>
     <s v="Production Technician II"/>
     <d v="1985-04-20T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -10322,7 +11823,7 @@
     <n v="65893"/>
     <s v="Production Technician II"/>
     <d v="1985-05-11T00:00:00"/>
-    <s v="M "/>
+    <x v="0"/>
     <s v="US Citizen"/>
     <d v="2014-07-07T00:00:00"/>
     <m/>
@@ -10340,7 +11841,7 @@
     <n v="48513"/>
     <s v="Production Technician I"/>
     <d v="1982-05-04T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2008-09-02T00:00:00"/>
     <d v="2015-09-29T00:00:00"/>
@@ -10358,7 +11859,7 @@
     <n v="220450"/>
     <s v="CIO"/>
     <d v="1979-08-30T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2010-04-10T00:00:00"/>
     <m/>
@@ -10376,7 +11877,7 @@
     <n v="89292"/>
     <s v="Data Analyst"/>
     <d v="1979-02-24T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2015-03-30T00:00:00"/>
     <m/>
@@ -10394,7 +11895,7 @@
     <n v="45046"/>
     <s v="Production Technician I"/>
     <d v="1978-08-17T00:00:00"/>
-    <s v="F"/>
+    <x v="1"/>
     <s v="US Citizen"/>
     <d v="2014-09-29T00:00:00"/>
     <m/>
@@ -10409,7 +11910,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{522A496A-A047-4258-90E9-EEA28A2DD2FD}" name="Зведена таблиця1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Department">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{522A496A-A047-4258-90E9-EEA28A2DD2FD}" name="Зведена таблиця1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Department">
   <location ref="A3:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -10782,6 +12283,192 @@
           </reference>
           <reference field="12" count="1" selected="0">
             <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{99C9EE08-55A3-4A4F-80AE-C08BB2D6FC1E}" name="Зведена таблиця1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Gender/ Employment status">
+  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="6"/>
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Кількість з EmploymentStatus" fld="11" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="7">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -12746,7 +14433,7 @@
   <dimension ref="A1:P313"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B12" sqref="A2:P312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22583,7 +24270,7 @@
       </c>
       <c r="O197">
         <f ca="1">DATEDIF(HRDataset_raw[[#This Row],[DOB]], TODAY(), "Y")</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P197">
         <f ca="1">DATEDIF(HRDataset_raw[[#This Row],[DateofHire]], IF(HRDataset_raw[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_raw[[#This Row],[DateofTermination]]),"Y")</f>
@@ -28388,7 +30075,7 @@
       </c>
       <c r="O313" s="7">
         <f ca="1">SUBTOTAL(101,HRDataset_raw[Age])</f>
-        <v>46.350482315112544</v>
+        <v>46.353697749196144</v>
       </c>
       <c r="P313" s="7">
         <f ca="1">SUBTOTAL(101,HRDataset_raw[Experience])</f>
@@ -28410,9 +30097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDDB79FC-3D38-4439-81DE-E0963891CD7B}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -28421,14 +30106,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>726</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -28442,7 +30127,7 @@
       <c r="A4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4">
         <v>209</v>
       </c>
     </row>
@@ -28450,7 +30135,7 @@
       <c r="A5" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5">
         <v>126</v>
       </c>
     </row>
@@ -28458,7 +30143,7 @@
       <c r="A6" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6">
         <v>8</v>
       </c>
     </row>
@@ -28466,7 +30151,7 @@
       <c r="A7" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7">
         <v>75</v>
       </c>
     </row>
@@ -28474,7 +30159,7 @@
       <c r="A8" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8">
         <v>50</v>
       </c>
     </row>
@@ -28482,7 +30167,7 @@
       <c r="A9" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9">
         <v>40</v>
       </c>
     </row>
@@ -28490,7 +30175,7 @@
       <c r="A10" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10">
         <v>4</v>
       </c>
     </row>
@@ -28498,7 +30183,7 @@
       <c r="A11" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11">
         <v>6</v>
       </c>
     </row>
@@ -28506,7 +30191,7 @@
       <c r="A12" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12">
         <v>31</v>
       </c>
     </row>
@@ -28514,7 +30199,7 @@
       <c r="A13" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13">
         <v>26</v>
       </c>
     </row>
@@ -28522,7 +30207,7 @@
       <c r="A14" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14">
         <v>2</v>
       </c>
     </row>
@@ -28530,7 +30215,7 @@
       <c r="A15" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15">
         <v>3</v>
       </c>
     </row>
@@ -28538,7 +30223,7 @@
       <c r="A16" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16">
         <v>11</v>
       </c>
     </row>
@@ -28546,7 +30231,7 @@
       <c r="A17" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17">
         <v>7</v>
       </c>
     </row>
@@ -28554,7 +30239,7 @@
       <c r="A18" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18">
         <v>1</v>
       </c>
     </row>
@@ -28562,7 +30247,7 @@
       <c r="A19" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19">
         <v>3</v>
       </c>
     </row>
@@ -28570,7 +30255,7 @@
       <c r="A20" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20">
         <v>9</v>
       </c>
     </row>
@@ -28578,7 +30263,7 @@
       <c r="A21" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21">
         <v>7</v>
       </c>
     </row>
@@ -28586,7 +30271,7 @@
       <c r="A22" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22">
         <v>1</v>
       </c>
     </row>
@@ -28594,7 +30279,7 @@
       <c r="A23" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23">
         <v>1</v>
       </c>
     </row>
@@ -28602,7 +30287,7 @@
       <c r="A24" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24">
         <v>1</v>
       </c>
     </row>
@@ -28610,7 +30295,7 @@
       <c r="A25" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25">
         <v>1</v>
       </c>
     </row>
@@ -28618,7 +30303,114 @@
       <c r="A26" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CAE9A5C-F3D5-495C-B8E0-9A4F69F2AB21}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>728</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="B3" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B4" s="13">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="13">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="B6" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="B7" s="13">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B8" s="13">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="B9" s="13">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="B10" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="B11" s="13">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="B12" s="13">
         <v>311</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add turnover analysis by working experience
1. Created a new sheet for turnover analysis by working experience.
2. Built a PivotTable showing termination types across different experience levels.
3. Added a horizontal bar chart to visualize how experience correlates with employee dismissal categories.
4. Wrote insights summarizing key findings:
   - The company retains experienced employees exceptionally well; they form the stable core of the workforce.
   - Turnover is highest among newcomers with low tenure.
   - Reason for dismissal does not significantly differ for new employees - both voluntarily and involuntarily terminated individuals have similarly short experience.
</commit_message>
<xml_diff>
--- a/HRDataset_analysis.xlsx
+++ b/HRDataset_analysis.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8beb163ab15076dd/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="572" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCAEDFC5-EEB9-42DA-A4C7-953D04092DC5}"/>
+  <xr:revisionPtr revIDLastSave="696" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DF92774-4B79-458E-A46B-AA4276B36B61}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
   </bookViews>
   <sheets>
     <sheet name="HRDataset_raw" sheetId="1" r:id="rId1"/>
     <sheet name="HRDataset_clean" sheetId="2" r:id="rId2"/>
     <sheet name="Turnover_by_department" sheetId="5" r:id="rId3"/>
     <sheet name="Turnover_by_gender" sheetId="6" r:id="rId4"/>
+    <sheet name="Turnover_by_experience" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">HRDataset_clean!$A$1:$N$312</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="732">
   <si>
     <t>Employee_Name,EmpID,MarriedID,MaritalStatusID,GenderID,EmpStatusID,DeptID,PerfScoreID,FromDiversityJobFairID,Salary,Termd,PositionID,Position,State,Zip,DOB,Sex,MaritalDesc,CitizenDesc,HispanicLatino,RaceDesc,DateofHire,DateofTermination,TermReason,EmploymentStatus,Department,ManagerName,ManagerID,RecruitmentSource,PerformanceScore,EngagementSurvey,EmpSatisfaction,SpecialProjectsCount,LastPerformanceReview_Date,DaysLateLast30,Absences</t>
   </si>
@@ -2237,12 +2238,24 @@
   </si>
   <si>
     <t>Does the turnover differ between men and women?</t>
+  </si>
+  <si>
+    <t>Середнє з Experience</t>
+  </si>
+  <si>
+    <t>Employment Status</t>
+  </si>
+  <si>
+    <t>What is the average experience of the terminated employees?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2785,7 +2798,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% – колірна тема 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4063,19 +4076,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="70000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -4688,6 +4689,556 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="uk-UA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[HRDataset_analysis.xlsx]Turnover_by_experience!Зведена таблиця1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>The average experience of the terminated employees</a:t>
+            </a:r>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="uk-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="diamond"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="uk-UA"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Turnover_by_experience!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Підсумок</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="uk-UA"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Turnover_by_experience!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Active</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terminated for Cause</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Voluntarily Terminated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Turnover_by_experience!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>11.768115942028986</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0795454545454546</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-54BC-4432-A5D7-541394251554}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
+        <c:axId val="425949696"/>
+        <c:axId val="425950176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="425949696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="425950176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="425950176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="425949696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="uk-UA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4729,6 +5280,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5752,6 +6343,508 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="341">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6222,6 +7315,242 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Діаграма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72B08445-2B5B-3EAD-ACD5-463887C99996}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27516639-ED0C-9B95-3C9B-F6C73B26139D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8185150" y="419100"/>
+          <a:ext cx="4864100" cy="2768600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>►</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Insights</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Active employees have longer experience (11.8 years), which is significantly higher than the total average (8.9 years). </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" u="sng"/>
+            <a:t>This suggests that the company has a core of experienced employees and those, who stay with the company, work for a long time.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Dismissed employees (both voluntarily and for cause) have a relatively lower experience - 3.1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>years. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" u="sng"/>
+            <a:t>This may indicate a high level of turnover among new employees</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.The reason for dismissal (forced or voluntary) does not greatly affect the experience - in both cases the experience is the same.The total average of the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>employees </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>working</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> experience</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>(8.9 years) is formed due to the long experience of active employees and the low </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>experience</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> of new employees.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Thus,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>the company retains long-term employees very well, but there is a problem with maintaining newcomers. Perhaps it is worth reviewing the system of adaptation, conditions or motivation in the first years of work to reduce early dismissals.</a:t>
+          </a:r>
+          <a:endParaRPr lang="uk-UA" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12486,6 +13815,80 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CD0F9E0-F6E8-4E42-A55B-30816338B9A3}" name="Зведена таблиця1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Employment Status">
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Середнє з Experience" fld="15" subtotal="average" baseField="11" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{388B7420-0CF7-4AE2-B5C1-F9E5B62D966B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="17" unboundColumnsRight="2">
@@ -18181,7 +19584,7 @@
       </c>
       <c r="O75">
         <f ca="1">DATEDIF(HRDataset_raw[[#This Row],[DOB]], TODAY(), "Y")</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P75">
         <f ca="1">DATEDIF(HRDataset_raw[[#This Row],[DateofHire]], IF(HRDataset_raw[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_raw[[#This Row],[DateofTermination]]),"Y")</f>
@@ -19577,7 +20980,7 @@
       </c>
       <c r="O103">
         <f ca="1">DATEDIF(HRDataset_raw[[#This Row],[DOB]], TODAY(), "Y")</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P103">
         <f ca="1">DATEDIF(HRDataset_raw[[#This Row],[DateofHire]], IF(HRDataset_raw[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_raw[[#This Row],[DateofTermination]]),"Y")</f>
@@ -24123,7 +25526,7 @@
       </c>
       <c r="O194">
         <f ca="1">DATEDIF(HRDataset_raw[[#This Row],[DOB]], TODAY(), "Y")</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P194">
         <f ca="1">DATEDIF(HRDataset_raw[[#This Row],[DateofHire]], IF(HRDataset_raw[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_raw[[#This Row],[DateofTermination]]),"Y")</f>
@@ -30075,7 +31478,7 @@
       </c>
       <c r="O313" s="7">
         <f ca="1">SUBTOTAL(101,HRDataset_raw[Age])</f>
-        <v>46.353697749196144</v>
+        <v>46.363344051446944</v>
       </c>
       <c r="P313" s="7">
         <f ca="1">SUBTOTAL(101,HRDataset_raw[Experience])</f>
@@ -30317,9 +31720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CAE9A5C-F3D5-495C-B8E0-9A4F69F2AB21}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -30346,7 +31747,7 @@
       <c r="A4" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4">
         <v>176</v>
       </c>
     </row>
@@ -30354,7 +31755,7 @@
       <c r="A5" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5">
         <v>116</v>
       </c>
     </row>
@@ -30362,7 +31763,7 @@
       <c r="A6" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6">
         <v>9</v>
       </c>
     </row>
@@ -30370,7 +31771,7 @@
       <c r="A7" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7">
         <v>51</v>
       </c>
     </row>
@@ -30378,7 +31779,7 @@
       <c r="A8" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8">
         <v>135</v>
       </c>
     </row>
@@ -30386,7 +31787,7 @@
       <c r="A9" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9">
         <v>91</v>
       </c>
     </row>
@@ -30394,7 +31795,7 @@
       <c r="A10" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10">
         <v>7</v>
       </c>
     </row>
@@ -30402,7 +31803,7 @@
       <c r="A11" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11">
         <v>37</v>
       </c>
     </row>
@@ -30410,8 +31811,77 @@
       <c r="A12" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12">
         <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E7C527-6DB8-4487-8FC3-B0D67CA75A59}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>731</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="B3" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="13">
+        <v>11.768115942028986</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" s="13">
+        <v>3.0625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B6" s="13">
+        <v>3.0795454545454546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="B7" s="13">
+        <v>8.8617363344051441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replace pie chart with bar chart in gender salary analysis
1. Improved clarity and readability of the salary comparison by using a chart type that is better suited for displaying differences between two groups.
</commit_message>
<xml_diff>
--- a/HRDataset_analysis.xlsx
+++ b/HRDataset_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8beb163ab15076dd/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="831" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE95503C-F077-486C-90D2-B23A545C4AFC}"/>
+  <xr:revisionPtr revIDLastSave="844" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36E6A1DF-CC96-459B-85CF-CFD714E4DFBA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="5" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2840,7 +2840,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2863,7 +2863,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="16" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2912,7 +2911,14 @@
   </cellStyles>
   <dxfs count="34">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2923,14 +2929,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -5383,8 +5382,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -5418,7 +5416,7 @@
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
@@ -5484,14 +5482,10 @@
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
-                <a:fld id="{081874C2-3C5D-4DB0-A2A1-11D9C745EA98}" type="PERCENTAGE">
+                <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:pPr>
-                    <a:defRPr/>
-                  </a:pPr>
-                  <a:t>[ВІДСОТОК]</a:t>
-                </a:fld>
-                <a:endParaRPr lang="uk-UA"/>
+                  <a:t>47,6%</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5525,7 +5519,7 @@
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
@@ -5557,8 +5551,8 @@
           <c:idx val="0"/>
           <c:layout>
             <c:manualLayout>
-              <c:x val="-7.9866888519134774E-2"/>
-              <c:y val="9.8495212038303692E-2"/>
+              <c:x val="0.16081334371754932"/>
+              <c:y val="-2.5686871466380095E-3"/>
             </c:manualLayout>
           </c:layout>
           <c:tx>
@@ -5594,14 +5588,10 @@
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
-                <a:fld id="{4FE36007-2092-46F4-A916-7A869A2E2044}" type="PERCENTAGE">
+                <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:pPr>
-                    <a:defRPr/>
-                  </a:pPr>
-                  <a:t>[ВІДСОТОК]</a:t>
-                </a:fld>
-                <a:endParaRPr lang="uk-UA"/>
+                  <a:t>52,4%</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5635,7 +5625,7 @@
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
@@ -5648,8 +5638,10 @@
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
-      <c:doughnutChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5665,6 +5657,32 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln w="12700">
               <a:solidFill>
                 <a:schemeClr val="accent1">
@@ -5672,9 +5690,12 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -5700,6 +5721,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -5748,12 +5770,10 @@
                     </a:r>
                   </a:p>
                   <a:p>
-                    <a:fld id="{081874C2-3C5D-4DB0-A2A1-11D9C745EA98}" type="PERCENTAGE">
+                    <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[ВІДСОТОК]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="uk-UA"/>
+                      <a:t>47,6%</a:t>
+                    </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -5761,7 +5781,7 @@
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
+              <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
@@ -5777,8 +5797,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.9866888519134774E-2"/>
-                  <c:y val="9.8495212038303692E-2"/>
+                  <c:x val="0.16081334371754932"/>
+                  <c:y val="-2.5686871466380095E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -5797,12 +5817,10 @@
                     </a:r>
                   </a:p>
                   <a:p>
-                    <a:fld id="{4FE36007-2092-46F4-A916-7A869A2E2044}" type="PERCENTAGE">
+                    <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[ВІДСОТОК]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="uk-UA"/>
+                      <a:t>52,4%</a:t>
+                    </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -5810,7 +5828,7 @@
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
+              <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
@@ -5852,24 +5870,26 @@
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
+            <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5914,11 +5934,110 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-        <c:holeSize val="75"/>
-      </c:doughnutChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="19026335"/>
+        <c:axId val="2134147343"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="19026335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2134147343"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2134147343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="19026335"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -14679,7 +14798,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{522A496A-A047-4258-90E9-EEA28A2DD2FD}" name="Зведена таблиця1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Department">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{522A496A-A047-4258-90E9-EEA28A2DD2FD}" name="Зведена таблиця1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Department">
   <location ref="A3:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -15070,7 +15189,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{99C9EE08-55A3-4A4F-80AE-C08BB2D6FC1E}" name="Зведена таблиця1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Gender/ Employment status">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{99C9EE08-55A3-4A4F-80AE-C08BB2D6FC1E}" name="Зведена таблиця1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Gender/ Employment status">
   <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -15256,7 +15375,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CD0F9E0-F6E8-4E42-A55B-30816338B9A3}" name="Зведена таблиця1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Employment Status">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CD0F9E0-F6E8-4E42-A55B-30816338B9A3}" name="Зведена таблиця1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Employment Status">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -15330,7 +15449,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B618E153-E906-4623-A1B0-AE62734F806F}" name="Зведена таблиця1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Gender">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B618E153-E906-4623-A1B0-AE62734F806F}" name="Зведена таблиця1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Gender">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -15473,7 +15592,7 @@
     <tableColumn id="16" xr3:uid="{4DB63E1C-C3BC-4899-8FC0-92DDE29B5436}" uniqueName="16" name="Experience" totalsRowFunction="average" queryTableFieldId="16" dataDxfId="4" totalsRowDxfId="3">
       <calculatedColumnFormula>DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{85CD6633-1FC4-49C5-AE01-4B6A7DA7D31A}" uniqueName="17" name="Стовпець1" queryTableFieldId="17" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="17" xr3:uid="{85CD6633-1FC4-49C5-AE01-4B6A7DA7D31A}" uniqueName="17" name="Стовпець1" queryTableFieldId="17" dataDxfId="2" totalsRowDxfId="1">
       <calculatedColumnFormula>LEN(HRDataset_clean[[#This Row],[Sex]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -17497,7 +17616,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q2" s="16">
+      <c r="Q2">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -17553,7 +17672,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -17609,7 +17728,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -17662,7 +17781,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>17</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -17718,7 +17837,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="Q6">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -17771,7 +17890,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -17824,7 +17943,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q8" s="16">
+      <c r="Q8">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -17877,7 +17996,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q9" s="16">
+      <c r="Q9">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -17930,7 +18049,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>16</v>
       </c>
-      <c r="Q10" s="16">
+      <c r="Q10">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -17983,7 +18102,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q11" s="16">
+      <c r="Q11">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -18039,7 +18158,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>6</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -18095,7 +18214,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q13" s="16">
+      <c r="Q13">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -18148,7 +18267,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="Q14">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -18201,7 +18320,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q15" s="16">
+      <c r="Q15">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -18257,7 +18376,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q16" s="16">
+      <c r="Q16">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -18313,7 +18432,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>6</v>
       </c>
-      <c r="Q17" s="16">
+      <c r="Q17">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -18366,7 +18485,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q18" s="16">
+      <c r="Q18">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -18419,7 +18538,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q19" s="16">
+      <c r="Q19">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -18475,7 +18594,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q20" s="16">
+      <c r="Q20">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -18528,7 +18647,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q21" s="16">
+      <c r="Q21">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -18581,7 +18700,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q22" s="16">
+      <c r="Q22">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -18634,7 +18753,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q23" s="16">
+      <c r="Q23">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -18687,7 +18806,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q24" s="16">
+      <c r="Q24">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -18740,7 +18859,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q25" s="16">
+      <c r="Q25">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -18796,7 +18915,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q26" s="16">
+      <c r="Q26">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -18852,7 +18971,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q27" s="16">
+      <c r="Q27">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -18905,7 +19024,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q28" s="16">
+      <c r="Q28">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -18961,7 +19080,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>0</v>
       </c>
-      <c r="Q29" s="16">
+      <c r="Q29">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -19017,7 +19136,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q30" s="16">
+      <c r="Q30">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19070,7 +19189,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>17</v>
       </c>
-      <c r="Q31" s="16">
+      <c r="Q31">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19123,7 +19242,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q32" s="16">
+      <c r="Q32">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -19176,7 +19295,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q33" s="16">
+      <c r="Q33">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19232,7 +19351,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q34" s="16">
+      <c r="Q34">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19285,7 +19404,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q35" s="16">
+      <c r="Q35">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19338,7 +19457,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q36" s="16">
+      <c r="Q36">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -19391,7 +19510,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q37" s="16">
+      <c r="Q37">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -19444,7 +19563,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q38" s="16">
+      <c r="Q38">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -19497,7 +19616,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q39" s="16">
+      <c r="Q39">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19550,7 +19669,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q40" s="16">
+      <c r="Q40">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -19603,7 +19722,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q41" s="16">
+      <c r="Q41">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19656,7 +19775,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q42" s="16">
+      <c r="Q42">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19709,7 +19828,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q43" s="16">
+      <c r="Q43">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19762,7 +19881,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q44" s="16">
+      <c r="Q44">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -19815,7 +19934,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q45" s="16">
+      <c r="Q45">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -19868,7 +19987,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q46" s="16">
+      <c r="Q46">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -19921,7 +20040,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q47" s="16">
+      <c r="Q47">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -19977,7 +20096,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q48" s="16">
+      <c r="Q48">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -20030,7 +20149,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q49" s="16">
+      <c r="Q49">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -20083,7 +20202,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q50" s="16">
+      <c r="Q50">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20139,7 +20258,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q51" s="16">
+      <c r="Q51">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -20195,7 +20314,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q52" s="16">
+      <c r="Q52">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20248,7 +20367,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q53" s="16">
+      <c r="Q53">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20301,7 +20420,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q54" s="16">
+      <c r="Q54">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20357,7 +20476,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q55" s="16">
+      <c r="Q55">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20410,7 +20529,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>15</v>
       </c>
-      <c r="Q56" s="16">
+      <c r="Q56">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20463,7 +20582,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>16</v>
       </c>
-      <c r="Q57" s="16">
+      <c r="Q57">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20516,7 +20635,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q58" s="16">
+      <c r="Q58">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -20569,7 +20688,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q59" s="16">
+      <c r="Q59">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20622,7 +20741,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q60" s="16">
+      <c r="Q60">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -20675,7 +20794,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q61" s="16">
+      <c r="Q61">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20728,7 +20847,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q62" s="16">
+      <c r="Q62">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -20781,7 +20900,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q63" s="16">
+      <c r="Q63">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -20834,7 +20953,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q64" s="16">
+      <c r="Q64">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -20887,7 +21006,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q65" s="16">
+      <c r="Q65">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20940,7 +21059,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>7</v>
       </c>
-      <c r="Q66" s="16">
+      <c r="Q66">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -20996,7 +21115,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q67" s="16">
+      <c r="Q67">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -21049,7 +21168,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q68" s="16">
+      <c r="Q68">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21102,7 +21221,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q69" s="16">
+      <c r="Q69">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -21158,7 +21277,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q70" s="16">
+      <c r="Q70">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21211,7 +21330,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q71" s="16">
+      <c r="Q71">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -21264,7 +21383,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>8</v>
       </c>
-      <c r="Q72" s="16">
+      <c r="Q72">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -21317,7 +21436,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q73" s="16">
+      <c r="Q73">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -21370,7 +21489,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q74" s="16">
+      <c r="Q74">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21423,7 +21542,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q75" s="16">
+      <c r="Q75">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21476,7 +21595,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q76" s="16">
+      <c r="Q76">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21529,7 +21648,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q77" s="16">
+      <c r="Q77">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21582,7 +21701,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q78" s="16">
+      <c r="Q78">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -21635,7 +21754,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q79" s="16">
+      <c r="Q79">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21688,7 +21807,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q80" s="16">
+      <c r="Q80">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21741,7 +21860,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>15</v>
       </c>
-      <c r="Q81" s="16">
+      <c r="Q81">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21797,7 +21916,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>6</v>
       </c>
-      <c r="Q82" s="16">
+      <c r="Q82">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -21850,7 +21969,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q83" s="16">
+      <c r="Q83">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -21903,7 +22022,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q84" s="16">
+      <c r="Q84">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -21956,7 +22075,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q85" s="16">
+      <c r="Q85">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22012,7 +22131,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>6</v>
       </c>
-      <c r="Q86" s="16">
+      <c r="Q86">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -22068,7 +22187,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q87" s="16">
+      <c r="Q87">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22124,7 +22243,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q88" s="16">
+      <c r="Q88">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22177,7 +22296,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q89" s="16">
+      <c r="Q89">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22230,7 +22349,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q90" s="16">
+      <c r="Q90">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22286,7 +22405,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q91" s="16">
+      <c r="Q91">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22339,7 +22458,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q92" s="16">
+      <c r="Q92">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -22392,7 +22511,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q93" s="16">
+      <c r="Q93">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -22445,7 +22564,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q94" s="16">
+      <c r="Q94">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22501,7 +22620,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q95" s="16">
+      <c r="Q95">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -22557,7 +22676,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q96" s="16">
+      <c r="Q96">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22613,7 +22732,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q97" s="16">
+      <c r="Q97">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -22666,7 +22785,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q98" s="16">
+      <c r="Q98">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -22719,7 +22838,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>16</v>
       </c>
-      <c r="Q99" s="16">
+      <c r="Q99">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22772,7 +22891,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q100" s="16">
+      <c r="Q100">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -22825,7 +22944,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>15</v>
       </c>
-      <c r="Q101" s="16">
+      <c r="Q101">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22878,7 +22997,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q102" s="16">
+      <c r="Q102">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -22931,7 +23050,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q103" s="16">
+      <c r="Q103">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -22984,7 +23103,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q104" s="16">
+      <c r="Q104">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23040,7 +23159,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q105" s="16">
+      <c r="Q105">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23096,7 +23215,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q106" s="16">
+      <c r="Q106">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23152,7 +23271,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q107" s="16">
+      <c r="Q107">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -23205,7 +23324,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q108" s="16">
+      <c r="Q108">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23258,7 +23377,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q109" s="16">
+      <c r="Q109">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23314,7 +23433,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>0</v>
       </c>
-      <c r="Q110" s="16">
+      <c r="Q110">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23367,7 +23486,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q111" s="16">
+      <c r="Q111">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -23420,7 +23539,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q112" s="16">
+      <c r="Q112">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23473,7 +23592,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q113" s="16">
+      <c r="Q113">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -23529,7 +23648,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q114" s="16">
+      <c r="Q114">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -23582,7 +23701,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q115" s="16">
+      <c r="Q115">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23635,7 +23754,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q116" s="16">
+      <c r="Q116">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23688,7 +23807,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q117" s="16">
+      <c r="Q117">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -23741,7 +23860,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q118" s="16">
+      <c r="Q118">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23794,7 +23913,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q119" s="16">
+      <c r="Q119">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23847,7 +23966,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q120" s="16">
+      <c r="Q120">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -23903,7 +24022,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q121" s="16">
+      <c r="Q121">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -23956,7 +24075,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>8</v>
       </c>
-      <c r="Q122" s="16">
+      <c r="Q122">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -24012,7 +24131,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q123" s="16">
+      <c r="Q123">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -24065,7 +24184,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q124" s="16">
+      <c r="Q124">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24118,7 +24237,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q125" s="16">
+      <c r="Q125">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -24174,7 +24293,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q126" s="16">
+      <c r="Q126">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24227,7 +24346,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q127" s="16">
+      <c r="Q127">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24280,7 +24399,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q128" s="16">
+      <c r="Q128">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -24336,7 +24455,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q129" s="16">
+      <c r="Q129">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24389,7 +24508,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q130" s="16">
+      <c r="Q130">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -24445,7 +24564,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>0</v>
       </c>
-      <c r="Q131" s="16">
+      <c r="Q131">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24498,7 +24617,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q132" s="16">
+      <c r="Q132">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24551,7 +24670,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q133" s="16">
+      <c r="Q133">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24607,7 +24726,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>0</v>
       </c>
-      <c r="Q134" s="16">
+      <c r="Q134">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24660,7 +24779,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q135" s="16">
+      <c r="Q135">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24713,7 +24832,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q136" s="16">
+      <c r="Q136">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24766,7 +24885,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q137" s="16">
+      <c r="Q137">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24822,7 +24941,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q138" s="16">
+      <c r="Q138">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24878,7 +24997,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q139" s="16">
+      <c r="Q139">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -24931,7 +25050,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q140" s="16">
+      <c r="Q140">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -24984,7 +25103,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q141" s="16">
+      <c r="Q141">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25037,7 +25156,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q142" s="16">
+      <c r="Q142">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25090,7 +25209,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q143" s="16">
+      <c r="Q143">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25143,7 +25262,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q144" s="16">
+      <c r="Q144">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25199,7 +25318,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>6</v>
       </c>
-      <c r="Q145" s="16">
+      <c r="Q145">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -25252,7 +25371,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q146" s="16">
+      <c r="Q146">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25305,7 +25424,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q147" s="16">
+      <c r="Q147">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25361,7 +25480,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q148" s="16">
+      <c r="Q148">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25417,7 +25536,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q149" s="16">
+      <c r="Q149">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25470,7 +25589,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q150" s="16">
+      <c r="Q150">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -25523,7 +25642,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q151" s="16">
+      <c r="Q151">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -25576,7 +25695,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q152" s="16">
+      <c r="Q152">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25632,7 +25751,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q153" s="16">
+      <c r="Q153">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25688,7 +25807,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q154" s="16">
+      <c r="Q154">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -25741,7 +25860,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q155" s="16">
+      <c r="Q155">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -25794,7 +25913,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q156" s="16">
+      <c r="Q156">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -25847,7 +25966,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q157" s="16">
+      <c r="Q157">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -25900,7 +26019,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q158" s="16">
+      <c r="Q158">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -25956,7 +26075,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q159" s="16">
+      <c r="Q159">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -26012,7 +26131,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q160" s="16">
+      <c r="Q160">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26065,7 +26184,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q161" s="16">
+      <c r="Q161">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -26118,7 +26237,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q162" s="16">
+      <c r="Q162">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -26174,7 +26293,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q163" s="16">
+      <c r="Q163">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -26227,7 +26346,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q164" s="16">
+      <c r="Q164">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26283,7 +26402,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>6</v>
       </c>
-      <c r="Q165" s="16">
+      <c r="Q165">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26336,7 +26455,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q166" s="16">
+      <c r="Q166">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -26389,7 +26508,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q167" s="16">
+      <c r="Q167">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -26442,7 +26561,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q168" s="16">
+      <c r="Q168">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -26495,7 +26614,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q169" s="16">
+      <c r="Q169">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26551,7 +26670,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>7</v>
       </c>
-      <c r="Q170" s="16">
+      <c r="Q170">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26604,7 +26723,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q171" s="16">
+      <c r="Q171">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -26657,7 +26776,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q172" s="16">
+      <c r="Q172">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26713,7 +26832,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q173" s="16">
+      <c r="Q173">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26766,7 +26885,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q174" s="16">
+      <c r="Q174">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26819,7 +26938,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q175" s="16">
+      <c r="Q175">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26875,7 +26994,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q176" s="16">
+      <c r="Q176">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -26931,7 +27050,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q177" s="16">
+      <c r="Q177">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -26984,7 +27103,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q178" s="16">
+      <c r="Q178">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27037,7 +27156,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q179" s="16">
+      <c r="Q179">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27093,7 +27212,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q180" s="16">
+      <c r="Q180">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27146,7 +27265,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q181" s="16">
+      <c r="Q181">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27199,7 +27318,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q182" s="16">
+      <c r="Q182">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27252,7 +27371,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q183" s="16">
+      <c r="Q183">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27305,7 +27424,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q184" s="16">
+      <c r="Q184">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27358,7 +27477,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q185" s="16">
+      <c r="Q185">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27411,7 +27530,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q186" s="16">
+      <c r="Q186">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -27467,7 +27586,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q187" s="16">
+      <c r="Q187">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27520,7 +27639,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q188" s="16">
+      <c r="Q188">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27573,7 +27692,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q189" s="16">
+      <c r="Q189">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -27629,7 +27748,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q190" s="16">
+      <c r="Q190">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -27682,7 +27801,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q191" s="16">
+      <c r="Q191">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -27735,7 +27854,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q192" s="16">
+      <c r="Q192">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -27788,7 +27907,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q193" s="16">
+      <c r="Q193">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27841,7 +27960,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q194" s="16">
+      <c r="Q194">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -27894,7 +28013,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q195" s="16">
+      <c r="Q195">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -27947,7 +28066,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q196" s="16">
+      <c r="Q196">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -28000,7 +28119,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q197" s="16">
+      <c r="Q197">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28053,7 +28172,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q198" s="16">
+      <c r="Q198">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28106,7 +28225,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>8</v>
       </c>
-      <c r="Q199" s="16">
+      <c r="Q199">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28162,7 +28281,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q200" s="16">
+      <c r="Q200">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28218,7 +28337,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q201" s="16">
+      <c r="Q201">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28271,7 +28390,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q202" s="16">
+      <c r="Q202">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28324,7 +28443,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q203" s="16">
+      <c r="Q203">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -28377,7 +28496,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q204" s="16">
+      <c r="Q204">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -28430,7 +28549,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q205" s="16">
+      <c r="Q205">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -28483,7 +28602,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q206" s="16">
+      <c r="Q206">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -28539,7 +28658,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q207" s="16">
+      <c r="Q207">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -28595,7 +28714,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q208" s="16">
+      <c r="Q208">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -28648,7 +28767,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q209" s="16">
+      <c r="Q209">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -28701,7 +28820,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q210" s="16">
+      <c r="Q210">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28754,7 +28873,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q211" s="16">
+      <c r="Q211">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28807,7 +28926,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q212" s="16">
+      <c r="Q212">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28863,7 +28982,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q213" s="16">
+      <c r="Q213">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -28919,7 +29038,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q214" s="16">
+      <c r="Q214">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -28975,7 +29094,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q215" s="16">
+      <c r="Q215">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -29031,7 +29150,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>6</v>
       </c>
-      <c r="Q216" s="16">
+      <c r="Q216">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -29087,7 +29206,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q217" s="16">
+      <c r="Q217">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29143,7 +29262,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q218" s="16">
+      <c r="Q218">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29199,7 +29318,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q219" s="16">
+      <c r="Q219">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29255,7 +29374,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q220" s="16">
+      <c r="Q220">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29308,7 +29427,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q221" s="16">
+      <c r="Q221">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29361,7 +29480,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q222" s="16">
+      <c r="Q222">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29417,7 +29536,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q223" s="16">
+      <c r="Q223">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -29470,7 +29589,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>18</v>
       </c>
-      <c r="Q224" s="16">
+      <c r="Q224">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -29523,7 +29642,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q225" s="16">
+      <c r="Q225">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29579,7 +29698,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>7</v>
       </c>
-      <c r="Q226" s="16">
+      <c r="Q226">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29632,7 +29751,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q227" s="16">
+      <c r="Q227">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -29688,7 +29807,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>0</v>
       </c>
-      <c r="Q228" s="16">
+      <c r="Q228">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29744,7 +29863,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q229" s="16">
+      <c r="Q229">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -29797,7 +29916,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q230" s="16">
+      <c r="Q230">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -29853,7 +29972,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>6</v>
       </c>
-      <c r="Q231" s="16">
+      <c r="Q231">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -29906,7 +30025,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q232" s="16">
+      <c r="Q232">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -29962,7 +30081,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q233" s="16">
+      <c r="Q233">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30015,7 +30134,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q234" s="16">
+      <c r="Q234">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -30071,7 +30190,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>0</v>
       </c>
-      <c r="Q235" s="16">
+      <c r="Q235">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -30127,7 +30246,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>0</v>
       </c>
-      <c r="Q236" s="16">
+      <c r="Q236">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30183,7 +30302,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q237" s="16">
+      <c r="Q237">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30239,7 +30358,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q238" s="16">
+      <c r="Q238">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -30292,7 +30411,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q239" s="16">
+      <c r="Q239">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30345,7 +30464,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q240" s="16">
+      <c r="Q240">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -30401,7 +30520,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q241" s="16">
+      <c r="Q241">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -30454,7 +30573,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>8</v>
       </c>
-      <c r="Q242" s="16">
+      <c r="Q242">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -30507,7 +30626,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q243" s="16">
+      <c r="Q243">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -30563,7 +30682,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>7</v>
       </c>
-      <c r="Q244" s="16">
+      <c r="Q244">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30616,7 +30735,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q245" s="16">
+      <c r="Q245">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30672,7 +30791,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q246" s="16">
+      <c r="Q246">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30725,7 +30844,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q247" s="16">
+      <c r="Q247">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -30778,7 +30897,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q248" s="16">
+      <c r="Q248">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -30834,7 +30953,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q249" s="16">
+      <c r="Q249">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30887,7 +31006,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>15</v>
       </c>
-      <c r="Q250" s="16">
+      <c r="Q250">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30943,7 +31062,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>0</v>
       </c>
-      <c r="Q251" s="16">
+      <c r="Q251">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -30996,7 +31115,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q252" s="16">
+      <c r="Q252">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31049,7 +31168,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q253" s="16">
+      <c r="Q253">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31102,7 +31221,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q254" s="16">
+      <c r="Q254">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31155,7 +31274,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q255" s="16">
+      <c r="Q255">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31208,7 +31327,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q256" s="16">
+      <c r="Q256">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -31261,7 +31380,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q257" s="16">
+      <c r="Q257">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31317,7 +31436,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q258" s="16">
+      <c r="Q258">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31370,7 +31489,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q259" s="16">
+      <c r="Q259">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -31423,7 +31542,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q260" s="16">
+      <c r="Q260">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -31479,7 +31598,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q261" s="16">
+      <c r="Q261">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31532,7 +31651,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q262" s="16">
+      <c r="Q262">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31585,7 +31704,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q263" s="16">
+      <c r="Q263">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31638,7 +31757,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>9</v>
       </c>
-      <c r="Q264" s="16">
+      <c r="Q264">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -31691,7 +31810,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q265" s="16">
+      <c r="Q265">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31744,7 +31863,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q266" s="16">
+      <c r="Q266">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31800,7 +31919,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q267" s="16">
+      <c r="Q267">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31853,7 +31972,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q268" s="16">
+      <c r="Q268">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -31906,7 +32025,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q269" s="16">
+      <c r="Q269">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -31959,7 +32078,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q270" s="16">
+      <c r="Q270">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -32012,7 +32131,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q271" s="16">
+      <c r="Q271">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -32065,7 +32184,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>15</v>
       </c>
-      <c r="Q272" s="16">
+      <c r="Q272">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32118,7 +32237,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>16</v>
       </c>
-      <c r="Q273" s="16">
+      <c r="Q273">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32171,7 +32290,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q274" s="16">
+      <c r="Q274">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -32224,7 +32343,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q275" s="16">
+      <c r="Q275">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32277,7 +32396,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q276" s="16">
+      <c r="Q276">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -32330,7 +32449,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>8</v>
       </c>
-      <c r="Q277" s="16">
+      <c r="Q277">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -32386,7 +32505,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q278" s="16">
+      <c r="Q278">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32442,7 +32561,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>6</v>
       </c>
-      <c r="Q279" s="16">
+      <c r="Q279">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32495,7 +32614,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q280" s="16">
+      <c r="Q280">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32551,7 +32670,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q281" s="16">
+      <c r="Q281">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32607,7 +32726,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q282" s="16">
+      <c r="Q282">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -32660,7 +32779,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>12</v>
       </c>
-      <c r="Q283" s="16">
+      <c r="Q283">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32713,7 +32832,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>19</v>
       </c>
-      <c r="Q284" s="16">
+      <c r="Q284">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -32766,7 +32885,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q285" s="16">
+      <c r="Q285">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32822,7 +32941,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q286" s="16">
+      <c r="Q286">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -32878,7 +32997,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>5</v>
       </c>
-      <c r="Q287" s="16">
+      <c r="Q287">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -32934,7 +33053,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q288" s="16">
+      <c r="Q288">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -32987,7 +33106,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q289" s="16">
+      <c r="Q289">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33040,7 +33159,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q290" s="16">
+      <c r="Q290">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -33096,7 +33215,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q291" s="16">
+      <c r="Q291">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33149,7 +33268,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>14</v>
       </c>
-      <c r="Q292" s="16">
+      <c r="Q292">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33202,7 +33321,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>13</v>
       </c>
-      <c r="Q293" s="16">
+      <c r="Q293">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33258,7 +33377,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>2</v>
       </c>
-      <c r="Q294" s="16">
+      <c r="Q294">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33314,7 +33433,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q295" s="16">
+      <c r="Q295">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -33367,7 +33486,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q296" s="16">
+      <c r="Q296">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -33420,7 +33539,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q297" s="16">
+      <c r="Q297">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33476,7 +33595,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>0</v>
       </c>
-      <c r="Q298" s="16">
+      <c r="Q298">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -33532,7 +33651,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q299" s="16">
+      <c r="Q299">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -33585,7 +33704,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>8</v>
       </c>
-      <c r="Q300" s="16">
+      <c r="Q300">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33638,7 +33757,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q301" s="16">
+      <c r="Q301">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -33694,7 +33813,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q302" s="16">
+      <c r="Q302">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33750,7 +33869,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>4</v>
       </c>
-      <c r="Q303" s="16">
+      <c r="Q303">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33806,7 +33925,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>1</v>
       </c>
-      <c r="Q304" s="16">
+      <c r="Q304">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -33862,7 +33981,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q305" s="16">
+      <c r="Q305">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -33918,7 +34037,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>3</v>
       </c>
-      <c r="Q306" s="16">
+      <c r="Q306">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -33971,7 +34090,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q307" s="16">
+      <c r="Q307">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -34024,7 +34143,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q308" s="16">
+      <c r="Q308">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>2</v>
       </c>
@@ -34080,7 +34199,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>7</v>
       </c>
-      <c r="Q309" s="16">
+      <c r="Q309">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -34133,7 +34252,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>15</v>
       </c>
-      <c r="Q310" s="16">
+      <c r="Q310">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -34186,7 +34305,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>10</v>
       </c>
-      <c r="Q311" s="16">
+      <c r="Q311">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -34239,7 +34358,7 @@
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
         <v>11</v>
       </c>
-      <c r="Q312" s="16">
+      <c r="Q312">
         <f>LEN(HRDataset_clean[[#This Row],[Sex]])</f>
         <v>1</v>
       </c>
@@ -34272,7 +34391,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -34680,7 +34799,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34740,7 +34859,7 @@
       <c r="B6" s="15">
         <v>69020.684887459807</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <f>MEDIAN(HRDataset_clean[Salary])</f>
         <v>62810</v>
       </c>

</xml_diff>

<commit_message>
Add salary analysis by department
1. Created a new sheet for salary analysis by department.
2. Built a PivotTable comparing average salary levels and the number of employees in different departments.
3. Added a bar chart to visualize the salary distribution between departments.
6. Wrote insights summarizing key findings:
- The company has a classic structure: high salaries in IT areas, low salaries in production, which makes up the majority of employees.
- The Executive Office cannot be analyzed through one person - this is an exception.
- A large number of employees from Production underestimates the total average salary of the company.
</commit_message>
<xml_diff>
--- a/HRDataset_analysis.xlsx
+++ b/HRDataset_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8beb163ab15076dd/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="844" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36E6A1DF-CC96-459B-85CF-CFD714E4DFBA}"/>
+  <xr:revisionPtr revIDLastSave="1024" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F439DACB-0EF1-4753-94C5-BE8113AEDF13}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="5" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="6" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
   </bookViews>
   <sheets>
     <sheet name="HRDataset_raw" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="Turnover_by_gender" sheetId="6" r:id="rId4"/>
     <sheet name="Turnover_by_experience" sheetId="7" r:id="rId5"/>
     <sheet name="Salary_by_gender" sheetId="8" r:id="rId6"/>
+    <sheet name="Salary_by_department" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">HRDataset_clean!$A$1:$N$312</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2870" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="739">
   <si>
     <t>Employee_Name,EmpID,MarriedID,MaritalStatusID,GenderID,EmpStatusID,DeptID,PerfScoreID,FromDiversityJobFairID,Salary,Termd,PositionID,Position,State,Zip,DOB,Sex,MaritalDesc,CitizenDesc,HispanicLatino,RaceDesc,DateofHire,DateofTermination,TermReason,EmploymentStatus,Department,ManagerName,ManagerID,RecruitmentSource,PerformanceScore,EngagementSurvey,EmpSatisfaction,SpecialProjectsCount,LastPerformanceReview_Date,DaysLateLast30,Absences</t>
   </si>
@@ -2285,6 +2286,12 @@
   </si>
   <si>
     <t>Is the average salary different for men and women?</t>
+  </si>
+  <si>
+    <t>Кількість з Position</t>
+  </si>
+  <si>
+    <t>Which departments have the highest and lowest salaries?</t>
   </si>
 </sst>
 </file>
@@ -2840,7 +2847,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2864,6 +2871,7 @@
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="16" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% – колірна тема 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5981,6 +5989,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2134147343"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -6036,6 +6045,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="19026335"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -6122,6 +6132,871 @@
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="uk-UA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[HRDataset_analysis.xlsx]Salary_by_department!Зведена таблиця1</c:name>
+    <c:fmtId val="3"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Average salary by departments</a:t>
+            </a:r>
+            <a:endParaRPr lang="uk-UA" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24800678040244969"/>
+          <c:y val="2.3148148148148147E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="uk-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="110000"/>
+                  <a:satMod val="105000"/>
+                  <a:tint val="67000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="105000"/>
+                  <a:satMod val="103000"/>
+                  <a:tint val="73000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="105000"/>
+                  <a:satMod val="109000"/>
+                  <a:tint val="81000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="4"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="uk-UA"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="110000"/>
+                  <a:satMod val="105000"/>
+                  <a:tint val="67000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="105000"/>
+                  <a:satMod val="103000"/>
+                  <a:tint val="73000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="105000"/>
+                  <a:satMod val="109000"/>
+                  <a:tint val="81000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="4"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="uk-UA"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Salary_by_department!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Середнє з Salary</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="uk-UA"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Salary_by_department!$A$4:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Executive Office</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>IT/IS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Software Engineering</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Admin Offices</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sales</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Production</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Salary_by_department!$B$4:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97064.639999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94989.454545454544</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71791.888888888891</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69061.258064516136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59953.545454545456</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-072A-4E17-A90B-684B271A0D8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Salary_by_department!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Кількість з Position</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="uk-UA"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Salary_by_department!$A$4:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Executive Office</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>IT/IS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Software Engineering</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Admin Offices</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sales</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Production</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Salary_by_department!$C$4:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>209</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-072A-4E17-A90B-684B271A0D8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="791425119"/>
+        <c:axId val="791419839"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="791425119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="791419839"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="791419839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="791425119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="uk-UA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
       </c14:pivotOptions>
     </c:ext>
     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
@@ -6254,6 +7129,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8247,6 +9162,531 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="206">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -9113,6 +10553,228 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>415925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>155574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>111125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Діаграма 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE1BD3D-8539-7A3A-69CD-82F7FF2CF962}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED7F8CDC-FFC9-A914-B0F8-B04650E91116}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8851900" y="412750"/>
+          <a:ext cx="4311650" cy="4819650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>►</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Conclusions from the table</a:t>
+          </a:r>
+          <a:endParaRPr lang="uk-UA" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="uk-UA" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>The highest salary by a large margin from other departments is in the Executive Office (250 K)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
+            <a:t> but it consists only of 1 person.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" u="sng"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>IT/IS and Software Engineering </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>have high average salaries (97-95 K). We can say that technical roles are one of the highest-paid areas in the company.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Admin Offices and Sales </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>earn salaries close to average (72-69 K). Thus, the sales department is at the average salary level in the company.This could mean: either a low base salary and bonuses, or that bonuses are included in salary</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>the pay structure is more steady.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>The lowest average salaries are in the Production department - 60 K. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none"/>
+            <a:t>Production makes up the majority of the company: 209  of 311 employees (67%).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The total average salary for all departments is 69 K.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>3 main business conclusions:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> The </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>company has a classic structure: high salaries in IT areas, low salaries in production, which makes up the majority of employees.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. The Executive Office cannot be analyzed through one person - this is an exception.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. The total average salary of the company is underestimated by a large number of employees from Production.</a:t>
+          </a:r>
+          <a:endParaRPr lang="uk-UA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -9136,7 +10798,39 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="45046" maxValue="250000"/>
     </cacheField>
     <cacheField name="Position" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="31">
+        <s v="Production Technician I"/>
+        <s v="Sr. DBA"/>
+        <s v="Production Technician II"/>
+        <s v="Software Engineer"/>
+        <s v="IT Support"/>
+        <s v="Data Analyst"/>
+        <s v="Database Administrator"/>
+        <s v="Enterprise Architect"/>
+        <s v="Sr. Accountant"/>
+        <s v="Production Manager"/>
+        <s v="Accountant I"/>
+        <s v="Area Sales Manager"/>
+        <s v="Software Engineering Manager"/>
+        <s v="BI Director"/>
+        <s v="Director of Operations"/>
+        <s v="Sr. Network Engineer"/>
+        <s v="Sales Manager"/>
+        <s v="BI Developer"/>
+        <s v="IT Manager - Support"/>
+        <s v="Network Engineer"/>
+        <s v="IT Director"/>
+        <s v="Director of Sales"/>
+        <s v="Administrative Assistant"/>
+        <s v="President &amp; CEO"/>
+        <s v="Senior BI Developer"/>
+        <s v="Shared Services Manager"/>
+        <s v="IT Manager - Infra"/>
+        <s v="Principal Data Architect"/>
+        <s v="Data Architect"/>
+        <s v="IT Manager - DB"/>
+        <s v="CIO"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="DOB" numFmtId="14">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1951-01-02T00:00:00" maxDate="1992-08-18T00:00:00"/>
@@ -9201,7 +10895,7 @@
     <n v="10026"/>
     <n v="1"/>
     <n v="62506"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-07-10T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9219,7 +10913,7 @@
     <n v="10084"/>
     <n v="1"/>
     <n v="104437"/>
-    <s v="Sr. DBA"/>
+    <x v="1"/>
     <d v="1975-05-05T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9237,7 +10931,7 @@
     <n v="10196"/>
     <n v="0"/>
     <n v="64955"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1988-09-19T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9255,7 +10949,7 @@
     <n v="10088"/>
     <n v="0"/>
     <n v="64991"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1988-09-27T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9273,7 +10967,7 @@
     <n v="10069"/>
     <n v="0"/>
     <n v="50825"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1989-09-08T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9291,7 +10985,7 @@
     <n v="10002"/>
     <n v="0"/>
     <n v="57568"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1977-05-22T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9309,7 +11003,7 @@
     <n v="10194"/>
     <n v="0"/>
     <n v="95660"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1979-05-24T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9327,7 +11021,7 @@
     <n v="10062"/>
     <n v="1"/>
     <n v="59365"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-02-18T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9345,7 +11039,7 @@
     <n v="10114"/>
     <n v="0"/>
     <n v="47837"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1970-02-11T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9363,7 +11057,7 @@
     <n v="10250"/>
     <n v="1"/>
     <n v="50178"/>
-    <s v="IT Support"/>
+    <x v="4"/>
     <d v="1988-01-07T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9381,7 +11075,7 @@
     <n v="10252"/>
     <n v="0"/>
     <n v="54670"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-01-12T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9399,7 +11093,7 @@
     <n v="10242"/>
     <n v="1"/>
     <n v="47211"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-02-21T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9417,7 +11111,7 @@
     <n v="10012"/>
     <n v="1"/>
     <n v="92328"/>
-    <s v="Data Analyst"/>
+    <x v="5"/>
     <d v="1988-07-04T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9435,7 +11129,7 @@
     <n v="10265"/>
     <n v="1"/>
     <n v="58709"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-07-20T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9453,7 +11147,7 @@
     <n v="10066"/>
     <n v="1"/>
     <n v="52505"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1977-07-15T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9471,7 +11165,7 @@
     <n v="10061"/>
     <n v="1"/>
     <n v="57834"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1981-10-18T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9489,7 +11183,7 @@
     <n v="10023"/>
     <n v="0"/>
     <n v="70131"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1966-04-17T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9507,7 +11201,7 @@
     <n v="10055"/>
     <n v="0"/>
     <n v="59026"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1970-10-27T00:00:00"/>
     <x v="1"/>
     <s v="Eligible NonCitizen"/>
@@ -9525,7 +11219,7 @@
     <n v="10245"/>
     <n v="0"/>
     <n v="110000"/>
-    <s v="Database Administrator"/>
+    <x v="6"/>
     <d v="1986-04-04T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9543,7 +11237,7 @@
     <n v="10277"/>
     <n v="1"/>
     <n v="53250"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1979-04-06T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9561,7 +11255,7 @@
     <n v="10046"/>
     <n v="1"/>
     <n v="51044"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1970-12-22T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9579,7 +11273,7 @@
     <n v="10226"/>
     <n v="0"/>
     <n v="64919"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1958-12-27T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9597,7 +11291,7 @@
     <n v="10003"/>
     <n v="0"/>
     <n v="62910"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1989-09-01T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9615,7 +11309,7 @@
     <n v="10294"/>
     <n v="0"/>
     <n v="66441"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1990-09-21T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9633,7 +11327,7 @@
     <n v="10267"/>
     <n v="0"/>
     <n v="57815"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1967-01-16T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9651,7 +11345,7 @@
     <n v="10199"/>
     <n v="1"/>
     <n v="103613"/>
-    <s v="Enterprise Architect"/>
+    <x v="7"/>
     <d v="1964-07-30T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9669,7 +11363,7 @@
     <n v="10081"/>
     <n v="0"/>
     <n v="106367"/>
-    <s v="Sr. Accountant"/>
+    <x v="8"/>
     <d v="1987-04-04T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9687,7 +11381,7 @@
     <n v="10175"/>
     <n v="1"/>
     <n v="74312"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1970-03-10T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9705,7 +11399,7 @@
     <n v="10177"/>
     <n v="0"/>
     <n v="53492"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1990-08-24T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9723,7 +11417,7 @@
     <n v="10238"/>
     <n v="0"/>
     <n v="63000"/>
-    <s v="Accountant I"/>
+    <x v="10"/>
     <d v="1987-11-24T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9741,7 +11435,7 @@
     <n v="10184"/>
     <n v="1"/>
     <n v="65288"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1983-07-28T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9759,7 +11453,7 @@
     <n v="10203"/>
     <n v="0"/>
     <n v="64375"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1969-10-30T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9777,7 +11471,7 @@
     <n v="10188"/>
     <n v="0"/>
     <n v="74326"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1964-06-01T00:00:00"/>
     <x v="1"/>
     <s v="Eligible NonCitizen"/>
@@ -9795,7 +11489,7 @@
     <n v="10107"/>
     <n v="0"/>
     <n v="63763"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1980-03-02T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9813,7 +11507,7 @@
     <n v="10181"/>
     <n v="1"/>
     <n v="62162"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1977-08-19T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9831,7 +11525,7 @@
     <n v="10150"/>
     <n v="1"/>
     <n v="77692"/>
-    <s v="Software Engineering Manager"/>
+    <x v="12"/>
     <d v="1966-11-22T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9849,7 +11543,7 @@
     <n v="10001"/>
     <n v="1"/>
     <n v="72640"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1983-08-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9867,7 +11561,7 @@
     <n v="10085"/>
     <n v="0"/>
     <n v="93396"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1987-04-05T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9885,7 +11579,7 @@
     <n v="10115"/>
     <n v="1"/>
     <n v="52846"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-02-02T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9903,7 +11597,7 @@
     <n v="10082"/>
     <n v="0"/>
     <n v="100031"/>
-    <s v="Sr. DBA"/>
+    <x v="1"/>
     <d v="1986-06-06T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9921,7 +11615,7 @@
     <n v="10040"/>
     <n v="0"/>
     <n v="71860"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1963-05-15T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9939,7 +11633,7 @@
     <n v="10067"/>
     <n v="0"/>
     <n v="61656"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1951-01-02T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9957,7 +11651,7 @@
     <n v="10108"/>
     <n v="1"/>
     <n v="110929"/>
-    <s v="BI Director"/>
+    <x v="13"/>
     <d v="1972-02-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -9975,7 +11669,7 @@
     <n v="10210"/>
     <n v="0"/>
     <n v="54237"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1979-02-12T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -9993,7 +11687,7 @@
     <n v="10154"/>
     <n v="1"/>
     <n v="60380"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-08-24T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10011,7 +11705,7 @@
     <n v="10200"/>
     <n v="1"/>
     <n v="66808"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1970-06-11T00:00:00"/>
     <x v="0"/>
     <s v="Eligible NonCitizen"/>
@@ -10029,7 +11723,7 @@
     <n v="10240"/>
     <n v="0"/>
     <n v="64786"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-08-27T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10047,7 +11741,7 @@
     <n v="10168"/>
     <n v="0"/>
     <n v="64816"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1988-05-31T00:00:00"/>
     <x v="1"/>
     <s v="Non-Citizen"/>
@@ -10065,7 +11759,7 @@
     <n v="10220"/>
     <n v="1"/>
     <n v="68678"/>
-    <s v="IT Support"/>
+    <x v="4"/>
     <d v="1985-09-05T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10083,7 +11777,7 @@
     <n v="10275"/>
     <n v="0"/>
     <n v="64066"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1981-08-31T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10101,7 +11795,7 @@
     <n v="10269"/>
     <n v="1"/>
     <n v="59369"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1978-11-25T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10119,7 +11813,7 @@
     <n v="10029"/>
     <n v="1"/>
     <n v="50373"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1980-08-26T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10137,7 +11831,7 @@
     <n v="10261"/>
     <n v="1"/>
     <n v="63108"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1977-09-08T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10155,7 +11849,7 @@
     <n v="10292"/>
     <n v="1"/>
     <n v="59144"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1979-08-12T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10173,7 +11867,7 @@
     <n v="10282"/>
     <n v="1"/>
     <n v="68051"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1975-12-17T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10191,7 +11885,7 @@
     <n v="10019"/>
     <n v="1"/>
     <n v="170500"/>
-    <s v="Director of Operations"/>
+    <x v="14"/>
     <d v="1983-03-19T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10209,7 +11903,7 @@
     <n v="10094"/>
     <n v="0"/>
     <n v="63381"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1977-03-31T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10227,7 +11921,7 @@
     <n v="10193"/>
     <n v="1"/>
     <n v="83552"/>
-    <s v="Data Analyst"/>
+    <x v="5"/>
     <d v="1986-08-26T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10245,7 +11939,7 @@
     <n v="10132"/>
     <n v="0"/>
     <n v="56149"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1987-04-10T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10263,7 +11957,7 @@
     <n v="10083"/>
     <n v="1"/>
     <n v="92329"/>
-    <s v="Sr. Network Engineer"/>
+    <x v="15"/>
     <d v="1965-09-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10281,7 +11975,7 @@
     <n v="10099"/>
     <n v="0"/>
     <n v="65729"/>
-    <s v="Sales Manager"/>
+    <x v="16"/>
     <d v="1990-04-19T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10299,7 +11993,7 @@
     <n v="10212"/>
     <n v="0"/>
     <n v="85028"/>
-    <s v="Sr. Network Engineer"/>
+    <x v="15"/>
     <d v="1952-01-18T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10317,7 +12011,7 @@
     <n v="10056"/>
     <n v="0"/>
     <n v="57583"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1978-11-05T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10335,7 +12029,7 @@
     <n v="10143"/>
     <n v="1"/>
     <n v="56294"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1979-09-14T00:00:00"/>
     <x v="0"/>
     <s v="Eligible NonCitizen"/>
@@ -10353,7 +12047,7 @@
     <n v="10311"/>
     <n v="1"/>
     <n v="56991"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1988-04-15T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10371,7 +12065,7 @@
     <n v="10070"/>
     <n v="1"/>
     <n v="55722"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1977-10-31T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10389,7 +12083,7 @@
     <n v="10155"/>
     <n v="0"/>
     <n v="101199"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1979-07-05T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10407,7 +12101,7 @@
     <n v="10306"/>
     <n v="1"/>
     <n v="61568"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1975-11-02T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10425,7 +12119,7 @@
     <n v="10100"/>
     <n v="0"/>
     <n v="58275"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1951-02-25T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10443,7 +12137,7 @@
     <n v="10310"/>
     <n v="1"/>
     <n v="53189"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1967-04-19T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10461,7 +12155,7 @@
     <n v="10197"/>
     <n v="1"/>
     <n v="96820"/>
-    <s v="BI Developer"/>
+    <x v="17"/>
     <d v="1983-09-04T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10479,7 +12173,7 @@
     <n v="10276"/>
     <n v="1"/>
     <n v="51259"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1982-11-15T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10497,7 +12191,7 @@
     <n v="10304"/>
     <n v="0"/>
     <n v="59231"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1987-05-14T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10515,7 +12209,7 @@
     <n v="10284"/>
     <n v="0"/>
     <n v="61584"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1978-12-02T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10533,7 +12227,7 @@
     <n v="10207"/>
     <n v="0"/>
     <n v="46335"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1986-10-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10551,7 +12245,7 @@
     <n v="10133"/>
     <n v="0"/>
     <n v="70621"/>
-    <s v="IT Support"/>
+    <x v="4"/>
     <d v="1988-07-18T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10569,7 +12263,7 @@
     <n v="10028"/>
     <n v="1"/>
     <n v="138888"/>
-    <s v="IT Manager - Support"/>
+    <x v="18"/>
     <d v="1970-07-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10587,7 +12281,7 @@
     <n v="10006"/>
     <n v="0"/>
     <n v="74241"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1988-11-08T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10605,7 +12299,7 @@
     <n v="10105"/>
     <n v="0"/>
     <n v="75188"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1973-11-28T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10623,7 +12317,7 @@
     <n v="10211"/>
     <n v="0"/>
     <n v="62514"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1973-09-23T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10641,7 +12335,7 @@
     <n v="10064"/>
     <n v="0"/>
     <n v="60070"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1991-09-05T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10659,7 +12353,7 @@
     <n v="10247"/>
     <n v="1"/>
     <n v="48888"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-05-31T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10677,7 +12371,7 @@
     <n v="10235"/>
     <n v="1"/>
     <n v="54285"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1978-08-25T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10695,7 +12389,7 @@
     <n v="10299"/>
     <n v="0"/>
     <n v="56847"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1989-08-25T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10713,7 +12407,7 @@
     <n v="10280"/>
     <n v="1"/>
     <n v="60340"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-09-02T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10731,7 +12425,7 @@
     <n v="10296"/>
     <n v="0"/>
     <n v="59124"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1989-05-06T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10749,7 +12443,7 @@
     <n v="10290"/>
     <n v="0"/>
     <n v="99280"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1987-05-15T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10767,7 +12461,7 @@
     <n v="10263"/>
     <n v="0"/>
     <n v="71776"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1978-09-22T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10785,7 +12479,7 @@
     <n v="10136"/>
     <n v="0"/>
     <n v="65902"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1987-09-27T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10803,7 +12497,7 @@
     <n v="10189"/>
     <n v="0"/>
     <n v="57748"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1955-04-14T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10821,7 +12515,7 @@
     <n v="10308"/>
     <n v="1"/>
     <n v="64057"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1989-10-18T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10839,7 +12533,7 @@
     <n v="10309"/>
     <n v="1"/>
     <n v="53366"/>
-    <s v="Network Engineer"/>
+    <x v="19"/>
     <d v="1987-06-18T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10857,7 +12551,7 @@
     <n v="10049"/>
     <n v="0"/>
     <n v="58530"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1981-03-16T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10875,7 +12569,7 @@
     <n v="10093"/>
     <n v="1"/>
     <n v="72609"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1981-10-01T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10893,7 +12587,7 @@
     <n v="10163"/>
     <n v="0"/>
     <n v="55965"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1983-11-08T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10911,7 +12605,7 @@
     <n v="10305"/>
     <n v="1"/>
     <n v="70187"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1975-07-07T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10929,7 +12623,7 @@
     <n v="10015"/>
     <n v="1"/>
     <n v="178000"/>
-    <s v="IT Director"/>
+    <x v="20"/>
     <d v="1980-07-05T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10947,7 +12641,7 @@
     <n v="10080"/>
     <n v="0"/>
     <n v="99351"/>
-    <s v="Sr. Accountant"/>
+    <x v="8"/>
     <d v="1979-04-16T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -10965,7 +12659,7 @@
     <n v="10258"/>
     <n v="1"/>
     <n v="67251"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1963-08-28T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -10983,7 +12677,7 @@
     <n v="10273"/>
     <n v="0"/>
     <n v="65707"/>
-    <s v="IT Support"/>
+    <x v="4"/>
     <d v="1968-07-06T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11001,7 +12695,7 @@
     <n v="10111"/>
     <n v="1"/>
     <n v="52249"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1985-09-15T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11019,7 +12713,7 @@
     <n v="10257"/>
     <n v="0"/>
     <n v="53171"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-12-02T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11037,7 +12731,7 @@
     <n v="10159"/>
     <n v="0"/>
     <n v="51337"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1990-10-01T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11055,7 +12749,7 @@
     <n v="10122"/>
     <n v="0"/>
     <n v="51505"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1970-05-15T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11073,7 +12767,7 @@
     <n v="10142"/>
     <n v="0"/>
     <n v="59370"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1971-07-10T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11091,7 +12785,7 @@
     <n v="10283"/>
     <n v="1"/>
     <n v="54933"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-08-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11109,7 +12803,7 @@
     <n v="10018"/>
     <n v="0"/>
     <n v="57815"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1980-05-08T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11127,7 +12821,7 @@
     <n v="10255"/>
     <n v="0"/>
     <n v="61555"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1989-09-22T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11145,7 +12839,7 @@
     <n v="10246"/>
     <n v="0"/>
     <n v="114800"/>
-    <s v="Database Administrator"/>
+    <x v="6"/>
     <d v="1971-10-23T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11163,7 +12857,7 @@
     <n v="10228"/>
     <n v="1"/>
     <n v="74679"/>
-    <s v="IT Support"/>
+    <x v="4"/>
     <d v="1989-11-24T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11181,7 +12875,7 @@
     <n v="10243"/>
     <n v="0"/>
     <n v="53018"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1992-06-18T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11199,7 +12893,7 @@
     <n v="10031"/>
     <n v="1"/>
     <n v="59892"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1969-09-29T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11217,7 +12911,7 @@
     <n v="10300"/>
     <n v="1"/>
     <n v="68898"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1964-10-12T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11235,7 +12929,7 @@
     <n v="10101"/>
     <n v="0"/>
     <n v="61242"/>
-    <s v="IT Support"/>
+    <x v="4"/>
     <d v="1981-04-16T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11253,7 +12947,7 @@
     <n v="10237"/>
     <n v="0"/>
     <n v="66825"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1986-05-25T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11271,7 +12965,7 @@
     <n v="10051"/>
     <n v="1"/>
     <n v="48285"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1979-05-21T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11289,7 +12983,7 @@
     <n v="10218"/>
     <n v="0"/>
     <n v="66149"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1983-12-08T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11307,7 +13001,7 @@
     <n v="10256"/>
     <n v="0"/>
     <n v="49256"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-10-09T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11325,7 +13019,7 @@
     <n v="10098"/>
     <n v="1"/>
     <n v="62957"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1981-07-11T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11343,7 +13037,7 @@
     <n v="10059"/>
     <n v="0"/>
     <n v="63813"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-05-21T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11361,7 +13055,7 @@
     <n v="10234"/>
     <n v="1"/>
     <n v="99020"/>
-    <s v="BI Developer"/>
+    <x v="17"/>
     <d v="1989-06-30T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11379,7 +13073,7 @@
     <n v="10109"/>
     <n v="1"/>
     <n v="71707"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1969-02-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11397,7 +13091,7 @@
     <n v="10125"/>
     <n v="0"/>
     <n v="54828"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1977-03-23T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11415,7 +13109,7 @@
     <n v="10074"/>
     <n v="1"/>
     <n v="64246"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1988-08-10T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11433,7 +13127,7 @@
     <n v="10097"/>
     <n v="0"/>
     <n v="52177"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1952-08-18T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11451,7 +13145,7 @@
     <n v="10007"/>
     <n v="0"/>
     <n v="62065"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-05-02T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11469,7 +13163,7 @@
     <n v="10129"/>
     <n v="1"/>
     <n v="46998"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1984-01-04T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11487,7 +13181,7 @@
     <n v="10075"/>
     <n v="0"/>
     <n v="68099"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1972-08-27T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11505,7 +13199,7 @@
     <n v="10167"/>
     <n v="1"/>
     <n v="70545"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1988-09-14T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11523,7 +13217,7 @@
     <n v="10195"/>
     <n v="0"/>
     <n v="63478"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1984-02-16T00:00:00"/>
     <x v="1"/>
     <s v="Non-Citizen"/>
@@ -11541,7 +13235,7 @@
     <n v="10112"/>
     <n v="0"/>
     <n v="97999"/>
-    <s v="Database Administrator"/>
+    <x v="6"/>
     <d v="1984-02-21T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11559,7 +13253,7 @@
     <n v="10272"/>
     <n v="0"/>
     <n v="180000"/>
-    <s v="Director of Sales"/>
+    <x v="21"/>
     <d v="1966-03-17T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11577,7 +13271,7 @@
     <n v="10182"/>
     <n v="0"/>
     <n v="49920"/>
-    <s v="Administrative Assistant"/>
+    <x v="22"/>
     <d v="1985-09-16T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11595,7 +13289,7 @@
     <n v="10248"/>
     <n v="0"/>
     <n v="55425"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1986-06-10T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11613,7 +13307,7 @@
     <n v="10201"/>
     <n v="0"/>
     <n v="69340"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1984-03-11T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11631,7 +13325,7 @@
     <n v="10214"/>
     <n v="0"/>
     <n v="64995"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1992-05-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11649,7 +13343,7 @@
     <n v="10160"/>
     <n v="0"/>
     <n v="68182"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1976-09-22T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11667,7 +13361,7 @@
     <n v="10289"/>
     <n v="1"/>
     <n v="83082"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1976-11-15T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11685,7 +13379,7 @@
     <n v="10139"/>
     <n v="0"/>
     <n v="51908"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1991-01-28T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11703,7 +13397,7 @@
     <n v="10227"/>
     <n v="0"/>
     <n v="61242"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1972-09-11T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11721,7 +13415,7 @@
     <n v="10236"/>
     <n v="0"/>
     <n v="45069"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1966-03-22T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11739,7 +13433,7 @@
     <n v="10009"/>
     <n v="0"/>
     <n v="60724"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1986-11-06T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11757,7 +13451,7 @@
     <n v="10060"/>
     <n v="0"/>
     <n v="60436"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1964-04-13T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11775,7 +13469,7 @@
     <n v="10034"/>
     <n v="1"/>
     <n v="46837"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1959-08-19T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11793,7 +13487,7 @@
     <n v="10156"/>
     <n v="0"/>
     <n v="105700"/>
-    <s v="Database Administrator"/>
+    <x v="6"/>
     <d v="1986-11-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11811,7 +13505,7 @@
     <n v="10036"/>
     <n v="0"/>
     <n v="63322"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1969-09-08T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11829,7 +13523,7 @@
     <n v="10138"/>
     <n v="0"/>
     <n v="61154"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1986-04-17T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11847,7 +13541,7 @@
     <n v="10244"/>
     <n v="0"/>
     <n v="68999"/>
-    <s v="Sales Manager"/>
+    <x v="16"/>
     <d v="1989-11-11T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11865,7 +13559,7 @@
     <n v="10192"/>
     <n v="1"/>
     <n v="50482"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1976-01-19T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11883,7 +13577,7 @@
     <n v="10231"/>
     <n v="1"/>
     <n v="65310"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1979-11-27T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11901,7 +13595,7 @@
     <n v="10089"/>
     <n v="0"/>
     <n v="250000"/>
-    <s v="President &amp; CEO"/>
+    <x v="23"/>
     <d v="1954-09-21T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11919,7 +13613,7 @@
     <n v="10166"/>
     <n v="0"/>
     <n v="54005"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1973-12-08T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11937,7 +13631,7 @@
     <n v="10170"/>
     <n v="0"/>
     <n v="45433"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1970-10-08T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -11955,7 +13649,7 @@
     <n v="10208"/>
     <n v="1"/>
     <n v="46654"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1977-11-10T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11973,7 +13667,7 @@
     <n v="10176"/>
     <n v="1"/>
     <n v="63973"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1980-02-02T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -11991,7 +13685,7 @@
     <n v="10165"/>
     <n v="1"/>
     <n v="71339"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1969-02-24T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12009,7 +13703,7 @@
     <n v="10113"/>
     <n v="1"/>
     <n v="93206"/>
-    <s v="Sr. Network Engineer"/>
+    <x v="15"/>
     <d v="1986-04-23T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12027,7 +13721,7 @@
     <n v="10092"/>
     <n v="1"/>
     <n v="82758"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1972-07-01T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12045,7 +13739,7 @@
     <n v="10106"/>
     <n v="0"/>
     <n v="66074"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1979-07-25T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12063,7 +13757,7 @@
     <n v="10052"/>
     <n v="1"/>
     <n v="46120"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1986-12-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12081,7 +13775,7 @@
     <n v="10038"/>
     <n v="1"/>
     <n v="64520"/>
-    <s v="Accountant I"/>
+    <x v="10"/>
     <d v="1984-04-26T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12099,7 +13793,7 @@
     <n v="10249"/>
     <n v="1"/>
     <n v="61962"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1984-05-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12117,7 +13811,7 @@
     <n v="10232"/>
     <n v="0"/>
     <n v="81584"/>
-    <s v="Senior BI Developer"/>
+    <x v="24"/>
     <d v="1987-06-14T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12135,7 +13829,7 @@
     <n v="10087"/>
     <n v="0"/>
     <n v="63676"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1979-01-17T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12153,7 +13847,7 @@
     <n v="10134"/>
     <n v="1"/>
     <n v="93046"/>
-    <s v="Shared Services Manager"/>
+    <x v="25"/>
     <d v="1984-06-10T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12171,7 +13865,7 @@
     <n v="10251"/>
     <n v="1"/>
     <n v="64738"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1982-09-02T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12189,7 +13883,7 @@
     <n v="10103"/>
     <n v="1"/>
     <n v="70468"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1988-12-27T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12207,7 +13901,7 @@
     <n v="10017"/>
     <n v="0"/>
     <n v="77915"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1981-10-26T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12225,7 +13919,7 @@
     <n v="10186"/>
     <n v="0"/>
     <n v="52624"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1981-03-26T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12243,7 +13937,7 @@
     <n v="10137"/>
     <n v="1"/>
     <n v="63450"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1979-03-19T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12261,7 +13955,7 @@
     <n v="10008"/>
     <n v="0"/>
     <n v="51777"/>
-    <s v="IT Support"/>
+    <x v="4"/>
     <d v="1988-10-05T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12279,7 +13973,7 @@
     <n v="10096"/>
     <n v="0"/>
     <n v="67237"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1976-12-26T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12297,7 +13991,7 @@
     <n v="10035"/>
     <n v="0"/>
     <n v="73330"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1982-03-28T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12315,7 +14009,7 @@
     <n v="10057"/>
     <n v="0"/>
     <n v="52057"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1975-10-22T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12333,7 +14027,7 @@
     <n v="10004"/>
     <n v="0"/>
     <n v="47434"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1973-02-14T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12351,7 +14045,7 @@
     <n v="10191"/>
     <n v="1"/>
     <n v="52788"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1972-11-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12369,7 +14063,7 @@
     <n v="10219"/>
     <n v="0"/>
     <n v="45395"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1986-07-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12387,7 +14081,7 @@
     <n v="10077"/>
     <n v="0"/>
     <n v="62385"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1976-08-25T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12405,7 +14099,7 @@
     <n v="10073"/>
     <n v="0"/>
     <n v="68407"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1986-12-10T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12423,7 +14117,7 @@
     <n v="10279"/>
     <n v="0"/>
     <n v="61349"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-11-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12441,7 +14135,7 @@
     <n v="10110"/>
     <n v="0"/>
     <n v="105688"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1987-11-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12459,7 +14153,7 @@
     <n v="10053"/>
     <n v="0"/>
     <n v="54132"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1977-11-22T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12477,7 +14171,7 @@
     <n v="10076"/>
     <n v="0"/>
     <n v="55315"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1987-05-21T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12495,7 +14189,7 @@
     <n v="10145"/>
     <n v="0"/>
     <n v="62810"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1987-01-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12513,7 +14207,7 @@
     <n v="10202"/>
     <n v="1"/>
     <n v="63291"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1984-07-01T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12531,7 +14225,7 @@
     <n v="10128"/>
     <n v="0"/>
     <n v="62659"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1968-05-30T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12549,7 +14243,7 @@
     <n v="10068"/>
     <n v="0"/>
     <n v="55688"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1976-09-22T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12567,7 +14261,7 @@
     <n v="10116"/>
     <n v="1"/>
     <n v="83667"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1981-08-10T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12585,7 +14279,7 @@
     <n v="10298"/>
     <n v="1"/>
     <n v="55800"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1985-06-29T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12603,7 +14297,7 @@
     <n v="10213"/>
     <n v="1"/>
     <n v="58207"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1992-08-17T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12621,7 +14315,7 @@
     <n v="10288"/>
     <n v="1"/>
     <n v="157000"/>
-    <s v="IT Manager - Infra"/>
+    <x v="26"/>
     <d v="1986-10-05T00:00:00"/>
     <x v="0"/>
     <s v="Eligible NonCitizen"/>
@@ -12639,7 +14333,7 @@
     <n v="10025"/>
     <n v="0"/>
     <n v="72460"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1970-04-24T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12657,7 +14351,7 @@
     <n v="10223"/>
     <n v="1"/>
     <n v="72106"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1976-12-03T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12675,7 +14369,7 @@
     <n v="10151"/>
     <n v="0"/>
     <n v="52599"/>
-    <s v="Network Engineer"/>
+    <x v="19"/>
     <d v="1979-04-04T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12693,7 +14387,7 @@
     <n v="10254"/>
     <n v="0"/>
     <n v="63430"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1984-07-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12711,7 +14405,7 @@
     <n v="10120"/>
     <n v="1"/>
     <n v="74417"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1974-12-01T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12729,7 +14423,7 @@
     <n v="10216"/>
     <n v="1"/>
     <n v="57575"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1980-04-18T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12747,7 +14441,7 @@
     <n v="10079"/>
     <n v="1"/>
     <n v="87921"/>
-    <s v="Senior BI Developer"/>
+    <x v="24"/>
     <d v="1970-04-25T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12765,7 +14459,7 @@
     <n v="10215"/>
     <n v="1"/>
     <n v="50470"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1989-05-02T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12783,7 +14477,7 @@
     <n v="10185"/>
     <n v="1"/>
     <n v="46664"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-03-28T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12801,7 +14495,7 @@
     <n v="10063"/>
     <n v="1"/>
     <n v="48495"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1977-04-08T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12819,7 +14513,7 @@
     <n v="10037"/>
     <n v="0"/>
     <n v="52984"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1967-06-03T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12837,7 +14531,7 @@
     <n v="10042"/>
     <n v="0"/>
     <n v="63695"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1989-03-31T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12855,7 +14549,7 @@
     <n v="10206"/>
     <n v="0"/>
     <n v="62061"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1984-07-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12873,7 +14567,7 @@
     <n v="10104"/>
     <n v="0"/>
     <n v="66738"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1985-11-23T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12891,7 +14585,7 @@
     <n v="10303"/>
     <n v="0"/>
     <n v="52674"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1980-09-30T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12909,7 +14603,7 @@
     <n v="10078"/>
     <n v="0"/>
     <n v="71966"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1952-02-11T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12927,7 +14621,7 @@
     <n v="10121"/>
     <n v="0"/>
     <n v="63051"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1990-05-11T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -12945,7 +14639,7 @@
     <n v="10021"/>
     <n v="1"/>
     <n v="47414"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1976-12-11T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12963,7 +14657,7 @@
     <n v="10281"/>
     <n v="1"/>
     <n v="53060"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1979-11-24T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12981,7 +14675,7 @@
     <n v="10041"/>
     <n v="1"/>
     <n v="68829"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1982-05-19T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -12999,7 +14693,7 @@
     <n v="10148"/>
     <n v="0"/>
     <n v="63515"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1979-05-01T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13017,7 +14711,7 @@
     <n v="10005"/>
     <n v="1"/>
     <n v="108987"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1979-02-20T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13035,7 +14729,7 @@
     <n v="10259"/>
     <n v="1"/>
     <n v="93093"/>
-    <s v="Data Analyst"/>
+    <x v="5"/>
     <d v="1984-09-05T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13053,7 +14747,7 @@
     <n v="10286"/>
     <n v="1"/>
     <n v="53564"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1988-03-17T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13071,7 +14765,7 @@
     <n v="10297"/>
     <n v="0"/>
     <n v="60270"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1989-07-18T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13089,7 +14783,7 @@
     <n v="10171"/>
     <n v="0"/>
     <n v="45998"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1986-07-20T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13107,7 +14801,7 @@
     <n v="10032"/>
     <n v="0"/>
     <n v="57954"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1986-08-17T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13125,7 +14819,7 @@
     <n v="10130"/>
     <n v="0"/>
     <n v="74669"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1977-05-09T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13143,7 +14837,7 @@
     <n v="10217"/>
     <n v="0"/>
     <n v="74226"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1979-03-10T00:00:00"/>
     <x v="1"/>
     <s v="Eligible NonCitizen"/>
@@ -13161,7 +14855,7 @@
     <n v="10016"/>
     <n v="0"/>
     <n v="93554"/>
-    <s v="Data Analyst"/>
+    <x v="5"/>
     <d v="1984-09-16T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13179,7 +14873,7 @@
     <n v="10050"/>
     <n v="1"/>
     <n v="64724"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1988-03-06T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13197,7 +14891,7 @@
     <n v="10164"/>
     <n v="1"/>
     <n v="47001"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1981-11-23T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13215,7 +14909,7 @@
     <n v="10124"/>
     <n v="0"/>
     <n v="61844"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1988-08-29T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13233,7 +14927,7 @@
     <n v="10187"/>
     <n v="0"/>
     <n v="46799"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1984-10-15T00:00:00"/>
     <x v="1"/>
     <s v="Eligible NonCitizen"/>
@@ -13251,7 +14945,7 @@
     <n v="10225"/>
     <n v="1"/>
     <n v="59472"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1961-06-19T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13269,7 +14963,7 @@
     <n v="10262"/>
     <n v="0"/>
     <n v="46430"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1970-09-22T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13287,7 +14981,7 @@
     <n v="10131"/>
     <n v="1"/>
     <n v="83363"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1984-11-06T00:00:00"/>
     <x v="0"/>
     <s v="Eligible NonCitizen"/>
@@ -13305,7 +14999,7 @@
     <n v="10239"/>
     <n v="0"/>
     <n v="95920"/>
-    <s v="BI Developer"/>
+    <x v="17"/>
     <d v="1980-05-12T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13323,7 +15017,7 @@
     <n v="10152"/>
     <n v="1"/>
     <n v="61729"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1984-12-31T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13341,7 +15035,7 @@
     <n v="10140"/>
     <n v="1"/>
     <n v="61809"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1954-10-12T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13359,7 +15053,7 @@
     <n v="10058"/>
     <n v="1"/>
     <n v="45115"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1982-07-22T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13377,7 +15071,7 @@
     <n v="10011"/>
     <n v="0"/>
     <n v="46738"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1973-01-12T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13395,7 +15089,7 @@
     <n v="10230"/>
     <n v="0"/>
     <n v="64971"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1981-09-05T00:00:00"/>
     <x v="1"/>
     <s v="Eligible NonCitizen"/>
@@ -13413,7 +15107,7 @@
     <n v="10224"/>
     <n v="1"/>
     <n v="55578"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1972-07-03T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13431,7 +15125,7 @@
     <n v="10047"/>
     <n v="1"/>
     <n v="50428"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-01-07T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13449,7 +15143,7 @@
     <n v="10285"/>
     <n v="0"/>
     <n v="61422"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1985-01-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13467,7 +15161,7 @@
     <n v="10020"/>
     <n v="1"/>
     <n v="63353"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1985-01-28T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13485,7 +15179,7 @@
     <n v="10162"/>
     <n v="0"/>
     <n v="89883"/>
-    <s v="Data Analyst"/>
+    <x v="5"/>
     <d v="1981-10-11T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13503,7 +15197,7 @@
     <n v="10149"/>
     <n v="0"/>
     <n v="120000"/>
-    <s v="Principal Data Architect"/>
+    <x v="27"/>
     <d v="1973-05-27T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13521,7 +15215,7 @@
     <n v="10086"/>
     <n v="0"/>
     <n v="150290"/>
-    <s v="Data Architect"/>
+    <x v="28"/>
     <d v="1972-11-21T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13539,7 +15233,7 @@
     <n v="10054"/>
     <n v="0"/>
     <n v="60627"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-12-05T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13557,7 +15251,7 @@
     <n v="10065"/>
     <n v="1"/>
     <n v="53180"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1987-03-18T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13575,7 +15269,7 @@
     <n v="10198"/>
     <n v="1"/>
     <n v="140920"/>
-    <s v="IT Manager - DB"/>
+    <x v="29"/>
     <d v="1973-04-05T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13593,7 +15287,7 @@
     <n v="10222"/>
     <n v="1"/>
     <n v="148999"/>
-    <s v="IT Manager - DB"/>
+    <x v="29"/>
     <d v="1964-01-04T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13611,7 +15305,7 @@
     <n v="10126"/>
     <n v="0"/>
     <n v="86214"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1986-07-24T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13629,7 +15323,7 @@
     <n v="10295"/>
     <n v="0"/>
     <n v="47750"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1968-06-06T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13647,7 +15341,7 @@
     <n v="10260"/>
     <n v="1"/>
     <n v="46428"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1974-12-21T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13665,7 +15359,7 @@
     <n v="10233"/>
     <n v="1"/>
     <n v="57975"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1986-04-26T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13683,7 +15377,7 @@
     <n v="10229"/>
     <n v="1"/>
     <n v="88527"/>
-    <s v="Data Analyst"/>
+    <x v="5"/>
     <d v="1987-12-17T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13701,7 +15395,7 @@
     <n v="10169"/>
     <n v="0"/>
     <n v="56147"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1988-07-10T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13719,7 +15413,7 @@
     <n v="10071"/>
     <n v="0"/>
     <n v="50923"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1975-03-10T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13737,7 +15431,7 @@
     <n v="10179"/>
     <n v="0"/>
     <n v="50750"/>
-    <s v="Network Engineer"/>
+    <x v="19"/>
     <d v="1981-04-14T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13755,7 +15449,7 @@
     <n v="10091"/>
     <n v="0"/>
     <n v="52087"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1985-08-24T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13773,7 +15467,7 @@
     <n v="10178"/>
     <n v="1"/>
     <n v="87826"/>
-    <s v="Data Analyst"/>
+    <x v="5"/>
     <d v="1970-02-08T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13791,7 +15485,7 @@
     <n v="10039"/>
     <n v="0"/>
     <n v="51920"/>
-    <s v="Administrative Assistant"/>
+    <x v="22"/>
     <d v="1988-05-19T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13809,7 +15503,7 @@
     <n v="10095"/>
     <n v="0"/>
     <n v="63878"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1987-11-25T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13827,7 +15521,7 @@
     <n v="10027"/>
     <n v="1"/>
     <n v="60656"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1963-10-30T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13845,7 +15539,7 @@
     <n v="10291"/>
     <n v="1"/>
     <n v="72992"/>
-    <s v="Sales Manager"/>
+    <x v="16"/>
     <d v="1984-08-16T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13863,7 +15557,7 @@
     <n v="10153"/>
     <n v="0"/>
     <n v="55000"/>
-    <s v="Administrative Assistant"/>
+    <x v="22"/>
     <d v="1987-06-14T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13881,7 +15575,7 @@
     <n v="10157"/>
     <n v="0"/>
     <n v="58939"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1965-02-02T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13899,7 +15593,7 @@
     <n v="10119"/>
     <n v="0"/>
     <n v="66593"/>
-    <s v="IT Support"/>
+    <x v="4"/>
     <d v="1973-03-12T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13917,7 +15611,7 @@
     <n v="10180"/>
     <n v="1"/>
     <n v="87565"/>
-    <s v="Sr. Network Engineer"/>
+    <x v="15"/>
     <d v="1983-02-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -13935,7 +15629,7 @@
     <n v="10302"/>
     <n v="0"/>
     <n v="64021"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1968-07-20T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13953,7 +15647,7 @@
     <n v="10090"/>
     <n v="0"/>
     <n v="65714"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1975-09-30T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13971,7 +15665,7 @@
     <n v="10030"/>
     <n v="0"/>
     <n v="62425"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1973-03-26T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -13989,7 +15683,7 @@
     <n v="10278"/>
     <n v="0"/>
     <n v="47961"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1982-08-25T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14007,7 +15701,7 @@
     <n v="10307"/>
     <n v="1"/>
     <n v="58273"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1974-05-09T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14025,7 +15719,7 @@
     <n v="10147"/>
     <n v="1"/>
     <n v="63003"/>
-    <s v="Accountant I"/>
+    <x v="10"/>
     <d v="1986-09-01T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14043,7 +15737,7 @@
     <n v="10266"/>
     <n v="1"/>
     <n v="61355"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1985-03-14T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14061,7 +15755,7 @@
     <n v="10241"/>
     <n v="0"/>
     <n v="60120"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1989-05-12T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14079,7 +15773,7 @@
     <n v="10158"/>
     <n v="0"/>
     <n v="63682"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1978-03-28T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14097,7 +15791,7 @@
     <n v="10117"/>
     <n v="1"/>
     <n v="63025"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1982-10-07T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14115,7 +15809,7 @@
     <n v="10209"/>
     <n v="0"/>
     <n v="59238"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1968-08-15T00:00:00"/>
     <x v="1"/>
     <s v="Eligible NonCitizen"/>
@@ -14133,7 +15827,7 @@
     <n v="10024"/>
     <n v="1"/>
     <n v="92989"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1983-05-06T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14151,7 +15845,7 @@
     <n v="10173"/>
     <n v="1"/>
     <n v="90100"/>
-    <s v="BI Developer"/>
+    <x v="17"/>
     <d v="1987-10-24T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14169,7 +15863,7 @@
     <n v="10221"/>
     <n v="0"/>
     <n v="60754"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1975-04-03T00:00:00"/>
     <x v="1"/>
     <s v="Non-Citizen"/>
@@ -14187,7 +15881,7 @@
     <n v="10146"/>
     <n v="0"/>
     <n v="72202"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1953-05-24T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14205,7 +15899,7 @@
     <n v="10161"/>
     <n v="0"/>
     <n v="58370"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1965-05-07T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14223,7 +15917,7 @@
     <n v="10141"/>
     <n v="0"/>
     <n v="48413"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1965-05-09T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14241,7 +15935,7 @@
     <n v="10268"/>
     <n v="1"/>
     <n v="67176"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1975-09-16T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14259,7 +15953,7 @@
     <n v="10123"/>
     <n v="0"/>
     <n v="56339"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1967-06-05T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14277,7 +15971,7 @@
     <n v="10013"/>
     <n v="1"/>
     <n v="64397"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1968-01-15T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14295,7 +15989,7 @@
     <n v="10287"/>
     <n v="0"/>
     <n v="63025"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-05-16T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14313,7 +16007,7 @@
     <n v="10044"/>
     <n v="1"/>
     <n v="75281"/>
-    <s v="Network Engineer"/>
+    <x v="19"/>
     <d v="1988-05-05T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14331,7 +16025,7 @@
     <n v="10102"/>
     <n v="1"/>
     <n v="100416"/>
-    <s v="Software Engineer"/>
+    <x v="3"/>
     <d v="1983-06-14T00:00:00"/>
     <x v="0"/>
     <s v="Non-Citizen"/>
@@ -14349,7 +16043,7 @@
     <n v="10270"/>
     <n v="0"/>
     <n v="74813"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1985-03-15T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14367,7 +16061,7 @@
     <n v="10045"/>
     <n v="1"/>
     <n v="76029"/>
-    <s v="Network Engineer"/>
+    <x v="19"/>
     <d v="1969-03-31T00:00:00"/>
     <x v="0"/>
     <s v="Eligible NonCitizen"/>
@@ -14385,7 +16079,7 @@
     <n v="10205"/>
     <n v="0"/>
     <n v="57859"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1991-05-23T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14403,7 +16097,7 @@
     <n v="10014"/>
     <n v="1"/>
     <n v="58523"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1987-01-31T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14421,7 +16115,7 @@
     <n v="10144"/>
     <n v="1"/>
     <n v="88976"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1968-10-10T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14439,7 +16133,7 @@
     <n v="10253"/>
     <n v="1"/>
     <n v="55875"/>
-    <s v="Area Sales Manager"/>
+    <x v="11"/>
     <d v="1989-07-11T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14457,7 +16151,7 @@
     <n v="10118"/>
     <n v="1"/>
     <n v="113999"/>
-    <s v="Database Administrator"/>
+    <x v="6"/>
     <d v="1986-08-07T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14475,7 +16169,7 @@
     <n v="10022"/>
     <n v="0"/>
     <n v="49773"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1986-06-03T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14493,7 +16187,7 @@
     <n v="10183"/>
     <n v="0"/>
     <n v="62068"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1985-04-06T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14511,7 +16205,7 @@
     <n v="10190"/>
     <n v="1"/>
     <n v="66541"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1976-02-10T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14529,7 +16223,7 @@
     <n v="10274"/>
     <n v="0"/>
     <n v="80512"/>
-    <s v="Production Manager"/>
+    <x v="9"/>
     <d v="1955-11-14T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14547,7 +16241,7 @@
     <n v="10293"/>
     <n v="0"/>
     <n v="50274"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1980-08-02T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14565,7 +16259,7 @@
     <n v="10172"/>
     <n v="1"/>
     <n v="84903"/>
-    <s v="Senior BI Developer"/>
+    <x v="24"/>
     <d v="1981-07-08T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14583,7 +16277,7 @@
     <n v="10127"/>
     <n v="0"/>
     <n v="107226"/>
-    <s v="Sr. Network Engineer"/>
+    <x v="15"/>
     <d v="1978-05-02T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14601,7 +16295,7 @@
     <n v="10072"/>
     <n v="1"/>
     <n v="58371"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1987-05-24T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14619,7 +16313,7 @@
     <n v="10048"/>
     <n v="1"/>
     <n v="55140"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1965-09-09T00:00:00"/>
     <x v="0"/>
     <s v="Eligible NonCitizen"/>
@@ -14637,7 +16331,7 @@
     <n v="10204"/>
     <n v="0"/>
     <n v="58062"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1983-07-30T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14655,7 +16349,7 @@
     <n v="10264"/>
     <n v="0"/>
     <n v="59728"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1969-10-02T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14673,7 +16367,7 @@
     <n v="10033"/>
     <n v="1"/>
     <n v="70507"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1958-11-07T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14691,7 +16385,7 @@
     <n v="10174"/>
     <n v="0"/>
     <n v="60446"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1985-04-20T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14709,7 +16403,7 @@
     <n v="10135"/>
     <n v="1"/>
     <n v="65893"/>
-    <s v="Production Technician II"/>
+    <x v="2"/>
     <d v="1985-05-11T00:00:00"/>
     <x v="0"/>
     <s v="US Citizen"/>
@@ -14727,7 +16421,7 @@
     <n v="10301"/>
     <n v="0"/>
     <n v="48513"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1982-05-04T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14745,7 +16439,7 @@
     <n v="10010"/>
     <n v="0"/>
     <n v="220450"/>
-    <s v="CIO"/>
+    <x v="30"/>
     <d v="1979-08-30T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14763,7 +16457,7 @@
     <n v="10043"/>
     <n v="0"/>
     <n v="89292"/>
-    <s v="Data Analyst"/>
+    <x v="5"/>
     <d v="1979-02-24T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -14781,7 +16475,7 @@
     <n v="10271"/>
     <n v="0"/>
     <n v="45046"/>
-    <s v="Production Technician I"/>
+    <x v="0"/>
     <d v="1978-08-17T00:00:00"/>
     <x v="1"/>
     <s v="US Citizen"/>
@@ -15542,6 +17236,154 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A51850A3-F1B9-473B-B145-9F934099C91C}" name="Зведена таблиця1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Department">
+  <location ref="A3:C10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="32">
+        <item x="10"/>
+        <item x="22"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="13"/>
+        <item x="30"/>
+        <item x="5"/>
+        <item x="28"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item x="7"/>
+        <item x="20"/>
+        <item x="29"/>
+        <item x="26"/>
+        <item x="18"/>
+        <item x="4"/>
+        <item x="19"/>
+        <item x="23"/>
+        <item x="27"/>
+        <item x="9"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="16"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="7">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="12"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Середнє з Salary" fld="3" subtotal="average" baseField="12" baseItem="0" numFmtId="1"/>
+    <dataField name="Кількість з Position" fld="4" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="3" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{388B7420-0CF7-4AE2-B5C1-F9E5B62D966B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="18" unboundColumnsRight="3">
@@ -17492,8 +19334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC33A37C-F375-4CF6-8684-0AFF9BDC5A1D}">
   <dimension ref="A1:Q313"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q3" sqref="A2:Q312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26178,7 +28020,7 @@
       </c>
       <c r="O161">
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DOB]], TODAY(), "Y")</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P161">
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
@@ -27206,7 +29048,7 @@
       </c>
       <c r="O180">
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DOB]], TODAY(), "Y")</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P180">
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
@@ -34382,7 +36224,7 @@
       </c>
       <c r="O313" s="7">
         <f ca="1">SUBTOTAL(101,HRDataset_clean[Age])</f>
-        <v>46.372990353697752</v>
+        <v>46.379421221864952</v>
       </c>
       <c r="P313" s="7">
         <f ca="1">SUBTOTAL(101,HRDataset_clean[Experience])</f>
@@ -34798,9 +36640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E1B752-E64F-4D4F-A5F6-F83CF7389B11}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -34862,6 +36702,124 @@
       <c r="C6" s="16">
         <f>MEDIAN(HRDataset_clean[Salary])</f>
         <v>62810</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96C3E72-ECDE-4205-8485-68AFDC3AF2A3}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>738</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" t="s">
+        <v>732</v>
+      </c>
+      <c r="C3" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="B4" s="15">
+        <v>250000</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B5" s="15">
+        <v>97064.639999999999</v>
+      </c>
+      <c r="C5" s="17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6" s="15">
+        <v>94989.454545454544</v>
+      </c>
+      <c r="C6" s="17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B7" s="15">
+        <v>71791.888888888891</v>
+      </c>
+      <c r="C7" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B8" s="15">
+        <v>69061.258064516136</v>
+      </c>
+      <c r="C8" s="17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B9" s="15">
+        <v>59953.545454545456</v>
+      </c>
+      <c r="C9" s="17">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="B10" s="15">
+        <v>69020.684887459807</v>
+      </c>
+      <c r="C10" s="17">
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add salary analysis by experience
1. Created a new sheet for salary analysis by experience.
2. Built a PivotTable comparing the average salaries of employees across different levels of experience.
3. Added a line chart to visualize the relationship between years of experience and salary.
4. Wrote insights summarizing key findings:
- In this company, salary levels are relatively standardized, and additional experience does not guarantee higher income.
- Salaries depend primarily on the department rather than on gender, age, or experience.
</commit_message>
<xml_diff>
--- a/HRDataset_analysis.xlsx
+++ b/HRDataset_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8beb163ab15076dd/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1092" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA49DE3F-E878-406D-854F-E0BFE422954B}"/>
+  <xr:revisionPtr revIDLastSave="1167" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4470506D-335D-4D2A-9C6D-4A5A4EB814B8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="7" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
   </bookViews>
   <sheets>
     <sheet name="HRDataset_raw" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,15 @@
     <sheet name="Salary_by_gender" sheetId="8" r:id="rId6"/>
     <sheet name="Salary_by_department" sheetId="9" r:id="rId7"/>
     <sheet name="Salary_by_age" sheetId="10" r:id="rId8"/>
+    <sheet name="Salary_by_experience" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">HRDataset_clean!$A$1:$N$312</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId9"/>
-    <pivotCache cacheId="5" r:id="rId10"/>
+    <pivotCache cacheId="6" r:id="rId10"/>
+    <pivotCache cacheId="9" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2884" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2888" uniqueCount="740">
   <si>
     <t>Employee_Name,EmpID,MarriedID,MaritalStatusID,GenderID,EmpStatusID,DeptID,PerfScoreID,FromDiversityJobFairID,Salary,Termd,PositionID,Position,State,Zip,DOB,Sex,MaritalDesc,CitizenDesc,HispanicLatino,RaceDesc,DateofHire,DateofTermination,TermReason,EmploymentStatus,Department,ManagerName,ManagerID,RecruitmentSource,PerformanceScore,EngagementSurvey,EmpSatisfaction,SpecialProjectsCount,LastPerformanceReview_Date,DaysLateLast30,Absences</t>
   </si>
@@ -2294,6 +2295,9 @@
   </si>
   <si>
     <t>Does salary depend on age?</t>
+  </si>
+  <si>
+    <t>Does total experience affect salary?</t>
   </si>
 </sst>
 </file>
@@ -2939,6 +2943,9 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
@@ -2946,6 +2953,133 @@
           <bgColor theme="9"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <fill>
@@ -2970,136 +3104,6 @@
           <bgColor theme="9"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -7526,6 +7530,498 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="uk-UA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[HRDataset_analysis.xlsx]Salary_by_experience!Зведена таблиця2</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Average salary by experience</a:t>
+            </a:r>
+            <a:endParaRPr lang="uk-UA" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="uk-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="uk-UA"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Salary_by_experience!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Підсумок</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Salary_by_experience!$A$4:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Salary_by_experience!$B$4:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>70947.555555555562</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69807.850000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73319.28571428571</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70365.789473684214</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57802.0625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60863.666666666664</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58991.333333333336</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51621.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>101509</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>73837.46666666666</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70206.620689655174</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>68069.528301886792</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64594.729729729726</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72849.275862068971</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66858.291666666672</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>89136.166666666672</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95342.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>63995.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>47001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>64397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E9D1-4BF3-92DC-2DB91CD373A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2053142096"/>
+        <c:axId val="2053139216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2053142096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2053139216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2053139216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2053142096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="uk-UA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7727,6 +8223,46 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10761,6 +11297,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -11989,6 +13041,164 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Діаграма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{218404C7-283F-9C6F-52A9-96ED686592CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBC87E7E-255F-EBD3-2F15-FC6BB596BB1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7994650" y="495300"/>
+          <a:ext cx="3035300" cy="2717800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>►</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Conclusions</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none"/>
+            <a:t>Salaries do not increase gradually with additional years</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t> of experience</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none"/>
+            <a:t>. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Regardless of experience, the average salary for most employees fluctuates within 60-80 K. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>This indicates that in this company, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1" u="sng"/>
+            <a:t>salary levels are relatively standardized, and additional experience does not guarantee higher income. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Moreover, based on insights from previous pivot tables, we can conclude that </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1" u="sng"/>
+            <a:t>salaries depend primarily on the department rather than on gender, age, or experience.</a:t>
+          </a:r>
+          <a:endParaRPr lang="uk-UA" sz="1100" b="1" u="sng"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -12195,7 +13405,30 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Experience" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="19"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="19" count="22">
+        <n v="14"/>
+        <n v="1"/>
+        <n v="17"/>
+        <n v="5"/>
+        <n v="13"/>
+        <n v="11"/>
+        <n v="12"/>
+        <n v="16"/>
+        <n v="10"/>
+        <n v="6"/>
+        <n v="4"/>
+        <n v="9"/>
+        <n v="3"/>
+        <n v="2"/>
+        <n v="0"/>
+        <n v="15"/>
+        <n v="7"/>
+        <n v="8"/>
+        <n v="18"/>
+        <n v="19"/>
+        <n v="8.8617363344051441"/>
+        <m/>
+      </sharedItems>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -17827,7 +19060,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="0"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Ait Sidi, Karthikeyan"/>
@@ -17845,7 +19078,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="1"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Akinkuolie, Sarah"/>
@@ -17863,7 +19096,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="2"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Alagbe,Trina"/>
@@ -17881,7 +19114,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="2"/>
-    <n v="17"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="Anderson, Carol"/>
@@ -17899,7 +19132,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="3"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Anderson, Linda"/>
@@ -17917,7 +19150,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="4"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Andreola, Colby"/>
@@ -17935,7 +19168,7 @@
     <s v="Software Engineering"/>
     <s v="Alex Sweetwater"/>
     <x v="5"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Athwal, Sam"/>
@@ -17953,7 +19186,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="0"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Bachiochi, Linda"/>
@@ -17971,7 +19204,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="6"/>
-    <n v="16"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="Bacong, Alejandro"/>
@@ -17989,7 +19222,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="2"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Baczenski, Rachael"/>
@@ -18007,7 +19240,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="7"/>
-    <n v="6"/>
+    <x v="9"/>
   </r>
   <r>
     <s v="Barbara, Thomas"/>
@@ -18025,7 +19258,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="7"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Barbossa, Hector"/>
@@ -18043,7 +19276,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="2"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Barone, Francesco  A"/>
@@ -18061,7 +19294,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="0"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Barton, Nader"/>
@@ -18079,7 +19312,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="4"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Bates, Norman"/>
@@ -18097,7 +19330,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="8"/>
-    <n v="6"/>
+    <x v="9"/>
   </r>
   <r>
     <s v="Beak, Kimberly"/>
@@ -18115,7 +19348,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="9"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Beatrice, Courtney"/>
@@ -18133,7 +19366,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="6"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Becker, Renee"/>
@@ -18151,7 +19384,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="10"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Becker, Scott"/>
@@ -18169,7 +19402,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="5"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Bernstein, Sean"/>
@@ -18187,7 +19420,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="11"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Biden, Lowan  M"/>
@@ -18205,7 +19438,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="12"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Billis, Helen"/>
@@ -18223,7 +19456,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="3"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Blount, Dianna"/>
@@ -18241,7 +19474,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="13"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Bondwell, Betsy"/>
@@ -18259,7 +19492,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="14"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Booth, Frank"/>
@@ -18277,7 +19510,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="15"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Boutwell, Bonalyn"/>
@@ -18295,7 +19528,7 @@
     <s v="Admin Offices"/>
     <s v="Brandon R. LeBlanc"/>
     <x v="16"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Bozzi, Charles"/>
@@ -18313,7 +19546,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="6"/>
-    <n v="0"/>
+    <x v="14"/>
   </r>
   <r>
     <s v="Brill, Donna"/>
@@ -18331,7 +19564,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="13"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Brown, Mia"/>
@@ -18349,7 +19582,7 @@
     <s v="Admin Offices"/>
     <s v="Brandon R. LeBlanc"/>
     <x v="16"/>
-    <n v="17"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="Buccheri, Joseph"/>
@@ -18367,7 +19600,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="0"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Bugali, Josephine"/>
@@ -18385,7 +19618,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="17"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Bunbury, Jessica"/>
@@ -18403,7 +19636,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="15"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Burke, Joelle"/>
@@ -18421,7 +19654,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="18"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Burkett, Benjamin"/>
@@ -18439,7 +19672,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="4"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Cady, Max"/>
@@ -18457,7 +19690,7 @@
     <s v="Software Engineering"/>
     <s v="Jennifer Zamora"/>
     <x v="9"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Candie, Calvin"/>
@@ -18475,7 +19708,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="0"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Carabbio, Judith"/>
@@ -18493,7 +19726,7 @@
     <s v="Software Engineering"/>
     <s v="Alex Sweetwater"/>
     <x v="16"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Carey, Michael"/>
@@ -18511,7 +19744,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="0"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Carr, Claudia  N"/>
@@ -18529,7 +19762,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="10"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Carter, Michelle"/>
@@ -18547,7 +19780,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="19"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Chace, Beatrice"/>
@@ -18565,7 +19798,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="20"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Champaigne, Brian"/>
@@ -18583,7 +19816,7 @@
     <s v="IT/IS"/>
     <s v="Jennifer Zamora"/>
     <x v="21"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Chan, Lin"/>
@@ -18601,7 +19834,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="5"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Chang, Donovan  E"/>
@@ -18619,7 +19852,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="0"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Chigurh, Anton"/>
@@ -18637,7 +19870,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="6"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Chivukula, Enola"/>
@@ -18655,7 +19888,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="0"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Cierpiszewski, Caroline"/>
@@ -18673,7 +19906,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="2"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Clayton, Rick"/>
@@ -18691,7 +19924,7 @@
     <s v="IT/IS"/>
     <s v="Eric Dougall"/>
     <x v="22"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Cloninger, Jennifer"/>
@@ -18709,7 +19942,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="8"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Close, Phil"/>
@@ -18727,7 +19960,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="23"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Clukey, Elijian"/>
@@ -18745,7 +19978,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="18"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Cockel, James"/>
@@ -18763,7 +19996,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="4"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Cole, Spencer"/>
@@ -18781,7 +20014,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="5"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Corleone, Michael"/>
@@ -18799,7 +20032,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="24"/>
-    <n v="15"/>
+    <x v="15"/>
   </r>
   <r>
     <s v="Corleone, Vito"/>
@@ -18817,7 +20050,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="0"/>
-    <n v="16"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="Cornett, Lisa"/>
@@ -18835,7 +20068,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="4"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Costello, Frank"/>
@@ -18853,7 +20086,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="10"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Crimmings,   Jean"/>
@@ -18871,7 +20104,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="16"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Cross, Noah"/>
@@ -18889,7 +20122,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="25"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Daneault, Lynn"/>
@@ -18907,7 +20140,7 @@
     <s v="Sales"/>
     <s v="Debra Houlihan"/>
     <x v="13"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Daniele, Ann"/>
@@ -18925,7 +20158,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="26"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Darson, Jene'ya"/>
@@ -18943,7 +20176,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="23"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Davis, Daniel"/>
@@ -18961,7 +20194,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="5"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Dee, Randy"/>
@@ -18979,7 +20212,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="2"/>
-    <n v="7"/>
+    <x v="16"/>
   </r>
   <r>
     <s v="DeGweck,  James"/>
@@ -18997,7 +20230,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="4"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Del Bosque, Keyla"/>
@@ -19015,7 +20248,7 @@
     <s v="Software Engineering"/>
     <s v="Alex Sweetwater"/>
     <x v="5"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Delarge, Alex"/>
@@ -19033,7 +20266,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="1"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Demita, Carla"/>
@@ -19051,7 +20284,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="20"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Desimone, Carl"/>
@@ -19069,7 +20302,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="14"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="DeVito, Tommy"/>
@@ -19087,7 +20320,7 @@
     <s v="IT/IS"/>
     <s v="Brian Champaigne"/>
     <x v="0"/>
-    <n v="8"/>
+    <x v="17"/>
   </r>
   <r>
     <s v="Dickinson, Geoff"/>
@@ -19105,7 +20338,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="27"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Dietrich, Jenna"/>
@@ -19123,7 +20356,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="16"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="DiNocco, Lily"/>
@@ -19141,7 +20374,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="23"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Dobrin, Denisa  S"/>
@@ -19159,7 +20392,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="10"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Dolan, Linda"/>
@@ -19177,7 +20410,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="2"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Dougall, Eric"/>
@@ -19195,7 +20428,7 @@
     <s v="IT/IS"/>
     <s v="Jennifer Zamora"/>
     <x v="6"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Driver, Elle"/>
@@ -19213,7 +20446,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="2"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Dunn, Amy"/>
@@ -19231,7 +20464,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="28"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Dunne, Amy"/>
@@ -19249,7 +20482,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="28"/>
-    <n v="15"/>
+    <x v="15"/>
   </r>
   <r>
     <s v="Eaton, Marianne"/>
@@ -19267,7 +20500,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="29"/>
-    <n v="6"/>
+    <x v="9"/>
   </r>
   <r>
     <s v="Engdahl, Jean"/>
@@ -19285,7 +20518,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="7"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="England, Rex"/>
@@ -19303,7 +20536,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="23"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Erilus, Angela"/>
@@ -19321,7 +20554,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="3"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Estremera, Miguel"/>
@@ -19339,7 +20572,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="0"/>
-    <n v="6"/>
+    <x v="9"/>
   </r>
   <r>
     <s v="Evensen, April"/>
@@ -19357,7 +20590,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="3"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Exantus, Susan"/>
@@ -19375,7 +20608,7 @@
     <s v="Software Engineering"/>
     <s v="Alex Sweetwater"/>
     <x v="16"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Faller, Megan"/>
@@ -19393,7 +20626,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="23"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Fancett, Nicole"/>
@@ -19411,7 +20644,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="16"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Ferguson, Susan"/>
@@ -19429,7 +20662,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="30"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Fernandes, Nilson"/>
@@ -19447,7 +20680,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="3"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Fett, Boba"/>
@@ -19465,7 +20698,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="16"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Fidelia,  Libby"/>
@@ -19483,7 +20716,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="8"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Fitzpatrick, Michael  J"/>
@@ -19501,7 +20734,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="8"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Foreman, Tanya"/>
@@ -19519,7 +20752,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="0"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Forrest, Alex"/>
@@ -19537,7 +20770,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="1"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Foss, Jason"/>
@@ -19555,7 +20788,7 @@
     <s v="IT/IS"/>
     <s v="Jennifer Zamora"/>
     <x v="18"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Foster-Baker, Amy"/>
@@ -19573,7 +20806,7 @@
     <s v="Admin Offices"/>
     <s v="Board of Directors"/>
     <x v="5"/>
-    <n v="16"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="Fraval, Maruk"/>
@@ -19591,7 +20824,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="19"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Galia, Lisa"/>
@@ -19609,7 +20842,7 @@
     <s v="IT/IS"/>
     <s v="Eric Dougall"/>
     <x v="31"/>
-    <n v="15"/>
+    <x v="15"/>
   </r>
   <r>
     <s v="Garcia, Raul"/>
@@ -19627,7 +20860,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="22"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Gaul, Barbara"/>
@@ -19645,7 +20878,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="0"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Gentry, Mildred"/>
@@ -19663,7 +20896,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="13"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Gerke, Melisa"/>
@@ -19681,7 +20914,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="6"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Gill, Whitney"/>
@@ -19699,7 +20932,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="11"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Gilles, Alex"/>
@@ -19717,7 +20950,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="7"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Girifalco, Evelyn"/>
@@ -19735,7 +20968,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="18"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Givens, Myriam"/>
@@ -19753,7 +20986,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="3"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Goble, Taisha"/>
@@ -19771,7 +21004,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="11"/>
-    <n v="0"/>
+    <x v="14"/>
   </r>
   <r>
     <s v="Goeth, Amon"/>
@@ -19789,7 +21022,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="3"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Gold, Shenice"/>
@@ -19807,7 +21040,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="32"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Gonzalez, Cayo"/>
@@ -19825,7 +21058,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="17"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Gonzalez, Juan"/>
@@ -19843,7 +21076,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="15"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Gonzalez, Maria"/>
@@ -19861,7 +21094,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="8"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Good, Susan"/>
@@ -19879,7 +21112,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="10"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Gordon, David"/>
@@ -19897,7 +21130,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="5"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Gosciminski, Phylicia"/>
@@ -19915,7 +21148,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="0"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Goyal, Roxana"/>
@@ -19933,7 +21166,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="7"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Gray, Elijiah"/>
@@ -19951,7 +21184,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="8"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Gross, Paula"/>
@@ -19969,7 +21202,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="0"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Gruber, Hans"/>
@@ -19987,7 +21220,7 @@
     <s v="IT/IS"/>
     <s v="Brian Champaigne"/>
     <x v="3"/>
-    <n v="8"/>
+    <x v="17"/>
   </r>
   <r>
     <s v="Guilianno, Mike"/>
@@ -20005,7 +21238,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="17"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Handschiegl, Joanne"/>
@@ -20023,7 +21256,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="4"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Hankard, Earnest"/>
@@ -20041,7 +21274,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="2"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Harrington, Christie"/>
@@ -20059,7 +21292,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="26"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Harrison, Kara"/>
@@ -20077,7 +21310,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="7"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Heitzman, Anthony"/>
@@ -20095,7 +21328,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="33"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Hendrickson, Trina"/>
@@ -20113,7 +21346,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="21"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Hitchcock, Alfred"/>
@@ -20131,7 +21364,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="2"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Homberger, Adrienne  J"/>
@@ -20149,7 +21382,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="33"/>
-    <n v="0"/>
+    <x v="14"/>
   </r>
   <r>
     <s v="Horton, Jayne"/>
@@ -20167,7 +21400,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="33"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Houlihan, Debra"/>
@@ -20185,7 +21418,7 @@
     <s v="Sales"/>
     <s v="Janet King"/>
     <x v="9"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Howard, Estelle"/>
@@ -20203,7 +21436,7 @@
     <s v="Admin Offices"/>
     <s v="Brandon R. LeBlanc"/>
     <x v="22"/>
-    <n v="0"/>
+    <x v="14"/>
   </r>
   <r>
     <s v="Hudson, Jane"/>
@@ -20221,7 +21454,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="10"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Hunts, Julissa"/>
@@ -20239,7 +21472,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="33"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Hutter, Rosalie"/>
@@ -20257,7 +21490,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="32"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Huynh, Ming"/>
@@ -20275,7 +21508,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="24"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Immediato, Walter"/>
@@ -20293,7 +21526,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="24"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Ivey, Rose"/>
@@ -20311,7 +21544,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="29"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Jackson, Maryellen"/>
@@ -20329,7 +21562,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="21"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Jacobi, Hannah"/>
@@ -20347,7 +21580,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="9"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Jeannite, Tayana"/>
@@ -20365,7 +21598,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="10"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Jhaveri, Sneha"/>
@@ -20383,7 +21616,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="15"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Johnson, George"/>
@@ -20401,7 +21634,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="12"/>
-    <n v="6"/>
+    <x v="9"/>
   </r>
   <r>
     <s v="Johnson, Noelle"/>
@@ -20419,7 +21652,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="10"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Johnston, Yen"/>
@@ -20437,7 +21670,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="17"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Jung, Judy"/>
@@ -20455,7 +21688,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="10"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Kampew, Donysha"/>
@@ -20473,7 +21706,7 @@
     <s v="Sales"/>
     <s v="Debra Houlihan"/>
     <x v="3"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Keatts, Kramer"/>
@@ -20491,7 +21724,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="24"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Khemmich, Bartholemew"/>
@@ -20509,7 +21742,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="5"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="King, Janet"/>
@@ -20527,7 +21760,7 @@
     <s v="Executive Office"/>
     <s v="Board of Directors"/>
     <x v="34"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Kinsella, Kathleen"/>
@@ -20545,7 +21778,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="28"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Kirill, Alexandra"/>
@@ -20563,7 +21796,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="6"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Knapp, Bradley  J"/>
@@ -20581,7 +21814,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="4"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Kretschmer, John"/>
@@ -20599,7 +21832,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="18"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Kreuger, Freddy"/>
@@ -20617,7 +21850,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="17"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Lajiri,  Jyoti"/>
@@ -20635,7 +21868,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="10"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Landa, Hans"/>
@@ -20653,7 +21886,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="21"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Langford, Lindsey"/>
@@ -20671,7 +21904,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="5"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Langton, Enrico"/>
@@ -20689,7 +21922,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="10"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="LaRotonda, William"/>
@@ -20707,7 +21940,7 @@
     <s v="Admin Offices"/>
     <s v="Brandon R. LeBlanc"/>
     <x v="33"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Latif, Mohammed"/>
@@ -20725,7 +21958,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="33"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Le, Binh"/>
@@ -20743,7 +21976,7 @@
     <s v="IT/IS"/>
     <s v="Brian Champaigne"/>
     <x v="16"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Leach, Dallas"/>
@@ -20761,7 +21994,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="5"/>
-    <n v="6"/>
+    <x v="9"/>
   </r>
   <r>
     <s v="LeBlanc, Brandon  R"/>
@@ -20779,7 +22012,7 @@
     <s v="Admin Offices"/>
     <s v="Janet King"/>
     <x v="33"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Lecter, Hannibal"/>
@@ -20797,7 +22030,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="27"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Leruth, Giovanni"/>
@@ -20815,7 +22048,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="3"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Liebig, Ketsia"/>
@@ -20833,7 +22066,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="8"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Linares, Marilyn"/>
@@ -20851,7 +22084,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="8"/>
-    <n v="7"/>
+    <x v="16"/>
   </r>
   <r>
     <s v="Linden, Mathew"/>
@@ -20869,7 +22102,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="5"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Lindsay, Leonara"/>
@@ -20887,7 +22120,7 @@
     <s v="IT/IS"/>
     <s v="Eric Dougall"/>
     <x v="2"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Lundy, Susan"/>
@@ -20905,7 +22138,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="4"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Lunquist, Lisa"/>
@@ -20923,7 +22156,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="27"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Lydon, Allison"/>
@@ -20941,7 +22174,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="1"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Lynch, Lindsay"/>
@@ -20959,7 +22192,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="28"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="MacLennan, Samuel"/>
@@ -20977,7 +22210,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="21"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Mahoney, Lauren"/>
@@ -20995,7 +22228,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="10"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Manchester, Robyn"/>
@@ -21013,7 +22246,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="24"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Mancuso, Karen"/>
@@ -21031,7 +22264,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="10"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Mangal, Debbie"/>
@@ -21049,7 +22282,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="7"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Martin, Sandra"/>
@@ -21067,7 +22300,7 @@
     <s v="Software Engineering"/>
     <s v="Alex Sweetwater"/>
     <x v="16"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Maurice, Shana"/>
@@ -21085,7 +22318,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="4"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Carthy, B'rigit"/>
@@ -21103,7 +22336,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="16"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Mckenna, Sandy"/>
@@ -21121,7 +22354,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="16"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="McKinzie, Jac"/>
@@ -21139,7 +22372,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="33"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Meads, Elizabeth"/>
@@ -21157,7 +22390,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="31"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Medeiros, Jennifer"/>
@@ -21175,7 +22408,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="24"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Miller, Brannon"/>
@@ -21193,7 +22426,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="8"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Miller, Ned"/>
@@ -21211,7 +22444,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="22"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Monkfish, Erasumus"/>
@@ -21229,7 +22462,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="32"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Monroe, Peter"/>
@@ -21247,7 +22480,7 @@
     <s v="IT/IS"/>
     <s v="Jennifer Zamora"/>
     <x v="10"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Monterro, Luisa"/>
@@ -21265,7 +22498,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="6"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Moran, Patrick"/>
@@ -21283,7 +22516,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="24"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Morway, Tanya"/>
@@ -21301,7 +22534,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="5"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Motlagh,  Dawn"/>
@@ -21319,7 +22552,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="33"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Moumanil, Maliki"/>
@@ -21337,7 +22570,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="7"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Myers, Michael"/>
@@ -21355,7 +22588,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="18"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Navathe, Kurt"/>
@@ -21373,7 +22606,7 @@
     <s v="IT/IS"/>
     <s v="Brian Champaigne"/>
     <x v="6"/>
-    <n v="8"/>
+    <x v="17"/>
   </r>
   <r>
     <s v="Ndzi, Colombui"/>
@@ -21391,7 +22624,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="3"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Ndzi, Horia"/>
@@ -21409,7 +22642,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Newman, Richard"/>
@@ -21427,7 +22660,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="4"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Ngodup, Shari"/>
@@ -21445,7 +22678,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="14"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Nguyen, Dheepa"/>
@@ -21463,7 +22696,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="3"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Nguyen, Lei-Ming"/>
@@ -21481,7 +22714,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="33"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Nowlan, Kristie"/>
@@ -21499,7 +22732,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="22"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="O'hare, Lynn"/>
@@ -21517,7 +22750,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="18"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Oliver, Brooke"/>
@@ -21535,7 +22768,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="26"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Onque, Jasmine"/>
@@ -21553,7 +22786,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="13"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Osturnka, Adeel"/>
@@ -21571,7 +22804,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="24"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Owad, Clinton"/>
@@ -21589,7 +22822,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="5"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Ozark, Travis"/>
@@ -21607,7 +22840,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="27"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Panjwani, Nina"/>
@@ -21625,7 +22858,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="5"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Patronick, Lucas"/>
@@ -21643,7 +22876,7 @@
     <s v="Software Engineering"/>
     <s v="Alex Sweetwater"/>
     <x v="5"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Pearson, Randall"/>
@@ -21661,7 +22894,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="33"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Smith, Martin"/>
@@ -21679,7 +22912,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="2"/>
-    <n v="6"/>
+    <x v="9"/>
   </r>
   <r>
     <s v="Pelletier, Ermine"/>
@@ -21697,7 +22930,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="3"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Perry, Shakira"/>
@@ -21715,7 +22948,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="10"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Peters, Lauren"/>
@@ -21733,7 +22966,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="10"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Peterson, Ebonee"/>
@@ -21751,7 +22984,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="4"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Petingill, Shana"/>
@@ -21769,7 +23002,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="5"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Petrowsky, Thelma"/>
@@ -21787,7 +23020,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="33"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Pham, Hong"/>
@@ -21805,7 +23038,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="2"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Pitt, Brad"/>
@@ -21823,7 +23056,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="8"/>
-    <n v="18"/>
+    <x v="18"/>
   </r>
   <r>
     <s v="Potts, Xana"/>
@@ -21841,7 +23074,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="2"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Power, Morissa"/>
@@ -21859,7 +23092,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="33"/>
-    <n v="7"/>
+    <x v="16"/>
   </r>
   <r>
     <s v="Punjabhi, Louis"/>
@@ -21877,7 +23110,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="35"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Purinton, Janine"/>
@@ -21895,7 +23128,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="6"/>
-    <n v="0"/>
+    <x v="14"/>
   </r>
   <r>
     <s v="Quinn, Sean"/>
@@ -21913,7 +23146,7 @@
     <s v="Software Engineering"/>
     <s v="Janet King"/>
     <x v="33"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Rachael, Maggie"/>
@@ -21931,7 +23164,7 @@
     <s v="IT/IS"/>
     <s v="Brian Champaigne"/>
     <x v="18"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Rarrick, Quinn"/>
@@ -21949,7 +23182,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="22"/>
-    <n v="6"/>
+    <x v="9"/>
   </r>
   <r>
     <s v="Ren, Kylo"/>
@@ -21967,7 +23200,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="34"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Rhoads, Thomas"/>
@@ -21985,7 +23218,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="27"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Rivera, Haley"/>
@@ -22003,7 +23236,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="28"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Roberson, May"/>
@@ -22021,7 +23254,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="8"/>
-    <n v="0"/>
+    <x v="14"/>
   </r>
   <r>
     <s v="Robertson, Peter"/>
@@ -22039,7 +23272,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="21"/>
-    <n v="0"/>
+    <x v="14"/>
   </r>
   <r>
     <s v="Robinson, Alain"/>
@@ -22057,7 +23290,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="7"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Robinson, Cherly"/>
@@ -22075,7 +23308,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="22"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Robinson, Elias"/>
@@ -22093,7 +23326,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="22"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Roby, Lori"/>
@@ -22111,7 +23344,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="8"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Roehrich, Bianca"/>
@@ -22129,7 +23362,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="28"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Roper, Katie"/>
@@ -22147,7 +23380,7 @@
     <s v="IT/IS"/>
     <s v="Brian Champaigne"/>
     <x v="21"/>
-    <n v="8"/>
+    <x v="17"/>
   </r>
   <r>
     <s v="Rose, Ashley"/>
@@ -22165,7 +23398,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="7"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Rossetti, Bruno"/>
@@ -22183,7 +23416,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="16"/>
-    <n v="7"/>
+    <x v="16"/>
   </r>
   <r>
     <s v="Roup,Simon"/>
@@ -22201,7 +23434,7 @@
     <s v="IT/IS"/>
     <s v="Jennifer Zamora"/>
     <x v="28"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Ruiz, Ricardo"/>
@@ -22219,7 +23452,7 @@
     <s v="IT/IS"/>
     <s v="Jennifer Zamora"/>
     <x v="15"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Saada, Adell"/>
@@ -22237,7 +23470,7 @@
     <s v="Software Engineering"/>
     <s v="Alex Sweetwater"/>
     <x v="10"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Saar-Beckles, Melinda"/>
@@ -22255,7 +23488,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="31"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Sadki, Nore"/>
@@ -22273,7 +23506,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="1"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Sahoo, Adil"/>
@@ -22291,7 +23524,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="10"/>
-    <n v="15"/>
+    <x v="15"/>
   </r>
   <r>
     <s v="Salter, Jason"/>
@@ -22309,7 +23542,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="2"/>
-    <n v="0"/>
+    <x v="14"/>
   </r>
   <r>
     <s v="Sander, Kamrin"/>
@@ -22327,7 +23560,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="2"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Sewkumar, Nori"/>
@@ -22345,7 +23578,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="1"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Shepard, Anita"/>
@@ -22363,7 +23596,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="8"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Shields, Seffi"/>
@@ -22381,7 +23614,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="22"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Simard, Kramer"/>
@@ -22399,7 +23632,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="6"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Singh, Nan"/>
@@ -22417,7 +23650,7 @@
     <s v="Admin Offices"/>
     <s v="Brandon R. LeBlanc"/>
     <x v="2"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Sloan, Constance"/>
@@ -22435,7 +23668,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="16"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Smith, Joe"/>
@@ -22453,7 +23686,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="19"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Smith, John"/>
@@ -22471,7 +23704,7 @@
     <s v="Sales"/>
     <s v="Debra Houlihan"/>
     <x v="33"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Smith, Leigh Ann"/>
@@ -22489,7 +23722,7 @@
     <s v="Admin Offices"/>
     <s v="Brandon R. LeBlanc"/>
     <x v="16"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Smith, Sade"/>
@@ -22507,7 +23740,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="25"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Soto, Julia"/>
@@ -22525,7 +23758,7 @@
     <s v="IT/IS"/>
     <s v="Eric Dougall"/>
     <x v="28"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Soze, Keyser"/>
@@ -22543,7 +23776,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="0"/>
-    <n v="9"/>
+    <x v="11"/>
   </r>
   <r>
     <s v="Sparks, Taylor"/>
@@ -22561,7 +23794,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="31"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Spirea, Kelley"/>
@@ -22579,7 +23812,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="1"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Squatrito, Kristen"/>
@@ -22597,7 +23830,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="28"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Stanford,Barbara  M"/>
@@ -22615,7 +23848,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="27"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Stansfield, Norman"/>
@@ -22633,7 +23866,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="7"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Steans, Tyrone"/>
@@ -22651,7 +23884,7 @@
     <s v="Admin Offices"/>
     <s v="Brandon R. LeBlanc"/>
     <x v="10"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Stoica, Rick"/>
@@ -22669,7 +23902,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="22"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Strong, Caitrin"/>
@@ -22687,7 +23920,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="3"/>
-    <n v="15"/>
+    <x v="15"/>
   </r>
   <r>
     <s v="Sullivan, Kissy"/>
@@ -22705,7 +23938,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="23"/>
-    <n v="16"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="Sullivan, Timothy"/>
@@ -22723,7 +23956,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="27"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Sutwell, Barbara"/>
@@ -22741,7 +23974,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="31"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Szabo, Andrew"/>
@@ -22759,7 +23992,7 @@
     <s v="Software Engineering"/>
     <s v="Alex Sweetwater"/>
     <x v="0"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Tannen, Biff"/>
@@ -22777,7 +24010,7 @@
     <s v="IT/IS"/>
     <s v="Brian Champaigne"/>
     <x v="16"/>
-    <n v="8"/>
+    <x v="17"/>
   </r>
   <r>
     <s v="Tavares, Desiree"/>
@@ -22795,7 +24028,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="1"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Tejeda, Lenora"/>
@@ -22813,7 +24046,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="36"/>
-    <n v="6"/>
+    <x v="9"/>
   </r>
   <r>
     <s v="Terry, Sharlene"/>
@@ -22831,7 +24064,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="25"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Theamstern, Sophia"/>
@@ -22849,7 +24082,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="25"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Thibaud, Kenneth"/>
@@ -22867,7 +24100,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="1"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Tippett, Jeanette"/>
@@ -22885,7 +24118,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="14"/>
-    <n v="12"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="Torrence, Jack"/>
@@ -22903,7 +24136,7 @@
     <s v="Sales"/>
     <s v="Lynn Daneault"/>
     <x v="31"/>
-    <n v="19"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="Trang, Mei"/>
@@ -22921,7 +24154,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="0"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Tredinnick, Neville"/>
@@ -22939,7 +24172,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="2"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="True, Edward"/>
@@ -22957,7 +24190,7 @@
     <s v="Software Engineering"/>
     <s v="Alex Sweetwater"/>
     <x v="0"/>
-    <n v="5"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Trzeciak, Cybil"/>
@@ -22975,7 +24208,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="22"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Turpin, Jumil"/>
@@ -22993,7 +24226,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="17"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Valentin,Jackie"/>
@@ -23011,7 +24244,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="29"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Veera, Abdellah"/>
@@ -23029,7 +24262,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="16"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Vega, Vincent"/>
@@ -23047,7 +24280,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="31"/>
-    <n v="14"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Villanueva, Noah"/>
@@ -23065,7 +24298,7 @@
     <s v="Sales"/>
     <s v="John Smith"/>
     <x v="3"/>
-    <n v="13"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Voldemort, Lord"/>
@@ -23083,7 +24316,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="10"/>
-    <n v="2"/>
+    <x v="13"/>
   </r>
   <r>
     <s v="Volk, Colleen"/>
@@ -23101,7 +24334,7 @@
     <s v="Production"/>
     <s v="Kelley Spirea"/>
     <x v="10"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Von Massenbach, Anna"/>
@@ -23119,7 +24352,7 @@
     <s v="Production"/>
     <s v="Michael Albert"/>
     <x v="22"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Walker, Roger"/>
@@ -23137,7 +24370,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="24"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Wallace, Courtney  E"/>
@@ -23155,7 +24388,7 @@
     <s v="Production"/>
     <s v="Janet King"/>
     <x v="30"/>
-    <n v="0"/>
+    <x v="14"/>
   </r>
   <r>
     <s v="Wallace, Theresa"/>
@@ -23173,7 +24406,7 @@
     <s v="Production"/>
     <s v="Elijiah Gray"/>
     <x v="18"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Wang, Charlie"/>
@@ -23191,7 +24424,7 @@
     <s v="IT/IS"/>
     <s v="Brian Champaigne"/>
     <x v="8"/>
-    <n v="8"/>
+    <x v="17"/>
   </r>
   <r>
     <s v="Warfield, Sarah"/>
@@ -23209,7 +24442,7 @@
     <s v="IT/IS"/>
     <s v="Peter Monroe"/>
     <x v="23"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Whittier, Scott"/>
@@ -23227,7 +24460,7 @@
     <s v="Production"/>
     <s v="Webster Butler"/>
     <x v="16"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Wilber, Barry"/>
@@ -23245,7 +24478,7 @@
     <s v="Production"/>
     <s v="Amy Dunn"/>
     <x v="25"/>
-    <n v="4"/>
+    <x v="10"/>
   </r>
   <r>
     <s v="Wilkes, Annie"/>
@@ -23263,7 +24496,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="0"/>
-    <n v="1"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Williams, Jacquelyn"/>
@@ -23281,7 +24514,7 @@
     <s v="Production"/>
     <s v="Ketsia Liebig"/>
     <x v="17"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Winthrop, Jordan"/>
@@ -23299,7 +24532,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="37"/>
-    <n v="3"/>
+    <x v="12"/>
   </r>
   <r>
     <s v="Wolk, Hang  T"/>
@@ -23317,7 +24550,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="22"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Woodson, Jason"/>
@@ -23335,7 +24568,7 @@
     <s v="Production"/>
     <s v="Kissy Sullivan"/>
     <x v="22"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Ybarra, Catherine"/>
@@ -23353,7 +24586,7 @@
     <s v="Production"/>
     <s v="Brannon Miller"/>
     <x v="27"/>
-    <n v="7"/>
+    <x v="16"/>
   </r>
   <r>
     <s v="Zamora, Jennifer"/>
@@ -23371,7 +24604,7 @@
     <s v="IT/IS"/>
     <s v="Janet King"/>
     <x v="5"/>
-    <n v="15"/>
+    <x v="15"/>
   </r>
   <r>
     <s v="Zhou, Julia"/>
@@ -23389,7 +24622,7 @@
     <s v="IT/IS"/>
     <s v="Simon Roup"/>
     <x v="5"/>
-    <n v="10"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="Zima, Colleen"/>
@@ -23407,7 +24640,7 @@
     <s v="Production"/>
     <s v="David Stanley"/>
     <x v="23"/>
-    <n v="11"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="Підсумок"/>
@@ -23425,7 +24658,7 @@
     <m/>
     <n v="311"/>
     <x v="38"/>
-    <n v="8.8617363344051441"/>
+    <x v="20"/>
   </r>
   <r>
     <m/>
@@ -23443,13 +24676,13 @@
     <m/>
     <m/>
     <x v="39"/>
-    <m/>
+    <x v="21"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{522A496A-A047-4258-90E9-EEA28A2DD2FD}" name="Зведена таблиця1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Department">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{522A496A-A047-4258-90E9-EEA28A2DD2FD}" name="Зведена таблиця1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Department">
   <location ref="A3:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -23840,7 +25073,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{99C9EE08-55A3-4A4F-80AE-C08BB2D6FC1E}" name="Зведена таблиця1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Gender/ Employment status">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{99C9EE08-55A3-4A4F-80AE-C08BB2D6FC1E}" name="Зведена таблиця1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Gender/ Employment status">
   <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -24026,7 +25259,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CD0F9E0-F6E8-4E42-A55B-30816338B9A3}" name="Зведена таблиця1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Employment Status">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CD0F9E0-F6E8-4E42-A55B-30816338B9A3}" name="Зведена таблиця1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Employment Status">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -24100,7 +25333,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B618E153-E906-4623-A1B0-AE62734F806F}" name="Зведена таблиця1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Gender">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B618E153-E906-4623-A1B0-AE62734F806F}" name="Зведена таблиця1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Gender">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -24194,7 +25427,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A51850A3-F1B9-473B-B145-9F934099C91C}" name="Зведена таблиця1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Department">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A51850A3-F1B9-473B-B145-9F934099C91C}" name="Зведена таблиця1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Department">
   <location ref="A3:C10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -24342,7 +25575,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{90482986-69AC-4AC3-8402-8DB7E8972187}" name="Зведена таблиця1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Age">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{90482986-69AC-4AC3-8402-8DB7E8972187}" name="Зведена таблиця1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Age">
   <location ref="A3:B42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -24557,6 +25790,150 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10D7127C-9B11-40DA-81BF-712D6B284100}" name="Зведена таблиця2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Experience">
+  <location ref="A3:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="23">
+        <item x="14"/>
+        <item x="1"/>
+        <item x="13"/>
+        <item x="12"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item h="1" x="20"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="15"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item h="1" x="21"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="15"/>
+  </rowFields>
+  <rowItems count="21">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Середнє з Salary" fld="3" subtotal="average" baseField="15" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{388B7420-0CF7-4AE2-B5C1-F9E5B62D966B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="18" unboundColumnsRight="2">
@@ -24586,24 +25963,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DCCABDF-7E51-42A4-BAF7-A2DF0D4A54BF}" name="HRDataset_clean" displayName="HRDataset_clean" ref="A1:P313" tableType="queryTable" totalsRowCount="1" totalsRowDxfId="31">
   <autoFilter ref="A1:P312" xr:uid="{6DCCABDF-7E51-42A4-BAF7-A2DF0D4A54BF}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{462F1512-129C-4F18-8C84-CD8C5BB364A2}" uniqueName="1" name="Employee_Name" totalsRowLabel="Підсумок" queryTableFieldId="1" dataDxfId="30" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{BEAB6FB1-D5C7-42F5-9F26-A9B447C44D34}" uniqueName="2" name="EmpID" queryTableFieldId="2" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{397CF102-4293-4481-BFAE-0B3D2B348160}" uniqueName="3" name="GenderID" queryTableFieldId="3" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{38A122EA-0347-4570-BF5B-4FA57F6BA9C5}" uniqueName="4" name="Salary" totalsRowFunction="average" queryTableFieldId="4" dataDxfId="29" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{92A7FDDB-7044-4095-B7E6-661E59EB5D74}" uniqueName="5" name="Position" queryTableFieldId="5" dataDxfId="28" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{C60E0FEE-1DFA-45E8-800A-2CC6600AF4F2}" uniqueName="6" name="DOB" queryTableFieldId="6" dataDxfId="27" totalsRowDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{CD8449F9-309B-45A3-A14A-C2429E7EA4C7}" uniqueName="7" name="Sex" queryTableFieldId="7" dataDxfId="26" totalsRowDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{1B446900-7DD4-4FC8-8495-8B92E69A854B}" uniqueName="8" name="CitizenDesc" queryTableFieldId="8" dataDxfId="25" totalsRowDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{294582B3-6CE5-4308-9124-823642574DEE}" uniqueName="9" name="DateofHire" queryTableFieldId="9" dataDxfId="24" totalsRowDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{9AD61435-7995-48F1-98A2-AE58EDB1CEEC}" uniqueName="10" name="DateofTermination" queryTableFieldId="10" dataDxfId="23" totalsRowDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{79D2E0D1-8707-4E8D-828D-34F246FEBE73}" uniqueName="11" name="TermReason" queryTableFieldId="11" dataDxfId="22" totalsRowDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{8E5FE07E-3A76-423C-9ED8-5EF75465016F}" uniqueName="12" name="EmploymentStatus" totalsRowFunction="count" queryTableFieldId="12" dataDxfId="21" totalsRowDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{14F95057-44E0-4669-9378-93872DCEB711}" uniqueName="13" name="Department" queryTableFieldId="13" dataDxfId="20" totalsRowDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{2D3C1819-424E-4E1C-BA32-2F3FEC5CE7D7}" uniqueName="14" name="ManagerName" totalsRowFunction="count" queryTableFieldId="14" dataDxfId="19" totalsRowDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{41A5A662-2EBA-4F0B-A187-319218E766C8}" uniqueName="15" name="Age" totalsRowFunction="average" queryTableFieldId="15" dataDxfId="18" totalsRowDxfId="2">
+    <tableColumn id="1" xr3:uid="{462F1512-129C-4F18-8C84-CD8C5BB364A2}" uniqueName="1" name="Employee_Name" totalsRowLabel="Підсумок" queryTableFieldId="1" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{BEAB6FB1-D5C7-42F5-9F26-A9B447C44D34}" uniqueName="2" name="EmpID" queryTableFieldId="2" totalsRowDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{397CF102-4293-4481-BFAE-0B3D2B348160}" uniqueName="3" name="GenderID" queryTableFieldId="3" totalsRowDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{38A122EA-0347-4570-BF5B-4FA57F6BA9C5}" uniqueName="4" name="Salary" totalsRowFunction="average" queryTableFieldId="4" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{92A7FDDB-7044-4095-B7E6-661E59EB5D74}" uniqueName="5" name="Position" queryTableFieldId="5" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{C60E0FEE-1DFA-45E8-800A-2CC6600AF4F2}" uniqueName="6" name="DOB" queryTableFieldId="6" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{CD8449F9-309B-45A3-A14A-C2429E7EA4C7}" uniqueName="7" name="Sex" queryTableFieldId="7" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{1B446900-7DD4-4FC8-8495-8B92E69A854B}" uniqueName="8" name="CitizenDesc" queryTableFieldId="8" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{294582B3-6CE5-4308-9124-823642574DEE}" uniqueName="9" name="DateofHire" queryTableFieldId="9" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{9AD61435-7995-48F1-98A2-AE58EDB1CEEC}" uniqueName="10" name="DateofTermination" queryTableFieldId="10" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{79D2E0D1-8707-4E8D-828D-34F246FEBE73}" uniqueName="11" name="TermReason" queryTableFieldId="11" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{8E5FE07E-3A76-423C-9ED8-5EF75465016F}" uniqueName="12" name="EmploymentStatus" totalsRowFunction="count" queryTableFieldId="12" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{14F95057-44E0-4669-9378-93872DCEB711}" uniqueName="13" name="Department" queryTableFieldId="13" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{2D3C1819-424E-4E1C-BA32-2F3FEC5CE7D7}" uniqueName="14" name="ManagerName" totalsRowFunction="count" queryTableFieldId="14" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{41A5A662-2EBA-4F0B-A187-319218E766C8}" uniqueName="15" name="Age" totalsRowFunction="average" queryTableFieldId="15" dataDxfId="4" totalsRowDxfId="3">
       <calculatedColumnFormula>DATEDIF(HRDataset_clean[[#This Row],[DOB]], TODAY(), "Y")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{4DB63E1C-C3BC-4899-8FC0-92DDE29B5436}" uniqueName="16" name="Experience" totalsRowFunction="average" queryTableFieldId="16" dataDxfId="17" totalsRowDxfId="1">
+    <tableColumn id="16" xr3:uid="{4DB63E1C-C3BC-4899-8FC0-92DDE29B5436}" uniqueName="16" name="Experience" totalsRowFunction="average" queryTableFieldId="16" dataDxfId="2" totalsRowDxfId="1">
       <calculatedColumnFormula>DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -42754,7 +44131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D9E133-0E77-4FD6-9DF4-4B3BC0531991}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -43088,6 +44465,211 @@
         <v>724</v>
       </c>
       <c r="B42" s="15">
+        <v>69020.684887459807</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA7DB75-23F8-40FF-AD11-2C111567608B}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>739</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="B3" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>0</v>
+      </c>
+      <c r="B4" s="15">
+        <v>70947.555555555562</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15">
+        <v>69807.850000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15">
+        <v>73319.28571428571</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="15">
+        <v>70365.789473684214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>4</v>
+      </c>
+      <c r="B8" s="15">
+        <v>57802.0625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>5</v>
+      </c>
+      <c r="B9" s="15">
+        <v>60863.666666666664</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>6</v>
+      </c>
+      <c r="B10" s="15">
+        <v>58991.333333333336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>7</v>
+      </c>
+      <c r="B11" s="15">
+        <v>51621.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>8</v>
+      </c>
+      <c r="B12" s="15">
+        <v>101509</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>9</v>
+      </c>
+      <c r="B13" s="15">
+        <v>73837.46666666666</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>10</v>
+      </c>
+      <c r="B14" s="15">
+        <v>70206.620689655174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
+        <v>11</v>
+      </c>
+      <c r="B15" s="15">
+        <v>68069.528301886792</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>12</v>
+      </c>
+      <c r="B16" s="15">
+        <v>64594.729729729726</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>13</v>
+      </c>
+      <c r="B17" s="15">
+        <v>72849.275862068971</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>14</v>
+      </c>
+      <c r="B18" s="15">
+        <v>66858.291666666672</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>15</v>
+      </c>
+      <c r="B19" s="15">
+        <v>89136.166666666672</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>16</v>
+      </c>
+      <c r="B20" s="15">
+        <v>95342.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>17</v>
+      </c>
+      <c r="B21" s="15">
+        <v>63995.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>18</v>
+      </c>
+      <c r="B22" s="15">
+        <v>47001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>19</v>
+      </c>
+      <c r="B23" s="15">
+        <v>64397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="B24" s="15">
         <v>69020.684887459807</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add project insights and recommendations
1. Created a summary sheet consolidating key insights from all analytical sections.
2. Formulated findings across turnover and salary analyses by department, gender, age, and experience.
3. Added practical, data-driven recommendations based on observed patterns.
4. Framed conclusions to support HR and management decision-making.
</commit_message>
<xml_diff>
--- a/HRDataset_analysis.xlsx
+++ b/HRDataset_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8beb163ab15076dd/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1466" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9760910D-55D2-4F03-BF8C-0100132CE359}"/>
+  <xr:revisionPtr revIDLastSave="1518" documentId="8_{1E6F348B-99C9-4E4D-B190-90CFADF3FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13796FF1-1DC4-4145-891D-1ADB75FF0C3C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="9" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="10" xr2:uid="{5D044F8E-927F-447A-A22D-B78F8FF00805}"/>
   </bookViews>
   <sheets>
     <sheet name="HRDataset_raw" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Salary_by_age" sheetId="10" r:id="rId8"/>
     <sheet name="Salary_by_experience" sheetId="11" r:id="rId9"/>
     <sheet name="Dashboard" sheetId="12" r:id="rId10"/>
+    <sheet name="Conclusions" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">HRDataset_clean!$A$1:$N$312</definedName>
@@ -31,14 +32,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId11"/>
-    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId13"/>
         <x14:slicerCache r:id="rId14"/>
+        <x14:slicerCache r:id="rId15"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2895" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2899" uniqueCount="751">
   <si>
     <t>Employee_Name,EmpID,MarriedID,MaritalStatusID,GenderID,EmpStatusID,DeptID,PerfScoreID,FromDiversityJobFairID,Salary,Termd,PositionID,Position,State,Zip,DOB,Sex,MaritalDesc,CitizenDesc,HispanicLatino,RaceDesc,DateofHire,DateofTermination,TermReason,EmploymentStatus,Department,ManagerName,ManagerID,RecruitmentSource,PerformanceScore,EngagementSurvey,EmpSatisfaction,SpecialProjectsCount,LastPerformanceReview_Date,DaysLateLast30,Absences</t>
   </si>
@@ -2331,6 +2332,18 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                                          Data Analysis for HR Department</t>
+  </si>
+  <si>
+    <t>Project Insights</t>
+  </si>
+  <si>
+    <t>Key Findings</t>
+  </si>
+  <si>
+    <t>Business Interpretation</t>
+  </si>
+  <si>
+    <t>Recommendations</t>
   </si>
 </sst>
 </file>
@@ -2341,7 +2354,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2536,6 +2549,22 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Display"/>
       <family val="2"/>
@@ -2938,7 +2967,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3008,7 +3037,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% – колірна тема 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -24484,8 +24515,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1041400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="10" name="Department">
@@ -24508,7 +24539,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -24562,8 +24593,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1047750</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="11" name="Sex">
@@ -24586,7 +24617,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -24625,6 +24656,511 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6164D815-7F3F-6355-6EAB-3A4A6F089CDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="692150"/>
+          <a:ext cx="7327900" cy="1682750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Employee turnover is concentrated primarily among newcomers with low experience, while experienced employees form a stable core of the company.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Salary levels do not significantly depend on gender, age, or years of experience.</a:t>
+          </a:r>
+          <a:endParaRPr lang="uk-UA">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0" rtl="0"/>
+          <a:r>
+            <a:rPr lang="uk-UA">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Average salaries remain within a relatively narrow range.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Department plays a much stronger role in salary differentiation than individual demographic factors.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Production and Sales departments show the highest levels of employee turnover.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Both men and women have a small number of high earners, which impacts average salary more than median salary.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Salary levels do not increase proportionally with experience, indicating flat salary progression across tenure levels.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Voluntary and involuntary terminations among new employees occur at similar experience levels.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="uk-UA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480B91F8-1E49-6162-3855-DB3614720190}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2762250"/>
+          <a:ext cx="7315200" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>The company demonstrates standardized compensation practices, where salary growth is primarily driven by departmental structure rather than personal characteristics or experience. High employee retention among experienced staff suggests effective long-term engagement strategies, while elevated turnover among newcomers may indicate onboarding or expectation alignment issues.</a:t>
+          </a:r>
+          <a:endParaRPr lang="uk-UA" sz="1100">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13CEA03B-D334-6830-A603-B54AB09C74E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4121150"/>
+          <a:ext cx="7315200" cy="1079500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Improve onboarding processes for new employees.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1100" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Focus retention efforts on the first </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>6-24</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> months of employment.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1100" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Analyze turnover drivers at the department level.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1100" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Consider reviewing career development and compensation progression frameworks to improve motivation and retention among early-career employees.</a:t>
+          </a:r>
+          <a:endParaRPr lang="uk-UA" sz="1100">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -39686,7 +40222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EFF950-EE91-4A48-B6DD-A39CACBEC3EE}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
@@ -39737,7 +40273,7 @@
       <c r="G4" s="22"/>
       <c r="J4" s="26">
         <f ca="1">HRDataset_clean[[#Totals],[Age]]</f>
-        <v>46.382636655948552</v>
+        <v>46.389067524115752</v>
       </c>
       <c r="K4" s="27"/>
       <c r="N4" s="26">
@@ -40694,6 +41230,49 @@
       </x14:slicerList>
     </ext>
   </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA4B702-2314-4A9F-9456-A57B310D3EE3}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="36" t="s">
+        <v>748</v>
+      </c>
+      <c r="B3" s="37"/>
+    </row>
+    <row r="14" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="36" t="s">
+        <v>749</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+    </row>
+    <row r="21" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="36" t="s">
+        <v>750</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -43513,7 +44092,7 @@
       </c>
       <c r="O56">
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DOB]], TODAY(), "Y")</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P56">
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
@@ -53266,7 +53845,7 @@
       </c>
       <c r="O251">
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DOB]], TODAY(), "Y")</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P251">
         <f ca="1">DATEDIF(HRDataset_clean[[#This Row],[DateofHire]], IF(HRDataset_clean[[#This Row],[DateofTermination]]="", TODAY(),HRDataset_clean[[#This Row],[DateofTermination]]),"Y")</f>
@@ -56344,7 +56923,7 @@
       </c>
       <c r="O313" s="7">
         <f ca="1">SUBTOTAL(101,HRDataset_clean[Age])</f>
-        <v>46.382636655948552</v>
+        <v>46.389067524115752</v>
       </c>
       <c r="P313" s="7">
         <f ca="1">SUBTOTAL(101,HRDataset_clean[Experience])</f>
@@ -56398,7 +56977,7 @@
       <c r="A4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4">
         <v>209</v>
       </c>
     </row>
@@ -56406,7 +56985,7 @@
       <c r="A5" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5">
         <v>126</v>
       </c>
     </row>
@@ -56414,7 +56993,7 @@
       <c r="A6" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6">
         <v>8</v>
       </c>
     </row>
@@ -56422,7 +57001,7 @@
       <c r="A7" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7">
         <v>75</v>
       </c>
     </row>
@@ -56430,7 +57009,7 @@
       <c r="A8" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8">
         <v>50</v>
       </c>
     </row>
@@ -56438,7 +57017,7 @@
       <c r="A9" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9">
         <v>40</v>
       </c>
     </row>
@@ -56446,7 +57025,7 @@
       <c r="A10" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10">
         <v>4</v>
       </c>
     </row>
@@ -56454,7 +57033,7 @@
       <c r="A11" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11">
         <v>6</v>
       </c>
     </row>
@@ -56462,7 +57041,7 @@
       <c r="A12" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12">
         <v>31</v>
       </c>
     </row>
@@ -56470,7 +57049,7 @@
       <c r="A13" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13">
         <v>26</v>
       </c>
     </row>
@@ -56478,7 +57057,7 @@
       <c r="A14" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14">
         <v>2</v>
       </c>
     </row>
@@ -56486,7 +57065,7 @@
       <c r="A15" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15">
         <v>3</v>
       </c>
     </row>
@@ -56494,7 +57073,7 @@
       <c r="A16" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16">
         <v>11</v>
       </c>
     </row>
@@ -56502,7 +57081,7 @@
       <c r="A17" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B17" s="35">
+      <c r="B17">
         <v>7</v>
       </c>
     </row>
@@ -56510,7 +57089,7 @@
       <c r="A18" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B18" s="35">
+      <c r="B18">
         <v>1</v>
       </c>
     </row>
@@ -56518,7 +57097,7 @@
       <c r="A19" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B19" s="35">
+      <c r="B19">
         <v>3</v>
       </c>
     </row>
@@ -56526,7 +57105,7 @@
       <c r="A20" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="B20" s="35">
+      <c r="B20">
         <v>9</v>
       </c>
     </row>
@@ -56534,7 +57113,7 @@
       <c r="A21" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B21" s="35">
+      <c r="B21">
         <v>7</v>
       </c>
     </row>
@@ -56542,7 +57121,7 @@
       <c r="A22" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B22" s="35">
+      <c r="B22">
         <v>1</v>
       </c>
     </row>
@@ -56550,7 +57129,7 @@
       <c r="A23" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B23" s="35">
+      <c r="B23">
         <v>1</v>
       </c>
     </row>
@@ -56558,7 +57137,7 @@
       <c r="A24" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="B24" s="35">
+      <c r="B24">
         <v>1</v>
       </c>
     </row>
@@ -56566,7 +57145,7 @@
       <c r="A25" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25">
         <v>1</v>
       </c>
     </row>
@@ -56574,7 +57153,7 @@
       <c r="A26" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="B26" s="35">
+      <c r="B26">
         <v>311</v>
       </c>
     </row>
@@ -56635,7 +57214,7 @@
       <c r="A4" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4">
         <v>176</v>
       </c>
     </row>
@@ -56643,7 +57222,7 @@
       <c r="A5" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5">
         <v>116</v>
       </c>
     </row>
@@ -56651,7 +57230,7 @@
       <c r="A6" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6">
         <v>9</v>
       </c>
     </row>
@@ -56659,7 +57238,7 @@
       <c r="A7" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7">
         <v>51</v>
       </c>
     </row>
@@ -56667,7 +57246,7 @@
       <c r="A8" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8">
         <v>135</v>
       </c>
     </row>
@@ -56675,7 +57254,7 @@
       <c r="A9" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9">
         <v>91</v>
       </c>
     </row>
@@ -56683,7 +57262,7 @@
       <c r="A10" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10">
         <v>7</v>
       </c>
     </row>
@@ -56691,7 +57270,7 @@
       <c r="A11" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11">
         <v>37</v>
       </c>
     </row>
@@ -56699,7 +57278,7 @@
       <c r="A12" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12">
         <v>311</v>
       </c>
     </row>
@@ -56895,7 +57474,7 @@
       <c r="B4" s="15">
         <v>250000</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
@@ -56906,7 +57485,7 @@
       <c r="B5" s="15">
         <v>97064.639999999999</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5">
         <v>50</v>
       </c>
     </row>
@@ -56917,7 +57496,7 @@
       <c r="B6" s="15">
         <v>94989.454545454544</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6">
         <v>11</v>
       </c>
     </row>
@@ -56928,7 +57507,7 @@
       <c r="B7" s="15">
         <v>71791.888888888891</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7">
         <v>9</v>
       </c>
     </row>
@@ -56939,7 +57518,7 @@
       <c r="B8" s="15">
         <v>69061.258064516136</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8">
         <v>31</v>
       </c>
     </row>
@@ -56950,7 +57529,7 @@
       <c r="B9" s="15">
         <v>59953.545454545456</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9">
         <v>209</v>
       </c>
     </row>
@@ -56961,7 +57540,7 @@
       <c r="B10" s="15">
         <v>69020.684887459807</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10">
         <v>311</v>
       </c>
     </row>

</xml_diff>